<commit_message>
Added row spacing and tillering data
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="12" windowWidth="12120" windowHeight="6456" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="192" yWindow="12" windowWidth="12120" windowHeight="6456" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="276">
   <si>
     <t>SimulationName</t>
   </si>
@@ -839,7 +839,16 @@
     <t>Wheat.Phenology.Zadok.Stage</t>
   </si>
   <si>
-    <t>Wheat.Structure.MainStemNodeNo</t>
+    <t>GattonRowSpacingRowSpace25cm</t>
+  </si>
+  <si>
+    <t>GattonRowSpacingRowSpace50cm</t>
+  </si>
+  <si>
+    <t>GattonRowSpacingRowSpaceN0</t>
+  </si>
+  <si>
+    <t>Wheat.Leaf.AppearedCohortNo</t>
   </si>
 </sst>
 </file>
@@ -1251,14 +1260,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE228"/>
+  <dimension ref="A1:AE231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="4164" ySplit="588" topLeftCell="AB210" activePane="bottomRight"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A227" sqref="A227"/>
-      <selection pane="bottomRight" activeCell="AB214" sqref="AB214"/>
+      <pane ySplit="864" topLeftCell="A92" activePane="bottomLeft"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -13266,6 +13273,75 @@
         <v>28.747393692751672</v>
       </c>
     </row>
+    <row r="229" spans="1:31">
+      <c r="A229" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="C229" s="1">
+        <v>90</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E229">
+        <v>1675.3</v>
+      </c>
+      <c r="G229">
+        <v>636.29999999999995</v>
+      </c>
+      <c r="AB229">
+        <v>16885</v>
+      </c>
+      <c r="AC229">
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="230" spans="1:31">
+      <c r="A230" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="C230" s="1">
+        <v>90</v>
+      </c>
+      <c r="D230" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E230">
+        <v>1492.5</v>
+      </c>
+      <c r="G230">
+        <v>554.25</v>
+      </c>
+      <c r="AB230">
+        <v>15830</v>
+      </c>
+      <c r="AC230">
+        <v>35.200000000000003</v>
+      </c>
+    </row>
+    <row r="231" spans="1:31">
+      <c r="A231" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C231" s="1">
+        <v>90</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E231">
+        <v>1238.7</v>
+      </c>
+      <c r="G231">
+        <v>380</v>
+      </c>
+      <c r="AB231">
+        <v>10025</v>
+      </c>
+      <c r="AC231">
+        <v>37.9</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A3:AD253">
     <sortCondition ref="A3:A253"/>
@@ -13277,17 +13353,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L114"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="528" topLeftCell="A49" activePane="bottomLeft"/>
-      <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="I50" sqref="I50:I59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4884" ySplit="528" topLeftCell="A60" activePane="bottomRight"/>
+      <selection sqref="A1:A1048576"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <selection pane="bottomRight" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
@@ -15237,6 +15315,725 @@
         <v>0</v>
       </c>
     </row>
+    <row r="60" spans="1:12">
+      <c r="A60" t="s">
+        <v>272</v>
+      </c>
+      <c r="B60" s="12">
+        <v>40745</v>
+      </c>
+      <c r="C60">
+        <v>480</v>
+      </c>
+      <c r="J60">
+        <v>25.9</v>
+      </c>
+      <c r="L60">
+        <v>0.41818507199999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" t="s">
+        <v>272</v>
+      </c>
+      <c r="B61" s="12">
+        <v>40752</v>
+      </c>
+      <c r="C61">
+        <v>880</v>
+      </c>
+      <c r="J61">
+        <v>86</v>
+      </c>
+      <c r="L61">
+        <v>1.45847481</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" t="s">
+        <v>272</v>
+      </c>
+      <c r="B62" s="12">
+        <v>40756</v>
+      </c>
+      <c r="C62">
+        <v>853.33333333333326</v>
+      </c>
+      <c r="E62">
+        <v>92.4</v>
+      </c>
+      <c r="F62">
+        <v>26.5</v>
+      </c>
+      <c r="J62">
+        <v>118.9</v>
+      </c>
+      <c r="L62">
+        <v>2.0131426069999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" t="s">
+        <v>272</v>
+      </c>
+      <c r="B63" s="12">
+        <v>40764</v>
+      </c>
+      <c r="C63">
+        <v>800</v>
+      </c>
+      <c r="E63">
+        <v>126.4</v>
+      </c>
+      <c r="F63">
+        <v>51.8</v>
+      </c>
+      <c r="J63">
+        <v>178.3</v>
+      </c>
+      <c r="L63">
+        <v>2.9735134680000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" t="s">
+        <v>272</v>
+      </c>
+      <c r="B64" s="12">
+        <v>40788</v>
+      </c>
+      <c r="C64">
+        <v>773.33333333333326</v>
+      </c>
+      <c r="E64">
+        <v>276.39999999999998</v>
+      </c>
+      <c r="F64">
+        <v>244.2</v>
+      </c>
+      <c r="J64">
+        <v>520.5</v>
+      </c>
+      <c r="L64">
+        <v>6.1201040439999996</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" t="s">
+        <v>272</v>
+      </c>
+      <c r="B65" s="12">
+        <v>40851</v>
+      </c>
+      <c r="C65">
+        <v>492.24674144728192</v>
+      </c>
+      <c r="I65">
+        <v>636.29999999999995</v>
+      </c>
+      <c r="J65">
+        <v>1675.3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" t="s">
+        <v>273</v>
+      </c>
+      <c r="B66" s="12">
+        <v>40745</v>
+      </c>
+      <c r="C66">
+        <v>240</v>
+      </c>
+      <c r="J66">
+        <v>16.7</v>
+      </c>
+      <c r="L66">
+        <v>0.24753102699999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" t="s">
+        <v>273</v>
+      </c>
+      <c r="B67" s="12">
+        <v>40752</v>
+      </c>
+      <c r="C67">
+        <v>466.66666666666663</v>
+      </c>
+      <c r="J67">
+        <v>50</v>
+      </c>
+      <c r="L67">
+        <v>0.846396072</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" t="s">
+        <v>273</v>
+      </c>
+      <c r="B68" s="12">
+        <v>40756</v>
+      </c>
+      <c r="C68">
+        <v>473.33333333333337</v>
+      </c>
+      <c r="E68">
+        <v>50.1</v>
+      </c>
+      <c r="F68">
+        <v>13.2</v>
+      </c>
+      <c r="J68">
+        <v>63.4</v>
+      </c>
+      <c r="L68">
+        <v>1.0147118559999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" t="s">
+        <v>273</v>
+      </c>
+      <c r="B69" s="12">
+        <v>40764</v>
+      </c>
+      <c r="C69">
+        <v>446.66666666666663</v>
+      </c>
+      <c r="E69">
+        <v>100.2</v>
+      </c>
+      <c r="F69">
+        <v>38.4</v>
+      </c>
+      <c r="J69">
+        <v>138.6</v>
+      </c>
+      <c r="L69">
+        <v>2.2704393980000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" t="s">
+        <v>273</v>
+      </c>
+      <c r="B70" s="12">
+        <v>40788</v>
+      </c>
+      <c r="C70">
+        <v>533.33333333333337</v>
+      </c>
+      <c r="E70">
+        <v>221.8</v>
+      </c>
+      <c r="F70">
+        <v>190.3</v>
+      </c>
+      <c r="J70">
+        <v>412</v>
+      </c>
+      <c r="L70">
+        <v>4.9096734560000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" t="s">
+        <v>273</v>
+      </c>
+      <c r="B71" s="12">
+        <v>40851</v>
+      </c>
+      <c r="C71">
+        <v>400.19794245747079</v>
+      </c>
+      <c r="I71">
+        <v>554.25</v>
+      </c>
+      <c r="J71">
+        <v>1492.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" t="s">
+        <v>274</v>
+      </c>
+      <c r="B72" s="12">
+        <v>40851</v>
+      </c>
+      <c r="C72">
+        <v>389.1151157936099</v>
+      </c>
+      <c r="I72">
+        <v>380</v>
+      </c>
+      <c r="J72">
+        <v>1238.7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B73" s="13">
+        <v>33798</v>
+      </c>
+      <c r="C73">
+        <v>127.49999618530273</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B74" s="14">
+        <v>33813</v>
+      </c>
+      <c r="C74">
+        <v>106.66666793823242</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B75" s="14">
+        <v>33840</v>
+      </c>
+      <c r="C75">
+        <v>243.58333587646484</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B76" s="14">
+        <v>33856</v>
+      </c>
+      <c r="C76">
+        <v>161.875</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B77" s="14">
+        <v>33877</v>
+      </c>
+      <c r="C77">
+        <v>130.90291213989258</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="A78" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B78" s="14">
+        <v>33889</v>
+      </c>
+      <c r="C78">
+        <v>125.54166793823242</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="A79" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B79" s="14">
+        <v>33907</v>
+      </c>
+      <c r="C79">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
+      <c r="A80" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B80" s="13">
+        <v>33798</v>
+      </c>
+      <c r="C80">
+        <v>109.58333206176758</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B81" s="14">
+        <v>33813</v>
+      </c>
+      <c r="C81">
+        <v>100.41666793823242</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B82" s="14">
+        <v>33840</v>
+      </c>
+      <c r="C82">
+        <v>468.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B83" s="14">
+        <v>33856</v>
+      </c>
+      <c r="C83">
+        <v>424.16667175292969</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B84" s="14">
+        <v>33877</v>
+      </c>
+      <c r="C84">
+        <v>167.77791595458984</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B85" s="14">
+        <v>33889</v>
+      </c>
+      <c r="C85">
+        <v>177.08332824707031</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B86" s="14">
+        <v>33907</v>
+      </c>
+      <c r="C86">
+        <v>214.9999974568685</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B87" s="13">
+        <v>33798</v>
+      </c>
+      <c r="C87">
+        <v>117.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B88" s="14">
+        <v>33813</v>
+      </c>
+      <c r="C88">
+        <v>108.33333587646484</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B89" s="14">
+        <v>33840</v>
+      </c>
+      <c r="C89">
+        <v>522.66665649414062</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B90" s="14">
+        <v>33856</v>
+      </c>
+      <c r="C90">
+        <v>344.69166564941406</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B91" s="14">
+        <v>33877</v>
+      </c>
+      <c r="C91">
+        <v>493.055419921875</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B92" s="14">
+        <v>33889</v>
+      </c>
+      <c r="C92">
+        <v>287.569580078125</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B93" s="14">
+        <v>33907</v>
+      </c>
+      <c r="C93">
+        <v>304.72207641601562</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B94" s="13">
+        <v>33798</v>
+      </c>
+      <c r="C94">
+        <v>118.75</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B95" s="14">
+        <v>33813</v>
+      </c>
+      <c r="C95">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B96" s="14">
+        <v>33840</v>
+      </c>
+      <c r="C96">
+        <v>523.5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B97" s="14">
+        <v>33856</v>
+      </c>
+      <c r="C97">
+        <v>501.52915954589844</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B98" s="14">
+        <v>33877</v>
+      </c>
+      <c r="C98">
+        <v>369.16665649414062</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B99" s="14">
+        <v>33889</v>
+      </c>
+      <c r="C99">
+        <v>351.59709167480469</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B100" s="14">
+        <v>33907</v>
+      </c>
+      <c r="C100">
+        <v>297.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101" s="13">
+        <v>33798</v>
+      </c>
+      <c r="C101">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B102" s="14">
+        <v>33813</v>
+      </c>
+      <c r="C102">
+        <v>112.08333206176758</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B103" s="14">
+        <v>33840</v>
+      </c>
+      <c r="C103">
+        <v>518.87501525878906</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B104" s="14">
+        <v>33856</v>
+      </c>
+      <c r="C104">
+        <v>534.09584045410156</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B105" s="14">
+        <v>33877</v>
+      </c>
+      <c r="C105">
+        <v>389.58332824707031</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B106" s="14">
+        <v>33889</v>
+      </c>
+      <c r="C106">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B107" s="14">
+        <v>33907</v>
+      </c>
+      <c r="C107">
+        <v>373.61125183105469</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B108" s="13">
+        <v>33798</v>
+      </c>
+      <c r="C108">
+        <v>121.24999618530273</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B109" s="14">
+        <v>33813</v>
+      </c>
+      <c r="C109">
+        <v>115.83333206176758</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B110" s="14">
+        <v>33840</v>
+      </c>
+      <c r="C110">
+        <v>786.08334350585937</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B111" s="14">
+        <v>33856</v>
+      </c>
+      <c r="C111">
+        <v>836.48747253417969</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B112" s="14">
+        <v>33877</v>
+      </c>
+      <c r="C112">
+        <v>450.20832824707031</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B113" s="14">
+        <v>33889</v>
+      </c>
+      <c r="C113">
+        <v>504.86123657226563</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B114" s="14">
+        <v>33907</v>
+      </c>
+      <c r="C114">
+        <v>422.36125183105469</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15244,12 +16041,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F382"/>
+  <dimension ref="A1:F395"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="576" topLeftCell="A370"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="576" activePane="bottomLeft"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C371" sqref="C371"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -15269,7 +16066,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D1" t="s">
         <v>209</v>
@@ -20073,6 +20870,135 @@
       <c r="F382">
         <v>5.8888888888888893</v>
       </c>
+    </row>
+    <row r="383" spans="1:6">
+      <c r="A383" t="s">
+        <v>272</v>
+      </c>
+      <c r="B383" s="12">
+        <v>40745</v>
+      </c>
+      <c r="C383">
+        <v>4.1666666670000003</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6">
+      <c r="A384" t="s">
+        <v>272</v>
+      </c>
+      <c r="B384" s="12">
+        <v>40752</v>
+      </c>
+      <c r="C384">
+        <v>5.4249999999999998</v>
+      </c>
+    </row>
+    <row r="385" spans="1:3">
+      <c r="A385" t="s">
+        <v>272</v>
+      </c>
+      <c r="B385" s="12">
+        <v>40756</v>
+      </c>
+      <c r="C385">
+        <v>5.9083333329999999</v>
+      </c>
+    </row>
+    <row r="386" spans="1:3">
+      <c r="A386" t="s">
+        <v>272</v>
+      </c>
+      <c r="B386" s="12">
+        <v>40764</v>
+      </c>
+      <c r="C386">
+        <v>6.5416666670000003</v>
+      </c>
+    </row>
+    <row r="387" spans="1:3">
+      <c r="A387" t="s">
+        <v>272</v>
+      </c>
+      <c r="B387" s="12">
+        <v>40788</v>
+      </c>
+      <c r="C387">
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="388" spans="1:3">
+      <c r="A388" t="s">
+        <v>272</v>
+      </c>
+      <c r="B388" s="12">
+        <v>40851</v>
+      </c>
+    </row>
+    <row r="389" spans="1:3">
+      <c r="A389" t="s">
+        <v>273</v>
+      </c>
+      <c r="B389" s="12">
+        <v>40745</v>
+      </c>
+      <c r="C389">
+        <v>4.1666666670000003</v>
+      </c>
+    </row>
+    <row r="390" spans="1:3">
+      <c r="A390" t="s">
+        <v>273</v>
+      </c>
+      <c r="B390" s="12">
+        <v>40752</v>
+      </c>
+      <c r="C390">
+        <v>5.2833333329999999</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3">
+      <c r="A391" t="s">
+        <v>273</v>
+      </c>
+      <c r="B391" s="12">
+        <v>40756</v>
+      </c>
+      <c r="C391">
+        <v>5.8416666670000001</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3">
+      <c r="A392" t="s">
+        <v>273</v>
+      </c>
+      <c r="B392" s="12">
+        <v>40764</v>
+      </c>
+      <c r="C392">
+        <v>6.7916666670000003</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3">
+      <c r="A393" t="s">
+        <v>273</v>
+      </c>
+      <c r="B393" s="12">
+        <v>40788</v>
+      </c>
+      <c r="C393">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3">
+      <c r="A394" t="s">
+        <v>273</v>
+      </c>
+      <c r="B394" s="12">
+        <v>40851</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3">
+      <c r="B395" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
YCreek soil water data
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="12" windowWidth="12120" windowHeight="6456" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="192" yWindow="12" windowWidth="12120" windowHeight="6456" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1738" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="280">
   <si>
     <t>SimulationName</t>
   </si>
@@ -857,13 +857,20 @@
   <si>
     <t>ET</t>
   </si>
+  <si>
+    <t>Soil.SoilWater.SW(9)</t>
+  </si>
+  <si>
+    <t>Soil.SoilWater.SW(10)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -940,7 +947,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -975,6 +982,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -21090,7 +21098,7 @@
   <dimension ref="A1:E419"/>
   <sheetViews>
     <sheetView topLeftCell="A403" workbookViewId="0">
-      <selection activeCell="A416" sqref="A416"/>
+      <selection activeCell="A415" sqref="A415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -25965,21 +25973,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K175"/>
+  <dimension ref="A1:M185"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="864" topLeftCell="A169" activePane="bottomLeft"/>
+      <selection activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -26013,8 +26024,14 @@
       <c r="K1" s="10" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="11" t="s">
         <v>197</v>
       </c>
@@ -26049,7 +26066,7 @@
         <v>0.19625000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="A3" s="11" t="s">
         <v>197</v>
       </c>
@@ -26084,7 +26101,7 @@
         <v>0.19750000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="A4" s="11" t="s">
         <v>197</v>
       </c>
@@ -26119,7 +26136,7 @@
         <v>0.19475000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="A5" s="11" t="s">
         <v>197</v>
       </c>
@@ -26154,7 +26171,7 @@
         <v>0.19350000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:13">
       <c r="A6" s="11" t="s">
         <v>197</v>
       </c>
@@ -26189,7 +26206,7 @@
         <v>0.19375000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:13">
       <c r="A7" s="11" t="s">
         <v>197</v>
       </c>
@@ -26224,7 +26241,7 @@
         <v>0.19500000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:13">
       <c r="A8" s="11" t="s">
         <v>197</v>
       </c>
@@ -26259,7 +26276,7 @@
         <v>0.21325000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:13">
       <c r="A9" s="11" t="s">
         <v>197</v>
       </c>
@@ -26294,7 +26311,7 @@
         <v>0.22274999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:13">
       <c r="A10" s="11" t="s">
         <v>197</v>
       </c>
@@ -26329,7 +26346,7 @@
         <v>0.22950000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:13">
       <c r="A11" s="11" t="s">
         <v>197</v>
       </c>
@@ -26364,7 +26381,7 @@
         <v>0.223</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:13">
       <c r="A12" s="11" t="s">
         <v>197</v>
       </c>
@@ -26399,7 +26416,7 @@
         <v>0.22075</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:13">
       <c r="A13" s="11" t="s">
         <v>197</v>
       </c>
@@ -26434,7 +26451,7 @@
         <v>0.22099999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:13">
       <c r="A14" s="11" t="s">
         <v>197</v>
       </c>
@@ -26469,7 +26486,7 @@
         <v>0.21724999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:13">
       <c r="A15" s="11" t="s">
         <v>197</v>
       </c>
@@ -26504,7 +26521,7 @@
         <v>0.21675</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:13">
       <c r="A16" s="11" t="s">
         <v>197</v>
       </c>
@@ -31579,7 +31596,7 @@
         <v>0.252</v>
       </c>
     </row>
-    <row r="161" spans="1:11">
+    <row r="161" spans="1:13">
       <c r="A161" s="11" t="s">
         <v>202</v>
       </c>
@@ -31614,7 +31631,7 @@
         <v>0.24975000000000003</v>
       </c>
     </row>
-    <row r="162" spans="1:11">
+    <row r="162" spans="1:13">
       <c r="A162" s="11" t="s">
         <v>202</v>
       </c>
@@ -31649,7 +31666,7 @@
         <v>0.24875</v>
       </c>
     </row>
-    <row r="163" spans="1:11">
+    <row r="163" spans="1:13">
       <c r="A163" s="11" t="s">
         <v>202</v>
       </c>
@@ -31684,7 +31701,7 @@
         <v>0.24600000000000002</v>
       </c>
     </row>
-    <row r="164" spans="1:11">
+    <row r="164" spans="1:13">
       <c r="A164" s="11" t="s">
         <v>202</v>
       </c>
@@ -31719,7 +31736,7 @@
         <v>0.24525000000000002</v>
       </c>
     </row>
-    <row r="165" spans="1:11">
+    <row r="165" spans="1:13">
       <c r="A165" s="11" t="s">
         <v>202</v>
       </c>
@@ -31754,7 +31771,7 @@
         <v>0.23925000000000002</v>
       </c>
     </row>
-    <row r="166" spans="1:11">
+    <row r="166" spans="1:13">
       <c r="A166" s="11" t="s">
         <v>202</v>
       </c>
@@ -31789,7 +31806,7 @@
         <v>0.23349999999999999</v>
       </c>
     </row>
-    <row r="167" spans="1:11">
+    <row r="167" spans="1:13">
       <c r="A167" s="11" t="s">
         <v>202</v>
       </c>
@@ -31824,7 +31841,7 @@
         <v>0.23199999999999998</v>
       </c>
     </row>
-    <row r="168" spans="1:11">
+    <row r="168" spans="1:13">
       <c r="A168" s="11" t="s">
         <v>202</v>
       </c>
@@ -31859,7 +31876,7 @@
         <v>0.22549999999999998</v>
       </c>
     </row>
-    <row r="169" spans="1:11">
+    <row r="169" spans="1:13">
       <c r="A169" s="11" t="s">
         <v>202</v>
       </c>
@@ -31894,7 +31911,7 @@
         <v>0.21525</v>
       </c>
     </row>
-    <row r="170" spans="1:11">
+    <row r="170" spans="1:13">
       <c r="A170" s="11" t="s">
         <v>202</v>
       </c>
@@ -31929,7 +31946,7 @@
         <v>0.20699999999999999</v>
       </c>
     </row>
-    <row r="171" spans="1:11">
+    <row r="171" spans="1:13">
       <c r="A171" s="11" t="s">
         <v>202</v>
       </c>
@@ -31964,7 +31981,7 @@
         <v>0.20325000000000004</v>
       </c>
     </row>
-    <row r="172" spans="1:11">
+    <row r="172" spans="1:13">
       <c r="A172" s="11" t="s">
         <v>202</v>
       </c>
@@ -31999,7 +32016,7 @@
         <v>0.19949999999999998</v>
       </c>
     </row>
-    <row r="173" spans="1:11">
+    <row r="173" spans="1:13">
       <c r="A173" s="11" t="s">
         <v>202</v>
       </c>
@@ -32034,7 +32051,7 @@
         <v>0.19949999999999998</v>
       </c>
     </row>
-    <row r="174" spans="1:11">
+    <row r="174" spans="1:13">
       <c r="A174" s="11" t="s">
         <v>202</v>
       </c>
@@ -32069,7 +32086,7 @@
         <v>0.19725000000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:11">
+    <row r="175" spans="1:13">
       <c r="A175" s="11" t="s">
         <v>202</v>
       </c>
@@ -32102,6 +32119,356 @@
       </c>
       <c r="K175">
         <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13">
+      <c r="A176" t="s">
+        <v>276</v>
+      </c>
+      <c r="B176" s="20">
+        <v>37068</v>
+      </c>
+      <c r="C176">
+        <v>904.78270880573837</v>
+      </c>
+      <c r="E176">
+        <v>0.46336650178340993</v>
+      </c>
+      <c r="F176">
+        <v>0.5287117995382894</v>
+      </c>
+      <c r="G176">
+        <v>0.54485817589700725</v>
+      </c>
+      <c r="H176">
+        <v>0.52897094450766613</v>
+      </c>
+      <c r="I176">
+        <v>0.51462622600062757</v>
+      </c>
+      <c r="J176">
+        <v>0.54345742022487398</v>
+      </c>
+      <c r="K176">
+        <v>0.50275464008076465</v>
+      </c>
+      <c r="L176">
+        <v>0.46624444147805399</v>
+      </c>
+      <c r="M176">
+        <v>0.43092339451799921</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13">
+      <c r="A177" t="s">
+        <v>276</v>
+      </c>
+      <c r="B177" s="20">
+        <v>37097</v>
+      </c>
+      <c r="C177">
+        <v>897.75645123572258</v>
+      </c>
+      <c r="E177">
+        <v>0.44612710192039051</v>
+      </c>
+      <c r="F177">
+        <v>0.52952518366686052</v>
+      </c>
+      <c r="G177">
+        <v>0.53790888791554647</v>
+      </c>
+      <c r="H177">
+        <v>0.52759201630554953</v>
+      </c>
+      <c r="I177">
+        <v>0.5065663217920181</v>
+      </c>
+      <c r="J177">
+        <v>0.53834621822054318</v>
+      </c>
+      <c r="K177">
+        <v>0.50228573792617592</v>
+      </c>
+      <c r="L177">
+        <v>0.46664457708616164</v>
+      </c>
+      <c r="M177">
+        <v>0.4337862113453661</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13">
+      <c r="A178" t="s">
+        <v>276</v>
+      </c>
+      <c r="B178" s="20">
+        <v>37103</v>
+      </c>
+      <c r="C178">
+        <v>936.55537238603972</v>
+      </c>
+      <c r="E178">
+        <v>0.5159983176857651</v>
+      </c>
+      <c r="F178">
+        <v>0.54256720218397247</v>
+      </c>
+      <c r="G178">
+        <v>0.55037263864340846</v>
+      </c>
+      <c r="H178">
+        <v>0.53493614691175806</v>
+      </c>
+      <c r="I178">
+        <v>0.52054159650691501</v>
+      </c>
+      <c r="J178">
+        <v>0.55307697682190471</v>
+      </c>
+      <c r="K178">
+        <v>0.5436136274616572</v>
+      </c>
+      <c r="L178">
+        <v>0.48395772090924005</v>
+      </c>
+      <c r="M178">
+        <v>0.43771263480557793</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13">
+      <c r="A179" t="s">
+        <v>276</v>
+      </c>
+      <c r="B179" s="20">
+        <v>37127</v>
+      </c>
+      <c r="C179">
+        <v>917.08209705901197</v>
+      </c>
+      <c r="E179">
+        <v>0.51961580866143964</v>
+      </c>
+      <c r="F179">
+        <v>0.54321630929966003</v>
+      </c>
+      <c r="G179">
+        <v>0.550913907041642</v>
+      </c>
+      <c r="H179">
+        <v>0.53011666279275726</v>
+      </c>
+      <c r="I179">
+        <v>0.52735824922219232</v>
+      </c>
+      <c r="J179">
+        <v>0.54973183641163337</v>
+      </c>
+      <c r="K179">
+        <v>0.48035779706697596</v>
+      </c>
+      <c r="L179">
+        <v>0.45473452662424946</v>
+      </c>
+      <c r="M179">
+        <v>0.42936538817450903</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13">
+      <c r="A180" t="s">
+        <v>276</v>
+      </c>
+      <c r="B180" s="20">
+        <v>37166</v>
+      </c>
+      <c r="C180">
+        <v>781.24223856149877</v>
+      </c>
+      <c r="E180">
+        <v>0.34382444998586331</v>
+      </c>
+      <c r="F180">
+        <v>0.3758451409405123</v>
+      </c>
+      <c r="G180">
+        <v>0.4213465884752241</v>
+      </c>
+      <c r="H180">
+        <v>0.4395812476839871</v>
+      </c>
+      <c r="I180">
+        <v>0.46439152101895348</v>
+      </c>
+      <c r="J180">
+        <v>0.51203355913485626</v>
+      </c>
+      <c r="K180">
+        <v>0.4737617484669765</v>
+      </c>
+      <c r="L180">
+        <v>0.45440500422598168</v>
+      </c>
+      <c r="M180">
+        <v>0.42102193287513956</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13">
+      <c r="A181" t="s">
+        <v>276</v>
+      </c>
+      <c r="B181" s="20">
+        <v>37174</v>
+      </c>
+      <c r="C181">
+        <v>760.95883640208854</v>
+      </c>
+      <c r="E181">
+        <v>0.33764096723288206</v>
+      </c>
+      <c r="F181">
+        <v>0.35624176126266333</v>
+      </c>
+      <c r="G181">
+        <v>0.39474561362548427</v>
+      </c>
+      <c r="H181">
+        <v>0.41791669295525219</v>
+      </c>
+      <c r="I181">
+        <v>0.44869264649829271</v>
+      </c>
+      <c r="J181">
+        <v>0.50706232309325261</v>
+      </c>
+      <c r="K181">
+        <v>0.47096823033137641</v>
+      </c>
+      <c r="L181">
+        <v>0.44990670380170061</v>
+      </c>
+      <c r="M181">
+        <v>0.42161924320953881</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13">
+      <c r="A182" t="s">
+        <v>276</v>
+      </c>
+      <c r="B182" s="20">
+        <v>37197</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13">
+      <c r="A183" t="s">
+        <v>276</v>
+      </c>
+      <c r="B183" s="20">
+        <v>37200</v>
+      </c>
+      <c r="C183">
+        <v>672.26132498316542</v>
+      </c>
+      <c r="E183">
+        <v>0.27391534189002842</v>
+      </c>
+      <c r="F183">
+        <v>0.29179351070458681</v>
+      </c>
+      <c r="G183">
+        <v>0.32172120887333044</v>
+      </c>
+      <c r="H183">
+        <v>0.34464302424277354</v>
+      </c>
+      <c r="I183">
+        <v>0.38121706217723073</v>
+      </c>
+      <c r="J183">
+        <v>0.44286482501949992</v>
+      </c>
+      <c r="K183">
+        <v>0.43931877262460134</v>
+      </c>
+      <c r="L183">
+        <v>0.44232547651572413</v>
+      </c>
+      <c r="M183">
+        <v>0.42350740286805172</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13">
+      <c r="A184" t="s">
+        <v>276</v>
+      </c>
+      <c r="B184" s="20">
+        <v>37216</v>
+      </c>
+      <c r="C184">
+        <v>687.68728594656227</v>
+      </c>
+      <c r="E184">
+        <v>0.34187749898448344</v>
+      </c>
+      <c r="F184">
+        <v>0.30741767271470127</v>
+      </c>
+      <c r="G184">
+        <v>0.32245484202390318</v>
+      </c>
+      <c r="H184">
+        <v>0.34060554711649133</v>
+      </c>
+      <c r="I184">
+        <v>0.37865568982417847</v>
+      </c>
+      <c r="J184">
+        <v>0.43902349445312649</v>
+      </c>
+      <c r="K184">
+        <v>0.43520393076437558</v>
+      </c>
+      <c r="L184">
+        <v>0.44342822444943819</v>
+      </c>
+      <c r="M184">
+        <v>0.42976952940211399</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13">
+      <c r="A185" t="s">
+        <v>276</v>
+      </c>
+      <c r="B185" s="20">
+        <v>37230</v>
+      </c>
+      <c r="C185">
+        <v>724.00029456307641</v>
+      </c>
+      <c r="E185">
+        <v>0.4311657365770607</v>
+      </c>
+      <c r="F185">
+        <v>0.36661783595799613</v>
+      </c>
+      <c r="G185">
+        <v>0.34921838875901734</v>
+      </c>
+      <c r="H185">
+        <v>0.35659408138284937</v>
+      </c>
+      <c r="I185">
+        <v>0.38457441496299843</v>
+      </c>
+      <c r="J185">
+        <v>0.44137710614422587</v>
+      </c>
+      <c r="K185">
+        <v>0.43300305927935284</v>
+      </c>
+      <c r="L185">
+        <v>0.43591572858981648</v>
+      </c>
+      <c r="M185">
+        <v>0.42153512116206493</v>
       </c>
     </row>
   </sheetData>
@@ -32113,7 +32480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added china flux data
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="12" windowWidth="12120" windowHeight="6456" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="192" yWindow="12" windowWidth="12120" windowHeight="6456" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1815" uniqueCount="283">
   <si>
     <t>SimulationName</t>
   </si>
@@ -863,6 +863,15 @@
   <si>
     <t>Wheat.Summariser.AboveGround.N</t>
   </si>
+  <si>
+    <t>Yucheng2002</t>
+  </si>
+  <si>
+    <t>Yucheng2003</t>
+  </si>
+  <si>
+    <t>Yucheng2004</t>
+  </si>
 </sst>
 </file>
 
@@ -1400,23 +1409,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="85630976"/>
-        <c:axId val="85634048"/>
+        <c:axId val="74805632"/>
+        <c:axId val="74807168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85630976"/>
+        <c:axId val="74805632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85634048"/>
+        <c:crossAx val="74807168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85634048"/>
+        <c:axId val="74807168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1424,7 +1433,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85630976"/>
+        <c:crossAx val="74805632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1436,7 +1445,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -13865,14 +13874,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M119"/>
+  <dimension ref="A1:M159"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4884" ySplit="528" topLeftCell="C81" activePane="bottomRight"/>
-      <selection sqref="A1:A1048576"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomRight" activeCell="F99" sqref="F99"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="576" topLeftCell="A142" activePane="bottomLeft"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="I159" sqref="I159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16804,11 +16811,559 @@
       <c r="B119" s="12">
         <v>37229</v>
       </c>
-      <c r="I119">
-        <v>720.8</v>
-      </c>
       <c r="J119">
         <v>1469.5293209876545</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="A120" t="s">
+        <v>280</v>
+      </c>
+      <c r="B120" s="12">
+        <v>37699</v>
+      </c>
+      <c r="J120">
+        <v>57.620000000000005</v>
+      </c>
+      <c r="L120">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="A121" t="s">
+        <v>280</v>
+      </c>
+      <c r="B121" s="12">
+        <v>37707</v>
+      </c>
+      <c r="J121">
+        <v>86.63</v>
+      </c>
+      <c r="L121">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122" t="s">
+        <v>280</v>
+      </c>
+      <c r="B122" s="12">
+        <v>37715</v>
+      </c>
+      <c r="J122">
+        <v>225.99</v>
+      </c>
+      <c r="L122">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
+      <c r="A123" t="s">
+        <v>280</v>
+      </c>
+      <c r="B123" s="12">
+        <v>37721</v>
+      </c>
+      <c r="J123">
+        <v>312.01</v>
+      </c>
+      <c r="L123">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
+      <c r="A124" t="s">
+        <v>280</v>
+      </c>
+      <c r="B124" s="12">
+        <v>37726</v>
+      </c>
+      <c r="J124">
+        <v>416.98</v>
+      </c>
+      <c r="L124">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
+      <c r="A125" t="s">
+        <v>280</v>
+      </c>
+      <c r="B125" s="12">
+        <v>37731</v>
+      </c>
+      <c r="L125">
+        <v>3.89</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
+      <c r="A126" t="s">
+        <v>280</v>
+      </c>
+      <c r="B126" s="12">
+        <v>37736</v>
+      </c>
+      <c r="J126">
+        <v>546.79</v>
+      </c>
+      <c r="L126">
+        <v>5.21</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
+      <c r="A127" t="s">
+        <v>280</v>
+      </c>
+      <c r="B127" s="12">
+        <v>37741</v>
+      </c>
+      <c r="L127">
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
+      <c r="A128" t="s">
+        <v>280</v>
+      </c>
+      <c r="B128" s="12">
+        <v>37746</v>
+      </c>
+      <c r="J128">
+        <v>797.05</v>
+      </c>
+      <c r="L128">
+        <v>4.8899999999999997</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
+      <c r="A129" t="s">
+        <v>280</v>
+      </c>
+      <c r="B129" s="12">
+        <v>37751</v>
+      </c>
+      <c r="L129">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
+      <c r="A130" t="s">
+        <v>280</v>
+      </c>
+      <c r="B130" s="12">
+        <v>37756</v>
+      </c>
+      <c r="J130">
+        <v>1128.73</v>
+      </c>
+      <c r="L130">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
+      <c r="A131" t="s">
+        <v>280</v>
+      </c>
+      <c r="B131" s="12">
+        <v>37766</v>
+      </c>
+      <c r="J131">
+        <v>1279.8</v>
+      </c>
+      <c r="L131">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
+      <c r="A132" t="s">
+        <v>280</v>
+      </c>
+      <c r="B132" s="12">
+        <v>37776</v>
+      </c>
+      <c r="I132">
+        <v>526</v>
+      </c>
+      <c r="J132">
+        <v>922.8</v>
+      </c>
+      <c r="L132">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
+      <c r="A133" t="s">
+        <v>281</v>
+      </c>
+      <c r="B133" s="12">
+        <v>38050</v>
+      </c>
+      <c r="J133">
+        <v>57.25</v>
+      </c>
+      <c r="L133">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
+      <c r="A134" t="s">
+        <v>281</v>
+      </c>
+      <c r="B134" s="12">
+        <v>38057</v>
+      </c>
+      <c r="J134">
+        <v>93.289999999999992</v>
+      </c>
+      <c r="L134">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
+      <c r="A135" t="s">
+        <v>281</v>
+      </c>
+      <c r="B135" s="12">
+        <v>38066</v>
+      </c>
+      <c r="J135">
+        <v>151.34</v>
+      </c>
+      <c r="L135">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
+      <c r="A136" t="s">
+        <v>281</v>
+      </c>
+      <c r="B136" s="12">
+        <v>38071</v>
+      </c>
+      <c r="J136">
+        <v>140.99</v>
+      </c>
+      <c r="L136">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
+      <c r="A137" t="s">
+        <v>281</v>
+      </c>
+      <c r="B137" s="12">
+        <v>38077</v>
+      </c>
+      <c r="J137">
+        <v>296.70999999999998</v>
+      </c>
+      <c r="L137">
+        <v>3.49</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
+      <c r="A138" t="s">
+        <v>281</v>
+      </c>
+      <c r="B138" s="12">
+        <v>38085</v>
+      </c>
+      <c r="J138">
+        <v>500.95</v>
+      </c>
+      <c r="L138">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
+      <c r="A139" t="s">
+        <v>281</v>
+      </c>
+      <c r="B139" s="12">
+        <v>38093</v>
+      </c>
+      <c r="J139">
+        <v>539.75</v>
+      </c>
+      <c r="L139">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
+      <c r="A140" t="s">
+        <v>281</v>
+      </c>
+      <c r="B140" s="12">
+        <v>38100</v>
+      </c>
+      <c r="J140">
+        <v>758</v>
+      </c>
+      <c r="L140">
+        <v>6.41</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
+      <c r="A141" t="s">
+        <v>281</v>
+      </c>
+      <c r="B141" s="12">
+        <v>38107</v>
+      </c>
+      <c r="J141">
+        <v>896.58999999999992</v>
+      </c>
+      <c r="L141">
+        <v>5.47</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12">
+      <c r="A142" t="s">
+        <v>281</v>
+      </c>
+      <c r="B142" s="12">
+        <v>38114</v>
+      </c>
+      <c r="J142">
+        <v>1194.78</v>
+      </c>
+      <c r="L142">
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12">
+      <c r="A143" t="s">
+        <v>281</v>
+      </c>
+      <c r="B143" s="12">
+        <v>38120</v>
+      </c>
+      <c r="J143">
+        <v>1302.02</v>
+      </c>
+      <c r="L143">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12">
+      <c r="A144" t="s">
+        <v>281</v>
+      </c>
+      <c r="B144" s="12">
+        <v>38127</v>
+      </c>
+      <c r="J144">
+        <v>1100.03</v>
+      </c>
+      <c r="L144">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12">
+      <c r="A145" t="s">
+        <v>281</v>
+      </c>
+      <c r="B145" s="12">
+        <v>38135</v>
+      </c>
+      <c r="J145">
+        <v>1581.04</v>
+      </c>
+      <c r="L145">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12">
+      <c r="A146" t="s">
+        <v>281</v>
+      </c>
+      <c r="B146" s="12">
+        <v>38142</v>
+      </c>
+      <c r="I146">
+        <v>523.5</v>
+      </c>
+      <c r="J146">
+        <v>1638.4299999999998</v>
+      </c>
+      <c r="L146">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12">
+      <c r="A147" t="s">
+        <v>282</v>
+      </c>
+      <c r="B147" s="12">
+        <v>38377</v>
+      </c>
+      <c r="J147">
+        <v>90.97</v>
+      </c>
+      <c r="L147">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12">
+      <c r="A148" t="s">
+        <v>282</v>
+      </c>
+      <c r="B148" s="12">
+        <v>38411</v>
+      </c>
+      <c r="J148">
+        <v>104.09</v>
+      </c>
+      <c r="L148">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12">
+      <c r="A149" t="s">
+        <v>282</v>
+      </c>
+      <c r="B149" s="12">
+        <v>38431</v>
+      </c>
+      <c r="J149">
+        <v>150.13</v>
+      </c>
+      <c r="L149">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12">
+      <c r="A150" t="s">
+        <v>282</v>
+      </c>
+      <c r="B150" s="12">
+        <v>38436</v>
+      </c>
+      <c r="J150">
+        <v>188.15</v>
+      </c>
+      <c r="L150">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12">
+      <c r="A151" t="s">
+        <v>282</v>
+      </c>
+      <c r="B151" s="12">
+        <v>38441</v>
+      </c>
+      <c r="J151">
+        <v>236.96999999999997</v>
+      </c>
+      <c r="L151">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12">
+      <c r="A152" t="s">
+        <v>282</v>
+      </c>
+      <c r="B152" s="12">
+        <v>38452</v>
+      </c>
+      <c r="J152">
+        <v>408</v>
+      </c>
+      <c r="L152">
+        <v>4.46</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12">
+      <c r="A153" t="s">
+        <v>282</v>
+      </c>
+      <c r="B153" s="12">
+        <v>38462</v>
+      </c>
+      <c r="J153">
+        <v>373.73</v>
+      </c>
+      <c r="L153">
+        <v>5.0199999999999996</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12">
+      <c r="A154" t="s">
+        <v>282</v>
+      </c>
+      <c r="B154" s="12">
+        <v>38472</v>
+      </c>
+      <c r="J154">
+        <v>819.46</v>
+      </c>
+      <c r="L154">
+        <v>5.51</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12">
+      <c r="A155" t="s">
+        <v>282</v>
+      </c>
+      <c r="B155" s="12">
+        <v>38482</v>
+      </c>
+      <c r="J155">
+        <v>1322.84</v>
+      </c>
+      <c r="L155">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12">
+      <c r="A156" t="s">
+        <v>282</v>
+      </c>
+      <c r="B156" s="12">
+        <v>38492</v>
+      </c>
+      <c r="J156">
+        <v>986.53</v>
+      </c>
+      <c r="L156">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12">
+      <c r="A157" t="s">
+        <v>282</v>
+      </c>
+      <c r="B157" s="12">
+        <v>38502</v>
+      </c>
+      <c r="J157">
+        <v>1662.9900000000002</v>
+      </c>
+      <c r="L157">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12">
+      <c r="A158" t="s">
+        <v>282</v>
+      </c>
+      <c r="B158" s="12">
+        <v>38508</v>
+      </c>
+      <c r="J158">
+        <v>1478.8899999999999</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12">
+      <c r="A159" t="s">
+        <v>282</v>
+      </c>
+      <c r="B159" s="12">
+        <v>38511</v>
+      </c>
+      <c r="I159">
+        <v>516.9</v>
       </c>
     </row>
   </sheetData>
@@ -26665,7 +27220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="864" topLeftCell="A193" activePane="bottomLeft"/>
       <selection activeCell="M2" sqref="M2"/>
       <selection pane="bottomLeft" activeCell="C207" sqref="C207"/>

</xml_diff>

<commit_message>
Wheat validation - putting more dots on graphs
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="12" windowWidth="12120" windowHeight="6456" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="192" yWindow="12" windowWidth="12024" windowHeight="5844"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2223" uniqueCount="295">
   <si>
     <t>SimulationName</t>
   </si>
@@ -872,6 +872,42 @@
   <si>
     <t>Yucheng2004</t>
   </si>
+  <si>
+    <t>RainShelterIrrigControl</t>
+  </si>
+  <si>
+    <t>RainShelterIrrigHalf</t>
+  </si>
+  <si>
+    <t>RainShelterIrrigSpringD1</t>
+  </si>
+  <si>
+    <t>RainShelterIrrigSpringD2</t>
+  </si>
+  <si>
+    <t>RainShelterIrrigSpringD3</t>
+  </si>
+  <si>
+    <t>RainShelterIrrigSpringD4</t>
+  </si>
+  <si>
+    <t>RainShelterIrrigSummerD1</t>
+  </si>
+  <si>
+    <t>RainShelterIrrigSummerD2</t>
+  </si>
+  <si>
+    <t>RainShelterIrrigSummerD3</t>
+  </si>
+  <si>
+    <t>RainShelterIrrigSummerD4</t>
+  </si>
+  <si>
+    <t>RainShelterIrrigSummerD5</t>
+  </si>
+  <si>
+    <t>RainShelterIrrigNil</t>
+  </si>
 </sst>
 </file>
 
@@ -1409,23 +1445,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="134104960"/>
-        <c:axId val="134106496"/>
+        <c:axId val="70469888"/>
+        <c:axId val="114243072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="134104960"/>
+        <c:axId val="70469888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134106496"/>
+        <c:crossAx val="114243072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="134106496"/>
+        <c:axId val="114243072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1433,7 +1469,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="134104960"/>
+        <c:crossAx val="70469888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1445,7 +1481,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1771,17 +1807,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE231"/>
+  <dimension ref="A1:AE471"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane xSplit="11280" ySplit="708" topLeftCell="F462" activePane="bottomLeft"/>
+      <selection activeCell="B443" sqref="B443"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="D460" sqref="D460:D471"/>
+      <selection pane="bottomRight" activeCell="G460" sqref="G460:G471"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="51.5546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.109375" customWidth="1"/>
     <col min="5" max="5" width="28.5546875" customWidth="1"/>
     <col min="6" max="6" width="34.33203125" customWidth="1"/>
@@ -13863,6 +13903,2832 @@
         <v>37.9</v>
       </c>
     </row>
+    <row r="232" spans="1:31">
+      <c r="A232" t="s">
+        <v>193</v>
+      </c>
+      <c r="B232" s="6">
+        <v>41459</v>
+      </c>
+      <c r="E232" s="7">
+        <v>259.60892857142858</v>
+      </c>
+      <c r="G232" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:31">
+      <c r="A233" t="s">
+        <v>193</v>
+      </c>
+      <c r="B233" s="6">
+        <v>41520</v>
+      </c>
+      <c r="E233" s="7">
+        <v>649.67857142857144</v>
+      </c>
+      <c r="G233" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:31">
+      <c r="A234" t="s">
+        <v>193</v>
+      </c>
+      <c r="B234" s="6">
+        <v>41569</v>
+      </c>
+      <c r="E234" s="7">
+        <v>1402.8307463434955</v>
+      </c>
+      <c r="G234" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:31">
+      <c r="A235" t="s">
+        <v>193</v>
+      </c>
+      <c r="B235" s="6">
+        <v>41582</v>
+      </c>
+      <c r="E235" s="7">
+        <v>1751.3349013553025</v>
+      </c>
+      <c r="G235" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:31">
+      <c r="A236" t="s">
+        <v>193</v>
+      </c>
+      <c r="B236" s="6">
+        <v>41596</v>
+      </c>
+      <c r="E236" s="7">
+        <v>1887.00612321624</v>
+      </c>
+      <c r="G236" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:31">
+      <c r="A237" t="s">
+        <v>193</v>
+      </c>
+      <c r="B237" s="6">
+        <v>41610</v>
+      </c>
+      <c r="E237" s="7">
+        <v>2249.0845984679604</v>
+      </c>
+      <c r="G237" s="7">
+        <v>75.125780348288274</v>
+      </c>
+    </row>
+    <row r="238" spans="1:31">
+      <c r="A238" t="s">
+        <v>193</v>
+      </c>
+      <c r="B238" s="6">
+        <v>41625</v>
+      </c>
+      <c r="E238" s="7">
+        <v>2993.4587204772688</v>
+      </c>
+      <c r="G238" s="7">
+        <v>674.19936772259132</v>
+      </c>
+    </row>
+    <row r="239" spans="1:31">
+      <c r="A239" t="s">
+        <v>193</v>
+      </c>
+      <c r="B239" s="6">
+        <v>41664</v>
+      </c>
+      <c r="C239" s="1">
+        <v>90</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E239" s="7">
+        <v>2625.4943707521256</v>
+      </c>
+      <c r="G239" s="7">
+        <v>885.4530850000001</v>
+      </c>
+    </row>
+    <row r="240" spans="1:31">
+      <c r="A240" t="s">
+        <v>194</v>
+      </c>
+      <c r="B240" s="6">
+        <v>41459</v>
+      </c>
+      <c r="E240" s="7">
+        <v>226.8970238095238</v>
+      </c>
+      <c r="G240" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7">
+      <c r="A241" t="s">
+        <v>194</v>
+      </c>
+      <c r="B241" s="6">
+        <v>41520</v>
+      </c>
+      <c r="E241" s="7">
+        <v>624.35714285714289</v>
+      </c>
+      <c r="G241" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7">
+      <c r="A242" t="s">
+        <v>194</v>
+      </c>
+      <c r="B242" s="6">
+        <v>41569</v>
+      </c>
+      <c r="E242" s="7">
+        <v>1362.8234278234299</v>
+      </c>
+      <c r="G242" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7">
+      <c r="A243" t="s">
+        <v>194</v>
+      </c>
+      <c r="B243" s="6">
+        <v>41582</v>
+      </c>
+      <c r="E243" s="7">
+        <v>1620.5776179914026</v>
+      </c>
+      <c r="G243" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7">
+      <c r="A244" t="s">
+        <v>194</v>
+      </c>
+      <c r="B244" s="6">
+        <v>41596</v>
+      </c>
+      <c r="E244" s="7">
+        <v>1948.067399882359</v>
+      </c>
+      <c r="G244" s="7">
+        <v>13.980240013994239</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7">
+      <c r="A245" t="s">
+        <v>194</v>
+      </c>
+      <c r="B245" s="6">
+        <v>41610</v>
+      </c>
+      <c r="E245" s="7">
+        <v>2109.728760647753</v>
+      </c>
+      <c r="G245" s="7">
+        <v>190.56940146327679</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7">
+      <c r="A246" t="s">
+        <v>194</v>
+      </c>
+      <c r="B246" s="6">
+        <v>41625</v>
+      </c>
+      <c r="E246" s="7">
+        <v>2370.9786599317072</v>
+      </c>
+      <c r="G246" s="7">
+        <v>590.5571996210947</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7">
+      <c r="A247" t="s">
+        <v>194</v>
+      </c>
+      <c r="B247" s="6">
+        <v>41664</v>
+      </c>
+      <c r="C247" s="1">
+        <v>90</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E247" s="7">
+        <v>2121.6746017489827</v>
+      </c>
+      <c r="G247" s="7">
+        <v>682.3106949999999</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7">
+      <c r="A248" t="s">
+        <v>195</v>
+      </c>
+      <c r="B248" s="6">
+        <v>41459</v>
+      </c>
+      <c r="E248" s="7">
+        <v>249.91249999999994</v>
+      </c>
+      <c r="G248" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7">
+      <c r="A249" t="s">
+        <v>195</v>
+      </c>
+      <c r="B249" s="6">
+        <v>41520</v>
+      </c>
+      <c r="E249" s="7">
+        <v>627.47023809523807</v>
+      </c>
+      <c r="G249" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7">
+      <c r="A250" t="s">
+        <v>195</v>
+      </c>
+      <c r="B250" s="6">
+        <v>41569</v>
+      </c>
+      <c r="E250" s="7">
+        <v>1264.469068519624</v>
+      </c>
+      <c r="G250" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7">
+      <c r="A251" t="s">
+        <v>195</v>
+      </c>
+      <c r="B251" s="6">
+        <v>41582</v>
+      </c>
+      <c r="E251" s="7">
+        <v>1697.7749033869459</v>
+      </c>
+      <c r="G251" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7">
+      <c r="A252" t="s">
+        <v>195</v>
+      </c>
+      <c r="B252" s="6">
+        <v>41596</v>
+      </c>
+      <c r="E252" s="7">
+        <v>1996.7879625524304</v>
+      </c>
+      <c r="G252" s="7">
+        <v>11.153680586309871</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7">
+      <c r="A253" t="s">
+        <v>195</v>
+      </c>
+      <c r="B253" s="6">
+        <v>41610</v>
+      </c>
+      <c r="E253" s="7">
+        <v>2130.6560161990783</v>
+      </c>
+      <c r="G253" s="7">
+        <v>168.78927445061521</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7">
+      <c r="A254" t="s">
+        <v>195</v>
+      </c>
+      <c r="B254" s="6">
+        <v>41625</v>
+      </c>
+      <c r="E254" s="7">
+        <v>2922.3662748673055</v>
+      </c>
+      <c r="G254" s="7">
+        <v>789.0796191460812</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7">
+      <c r="A255" t="s">
+        <v>195</v>
+      </c>
+      <c r="B255" s="6">
+        <v>41664</v>
+      </c>
+      <c r="C255" s="1">
+        <v>90</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E255" s="7">
+        <v>2408.9480068087651</v>
+      </c>
+      <c r="G255" s="7">
+        <v>939.17181999999991</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7">
+      <c r="A256" t="s">
+        <v>196</v>
+      </c>
+      <c r="B256" s="6">
+        <v>41459</v>
+      </c>
+      <c r="E256" s="7">
+        <v>234.35535714285714</v>
+      </c>
+      <c r="G256" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7">
+      <c r="A257" t="s">
+        <v>196</v>
+      </c>
+      <c r="B257" s="6">
+        <v>41520</v>
+      </c>
+      <c r="E257" s="7">
+        <v>609.67261904761904</v>
+      </c>
+      <c r="G257" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7">
+      <c r="A258" t="s">
+        <v>196</v>
+      </c>
+      <c r="B258" s="6">
+        <v>41569</v>
+      </c>
+      <c r="E258" s="7">
+        <v>1221.1821011129721</v>
+      </c>
+      <c r="G258" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7">
+      <c r="A259" t="s">
+        <v>196</v>
+      </c>
+      <c r="B259" s="6">
+        <v>41582</v>
+      </c>
+      <c r="E259" s="7">
+        <v>1741.3625136754131</v>
+      </c>
+      <c r="G259" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7">
+      <c r="A260" t="s">
+        <v>196</v>
+      </c>
+      <c r="B260" s="6">
+        <v>41596</v>
+      </c>
+      <c r="E260" s="7">
+        <v>2123.5220807464707</v>
+      </c>
+      <c r="G260" s="7">
+        <v>19.173452652310573</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7">
+      <c r="A261" t="s">
+        <v>196</v>
+      </c>
+      <c r="B261" s="6">
+        <v>41610</v>
+      </c>
+      <c r="E261" s="7">
+        <v>2263.3544949769112</v>
+      </c>
+      <c r="G261" s="7">
+        <v>190.79860792638289</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7">
+      <c r="A262" t="s">
+        <v>196</v>
+      </c>
+      <c r="B262" s="6">
+        <v>41625</v>
+      </c>
+      <c r="E262" s="7">
+        <v>2799.2876533741037</v>
+      </c>
+      <c r="G262" s="7">
+        <v>793.51438215060045</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7">
+      <c r="A263" t="s">
+        <v>196</v>
+      </c>
+      <c r="B263" s="6">
+        <v>41664</v>
+      </c>
+      <c r="C263" s="1">
+        <v>90</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E263" s="7">
+        <v>2468.3094723972449</v>
+      </c>
+      <c r="G263" s="7">
+        <v>954.44929750000006</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7">
+      <c r="A264" t="s">
+        <v>197</v>
+      </c>
+      <c r="B264" s="6">
+        <v>41459</v>
+      </c>
+      <c r="E264" s="7">
+        <v>265.64404761904763</v>
+      </c>
+      <c r="G264" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7">
+      <c r="A265" t="s">
+        <v>197</v>
+      </c>
+      <c r="B265" s="6">
+        <v>41520</v>
+      </c>
+      <c r="E265" s="7">
+        <v>675.00595238095241</v>
+      </c>
+      <c r="G265" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7">
+      <c r="A266" t="s">
+        <v>197</v>
+      </c>
+      <c r="B266" s="6">
+        <v>41569</v>
+      </c>
+      <c r="E266" s="7">
+        <v>1297.9274261316932</v>
+      </c>
+      <c r="G266" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7">
+      <c r="A267" t="s">
+        <v>197</v>
+      </c>
+      <c r="B267" s="6">
+        <v>41582</v>
+      </c>
+      <c r="E267" s="7">
+        <v>1793.2180091010782</v>
+      </c>
+      <c r="G267" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7">
+      <c r="A268" t="s">
+        <v>197</v>
+      </c>
+      <c r="B268" s="6">
+        <v>41596</v>
+      </c>
+      <c r="E268" s="7">
+        <v>2003.9743996700238</v>
+      </c>
+      <c r="G268" s="7">
+        <v>3.4552826398587286</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7">
+      <c r="A269" t="s">
+        <v>197</v>
+      </c>
+      <c r="B269" s="6">
+        <v>41610</v>
+      </c>
+      <c r="E269" s="7">
+        <v>2222.9738840553596</v>
+      </c>
+      <c r="G269" s="7">
+        <v>147.75605742630131</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7">
+      <c r="A270" t="s">
+        <v>197</v>
+      </c>
+      <c r="B270" s="6">
+        <v>41625</v>
+      </c>
+      <c r="E270" s="7">
+        <v>2842.3258907459699</v>
+      </c>
+      <c r="G270" s="7">
+        <v>750.80083243980357</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7">
+      <c r="A271" t="s">
+        <v>197</v>
+      </c>
+      <c r="B271" s="6">
+        <v>41664</v>
+      </c>
+      <c r="C271" s="1">
+        <v>90</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E271" s="7">
+        <v>2474.0820469697851</v>
+      </c>
+      <c r="G271" s="7">
+        <v>861.81991500000004</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7">
+      <c r="A272" t="s">
+        <v>198</v>
+      </c>
+      <c r="B272" s="6">
+        <v>41459</v>
+      </c>
+      <c r="E272" s="7">
+        <v>244.48333333333335</v>
+      </c>
+      <c r="G272" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7">
+      <c r="A273" t="s">
+        <v>198</v>
+      </c>
+      <c r="B273" s="6">
+        <v>41520</v>
+      </c>
+      <c r="E273" s="7">
+        <v>608.39285714285711</v>
+      </c>
+      <c r="G273" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7">
+      <c r="A274" t="s">
+        <v>198</v>
+      </c>
+      <c r="B274" s="12">
+        <v>41569</v>
+      </c>
+      <c r="E274">
+        <v>1466.2124007666825</v>
+      </c>
+      <c r="G274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7">
+      <c r="A275" t="s">
+        <v>198</v>
+      </c>
+      <c r="B275" s="12">
+        <v>41582</v>
+      </c>
+      <c r="E275">
+        <v>1781.801942144639</v>
+      </c>
+      <c r="G275">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7">
+      <c r="A276" t="s">
+        <v>198</v>
+      </c>
+      <c r="B276" s="12">
+        <v>41596</v>
+      </c>
+      <c r="E276">
+        <v>2089.064179160293</v>
+      </c>
+      <c r="G276">
+        <v>0.28549387128289255</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7">
+      <c r="A277" t="s">
+        <v>198</v>
+      </c>
+      <c r="B277" s="12">
+        <v>41610</v>
+      </c>
+      <c r="E277">
+        <v>2427.434594961032</v>
+      </c>
+      <c r="G277">
+        <v>154.97552617836226</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7">
+      <c r="A278" t="s">
+        <v>198</v>
+      </c>
+      <c r="B278" s="12">
+        <v>41625</v>
+      </c>
+      <c r="E278">
+        <v>2932.0284623086782</v>
+      </c>
+      <c r="G278">
+        <v>675.26504150544918</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7">
+      <c r="A279" t="s">
+        <v>198</v>
+      </c>
+      <c r="B279" s="12">
+        <v>41664</v>
+      </c>
+      <c r="C279" s="1">
+        <v>90</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E279">
+        <v>2619.6985123527334</v>
+      </c>
+      <c r="G279">
+        <v>904.03921750000006</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7">
+      <c r="A280" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B280" s="12">
+        <v>33505</v>
+      </c>
+      <c r="E280">
+        <v>176.9</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7">
+      <c r="A281" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B281" s="12">
+        <v>33505</v>
+      </c>
+      <c r="E281">
+        <v>263.75</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7">
+      <c r="A282" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B282" s="12">
+        <v>33505</v>
+      </c>
+      <c r="E282">
+        <v>183.7</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7">
+      <c r="A283" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B283" s="12">
+        <v>33505</v>
+      </c>
+      <c r="E283">
+        <v>216.98</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7">
+      <c r="A284" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B284" s="12">
+        <v>33505</v>
+      </c>
+      <c r="E284">
+        <v>231.05</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7">
+      <c r="A285" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B285" s="12">
+        <v>33505</v>
+      </c>
+      <c r="E285">
+        <v>249.6</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7">
+      <c r="A286" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B286" s="12">
+        <v>33505</v>
+      </c>
+      <c r="E286">
+        <v>230.43</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7">
+      <c r="A287" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B287" s="12">
+        <v>33505</v>
+      </c>
+      <c r="E287">
+        <v>202.2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7">
+      <c r="A288" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B288" s="12">
+        <v>33505</v>
+      </c>
+      <c r="E288">
+        <v>182.98</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5">
+      <c r="A289" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B289" s="12">
+        <v>33505</v>
+      </c>
+      <c r="E289">
+        <v>250.8</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5">
+      <c r="A290" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B290" s="12">
+        <v>33505</v>
+      </c>
+      <c r="E290">
+        <v>187.53</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5">
+      <c r="A291" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B291" s="12">
+        <v>33505</v>
+      </c>
+      <c r="E291">
+        <v>164.83</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5">
+      <c r="A292" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B292" s="12">
+        <v>33521</v>
+      </c>
+      <c r="E292">
+        <v>419.2</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5">
+      <c r="A293" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B293" s="12">
+        <v>33521</v>
+      </c>
+      <c r="E293">
+        <v>450.5</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5">
+      <c r="A294" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B294" s="12">
+        <v>33521</v>
+      </c>
+      <c r="E294">
+        <v>372.2</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5">
+      <c r="A295" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B295" s="12">
+        <v>33521</v>
+      </c>
+      <c r="E295">
+        <v>497.48</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5">
+      <c r="A296" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B296" s="12">
+        <v>33521</v>
+      </c>
+      <c r="E296">
+        <v>516.85</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5">
+      <c r="A297" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B297" s="12">
+        <v>33521</v>
+      </c>
+      <c r="E297">
+        <v>467.08</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5">
+      <c r="A298" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B298" s="12">
+        <v>33521</v>
+      </c>
+      <c r="E298">
+        <v>457.68</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5">
+      <c r="A299" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B299" s="12">
+        <v>33521</v>
+      </c>
+      <c r="E299">
+        <v>401.83</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5">
+      <c r="A300" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B300" s="12">
+        <v>33521</v>
+      </c>
+      <c r="E300">
+        <v>414.43</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5">
+      <c r="A301" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B301" s="12">
+        <v>33521</v>
+      </c>
+      <c r="E301">
+        <v>438.08</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5">
+      <c r="A302" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B302" s="12">
+        <v>33521</v>
+      </c>
+      <c r="E302">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5">
+      <c r="A303" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B303" s="12">
+        <v>33521</v>
+      </c>
+      <c r="E303">
+        <v>395.75</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5">
+      <c r="A304" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B304" s="12">
+        <v>33533</v>
+      </c>
+      <c r="E304">
+        <v>589.63</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5">
+      <c r="A305" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B305" s="12">
+        <v>33533</v>
+      </c>
+      <c r="E305">
+        <v>735.55</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5">
+      <c r="A306" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B306" s="12">
+        <v>33533</v>
+      </c>
+      <c r="E306">
+        <v>618.48</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5">
+      <c r="A307" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B307" s="12">
+        <v>33533</v>
+      </c>
+      <c r="E307">
+        <v>781.45</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5">
+      <c r="A308" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B308" s="12">
+        <v>33533</v>
+      </c>
+      <c r="E308">
+        <v>814.3</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5">
+      <c r="A309" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B309" s="12">
+        <v>33533</v>
+      </c>
+      <c r="E309">
+        <v>679.58</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5">
+      <c r="A310" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B310" s="12">
+        <v>33533</v>
+      </c>
+      <c r="E310">
+        <v>623.20000000000005</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5">
+      <c r="A311" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B311" s="12">
+        <v>33533</v>
+      </c>
+      <c r="E311">
+        <v>771.53</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5">
+      <c r="A312" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B312" s="12">
+        <v>33533</v>
+      </c>
+      <c r="E312">
+        <v>682.15</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5">
+      <c r="A313" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B313" s="12">
+        <v>33533</v>
+      </c>
+      <c r="E313">
+        <v>573.20000000000005</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5">
+      <c r="A314" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B314" s="12">
+        <v>33533</v>
+      </c>
+      <c r="E314">
+        <v>676.3</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5">
+      <c r="A315" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B315" s="12">
+        <v>33533</v>
+      </c>
+      <c r="E315">
+        <v>569.78</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5">
+      <c r="A316" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B316" s="12">
+        <v>33547</v>
+      </c>
+      <c r="E316">
+        <v>963.05</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5">
+      <c r="A317" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B317" s="12">
+        <v>33547</v>
+      </c>
+      <c r="E317">
+        <v>1057.8800000000001</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5">
+      <c r="A318" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B318" s="12">
+        <v>33547</v>
+      </c>
+      <c r="E318">
+        <v>862.88</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5">
+      <c r="A319" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B319" s="12">
+        <v>33547</v>
+      </c>
+      <c r="E319">
+        <v>845.6</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5">
+      <c r="A320" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B320" s="12">
+        <v>33547</v>
+      </c>
+      <c r="E320">
+        <v>1106.95</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5">
+      <c r="A321" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B321" s="12">
+        <v>33547</v>
+      </c>
+      <c r="E321">
+        <v>887.9</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5">
+      <c r="A322" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B322" s="12">
+        <v>33547</v>
+      </c>
+      <c r="E322">
+        <v>750.13</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5">
+      <c r="A323" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B323" s="12">
+        <v>33547</v>
+      </c>
+      <c r="E323">
+        <v>1092.8</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5">
+      <c r="A324" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B324" s="12">
+        <v>33547</v>
+      </c>
+      <c r="E324">
+        <v>824.58</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5">
+      <c r="A325" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B325" s="12">
+        <v>33547</v>
+      </c>
+      <c r="E325">
+        <v>874.25</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5">
+      <c r="A326" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B326" s="12">
+        <v>33547</v>
+      </c>
+      <c r="E326">
+        <v>1088.4000000000001</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5">
+      <c r="A327" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B327" s="12">
+        <v>33547</v>
+      </c>
+      <c r="E327">
+        <v>818.53</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5">
+      <c r="A328" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B328" s="12">
+        <v>33561</v>
+      </c>
+      <c r="E328">
+        <v>1307.08</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5">
+      <c r="A329" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B329" s="12">
+        <v>33561</v>
+      </c>
+      <c r="E329">
+        <v>1591.55</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5">
+      <c r="A330" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B330" s="12">
+        <v>33561</v>
+      </c>
+      <c r="E330">
+        <v>1501.1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5">
+      <c r="A331" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B331" s="12">
+        <v>33561</v>
+      </c>
+      <c r="E331">
+        <v>1520.2</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5">
+      <c r="A332" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B332" s="12">
+        <v>33561</v>
+      </c>
+      <c r="E332">
+        <v>1228.05</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5">
+      <c r="A333" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B333" s="12">
+        <v>33561</v>
+      </c>
+      <c r="E333">
+        <v>1151.83</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5">
+      <c r="A334" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B334" s="12">
+        <v>33561</v>
+      </c>
+      <c r="E334">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5">
+      <c r="A335" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B335" s="12">
+        <v>33561</v>
+      </c>
+      <c r="E335">
+        <v>1508.83</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5">
+      <c r="A336" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B336" s="12">
+        <v>33561</v>
+      </c>
+      <c r="E336">
+        <v>1647.48</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5">
+      <c r="A337" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B337" s="12">
+        <v>33561</v>
+      </c>
+      <c r="E337">
+        <v>1575.03</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5">
+      <c r="A338" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B338" s="12">
+        <v>33561</v>
+      </c>
+      <c r="E338">
+        <v>1266.18</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5">
+      <c r="A339" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B339" s="12">
+        <v>33561</v>
+      </c>
+      <c r="E339">
+        <v>1024.25</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5">
+      <c r="A340" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B340" s="12">
+        <v>33568</v>
+      </c>
+      <c r="E340">
+        <v>1501.28</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5">
+      <c r="A341" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B341" s="12">
+        <v>33568</v>
+      </c>
+      <c r="E341">
+        <v>1047.23</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5">
+      <c r="A342" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B342" s="12">
+        <v>33568</v>
+      </c>
+      <c r="E342">
+        <v>1662.8</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5">
+      <c r="A343" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B343" s="12">
+        <v>33568</v>
+      </c>
+      <c r="E343">
+        <v>1418.4</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5">
+      <c r="A344" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B344" s="12">
+        <v>33568</v>
+      </c>
+      <c r="E344">
+        <v>1706.63</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5">
+      <c r="A345" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B345" s="12">
+        <v>33568</v>
+      </c>
+      <c r="E345">
+        <v>1281.5999999999999</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5">
+      <c r="A346" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B346" s="12">
+        <v>33568</v>
+      </c>
+      <c r="E346">
+        <v>1341.55</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5">
+      <c r="A347" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B347" s="12">
+        <v>33568</v>
+      </c>
+      <c r="E347">
+        <v>1483.85</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5">
+      <c r="A348" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B348" s="12">
+        <v>33568</v>
+      </c>
+      <c r="E348">
+        <v>1689.18</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5">
+      <c r="A349" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B349" s="12">
+        <v>33568</v>
+      </c>
+      <c r="E349">
+        <v>1622.85</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5">
+      <c r="A350" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B350" s="12">
+        <v>33568</v>
+      </c>
+      <c r="E350">
+        <v>1751.78</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5">
+      <c r="A351" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B351" s="12">
+        <v>33568</v>
+      </c>
+      <c r="E351">
+        <v>1055.43</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5">
+      <c r="A352" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B352" s="12">
+        <v>33574</v>
+      </c>
+      <c r="E352">
+        <v>1751.78</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5">
+      <c r="A353" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B353" s="12">
+        <v>33574</v>
+      </c>
+      <c r="E353">
+        <v>1591.6</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5">
+      <c r="A354" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B354" s="12">
+        <v>33574</v>
+      </c>
+      <c r="E354">
+        <v>1647.38</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5">
+      <c r="A355" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B355" s="12">
+        <v>33574</v>
+      </c>
+      <c r="E355">
+        <v>2095.0300000000002</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5">
+      <c r="A356" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B356" s="12">
+        <v>33574</v>
+      </c>
+      <c r="E356">
+        <v>1282.25</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5">
+      <c r="A357" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B357" s="12">
+        <v>33574</v>
+      </c>
+      <c r="E357">
+        <v>1377.55</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5">
+      <c r="A358" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B358" s="12">
+        <v>33574</v>
+      </c>
+      <c r="E358">
+        <v>1476.58</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5">
+      <c r="A359" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B359" s="12">
+        <v>33574</v>
+      </c>
+      <c r="E359">
+        <v>1662.78</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5">
+      <c r="A360" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B360" s="12">
+        <v>33574</v>
+      </c>
+      <c r="E360">
+        <v>1701.48</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5">
+      <c r="A361" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B361" s="12">
+        <v>33574</v>
+      </c>
+      <c r="E361">
+        <v>2028.48</v>
+      </c>
+    </row>
+    <row r="362" spans="1:5">
+      <c r="A362" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B362" s="12">
+        <v>33574</v>
+      </c>
+      <c r="E362">
+        <v>1984.3</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5">
+      <c r="A363" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B363" s="12">
+        <v>33574</v>
+      </c>
+      <c r="E363">
+        <v>1266.68</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5">
+      <c r="A364" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B364" s="12">
+        <v>33581</v>
+      </c>
+      <c r="E364">
+        <v>2299.75</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5">
+      <c r="A365" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B365" s="12">
+        <v>33581</v>
+      </c>
+      <c r="E365">
+        <v>2155.3000000000002</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5">
+      <c r="A366" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B366" s="12">
+        <v>33581</v>
+      </c>
+      <c r="E366">
+        <v>2025.98</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5">
+      <c r="A367" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B367" s="12">
+        <v>33581</v>
+      </c>
+      <c r="E367">
+        <v>1881.5</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5">
+      <c r="A368" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B368" s="12">
+        <v>33581</v>
+      </c>
+      <c r="E368">
+        <v>1769.48</v>
+      </c>
+    </row>
+    <row r="369" spans="1:5">
+      <c r="A369" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B369" s="12">
+        <v>33581</v>
+      </c>
+      <c r="E369">
+        <v>1525.78</v>
+      </c>
+    </row>
+    <row r="370" spans="1:5">
+      <c r="A370" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B370" s="12">
+        <v>33581</v>
+      </c>
+      <c r="E370">
+        <v>1651.03</v>
+      </c>
+    </row>
+    <row r="371" spans="1:5">
+      <c r="A371" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B371" s="12">
+        <v>33581</v>
+      </c>
+      <c r="E371">
+        <v>2105.9</v>
+      </c>
+    </row>
+    <row r="372" spans="1:5">
+      <c r="A372" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B372" s="12">
+        <v>33581</v>
+      </c>
+      <c r="E372">
+        <v>2266.4299999999998</v>
+      </c>
+    </row>
+    <row r="373" spans="1:5">
+      <c r="A373" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B373" s="12">
+        <v>33581</v>
+      </c>
+      <c r="E373">
+        <v>2044.33</v>
+      </c>
+    </row>
+    <row r="374" spans="1:5">
+      <c r="A374" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B374" s="12">
+        <v>33581</v>
+      </c>
+      <c r="E374">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="375" spans="1:5">
+      <c r="A375" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B375" s="12">
+        <v>33581</v>
+      </c>
+      <c r="E375">
+        <v>1387.15</v>
+      </c>
+    </row>
+    <row r="376" spans="1:5">
+      <c r="A376" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B376" s="12">
+        <v>33585</v>
+      </c>
+      <c r="E376">
+        <v>2326.25</v>
+      </c>
+    </row>
+    <row r="377" spans="1:5">
+      <c r="A377" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B377" s="12">
+        <v>33585</v>
+      </c>
+      <c r="E377">
+        <v>2204.6999999999998</v>
+      </c>
+    </row>
+    <row r="378" spans="1:5">
+      <c r="A378" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B378" s="12">
+        <v>33585</v>
+      </c>
+      <c r="E378">
+        <v>1656.98</v>
+      </c>
+    </row>
+    <row r="379" spans="1:5">
+      <c r="A379" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B379" s="12">
+        <v>33585</v>
+      </c>
+      <c r="E379">
+        <v>2187.5500000000002</v>
+      </c>
+    </row>
+    <row r="380" spans="1:5">
+      <c r="A380" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B380" s="12">
+        <v>33585</v>
+      </c>
+      <c r="E380">
+        <v>1650.3</v>
+      </c>
+    </row>
+    <row r="381" spans="1:5">
+      <c r="A381" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B381" s="12">
+        <v>33585</v>
+      </c>
+      <c r="E381">
+        <v>1350.48</v>
+      </c>
+    </row>
+    <row r="382" spans="1:5">
+      <c r="A382" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B382" s="12">
+        <v>33585</v>
+      </c>
+      <c r="E382">
+        <v>1632.25</v>
+      </c>
+    </row>
+    <row r="383" spans="1:5">
+      <c r="A383" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B383" s="12">
+        <v>33585</v>
+      </c>
+      <c r="E383">
+        <v>2091.73</v>
+      </c>
+    </row>
+    <row r="384" spans="1:5">
+      <c r="A384" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B384" s="12">
+        <v>33585</v>
+      </c>
+      <c r="E384">
+        <v>2056</v>
+      </c>
+    </row>
+    <row r="385" spans="1:5">
+      <c r="A385" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B385" s="12">
+        <v>33585</v>
+      </c>
+      <c r="E385">
+        <v>1968.43</v>
+      </c>
+    </row>
+    <row r="386" spans="1:5">
+      <c r="A386" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B386" s="12">
+        <v>33585</v>
+      </c>
+      <c r="E386">
+        <v>2301.6799999999998</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5">
+      <c r="A387" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B387" s="12">
+        <v>33585</v>
+      </c>
+      <c r="E387">
+        <v>1231.43</v>
+      </c>
+    </row>
+    <row r="388" spans="1:5">
+      <c r="A388" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B388" s="12">
+        <v>33590</v>
+      </c>
+      <c r="E388">
+        <v>2224.7800000000002</v>
+      </c>
+    </row>
+    <row r="389" spans="1:5">
+      <c r="A389" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B389" s="12">
+        <v>33590</v>
+      </c>
+      <c r="E389">
+        <v>1912.63</v>
+      </c>
+    </row>
+    <row r="390" spans="1:5">
+      <c r="A390" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B390" s="12">
+        <v>33590</v>
+      </c>
+      <c r="E390">
+        <v>2054.35</v>
+      </c>
+    </row>
+    <row r="391" spans="1:5">
+      <c r="A391" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B391" s="12">
+        <v>33590</v>
+      </c>
+      <c r="E391">
+        <v>2122.0500000000002</v>
+      </c>
+    </row>
+    <row r="392" spans="1:5">
+      <c r="A392" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B392" s="12">
+        <v>33590</v>
+      </c>
+      <c r="E392">
+        <v>1663.3</v>
+      </c>
+    </row>
+    <row r="393" spans="1:5">
+      <c r="A393" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B393" s="12">
+        <v>33590</v>
+      </c>
+      <c r="E393">
+        <v>1502.85</v>
+      </c>
+    </row>
+    <row r="394" spans="1:5">
+      <c r="A394" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B394" s="12">
+        <v>33590</v>
+      </c>
+      <c r="E394">
+        <v>1452.43</v>
+      </c>
+    </row>
+    <row r="395" spans="1:5">
+      <c r="A395" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B395" s="12">
+        <v>33590</v>
+      </c>
+      <c r="E395">
+        <v>1681.98</v>
+      </c>
+    </row>
+    <row r="396" spans="1:5">
+      <c r="A396" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B396" s="12">
+        <v>33590</v>
+      </c>
+      <c r="E396">
+        <v>1863.68</v>
+      </c>
+    </row>
+    <row r="397" spans="1:5">
+      <c r="A397" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B397" s="12">
+        <v>33590</v>
+      </c>
+      <c r="E397">
+        <v>2257.63</v>
+      </c>
+    </row>
+    <row r="398" spans="1:5">
+      <c r="A398" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B398" s="12">
+        <v>33590</v>
+      </c>
+      <c r="E398">
+        <v>2140.4499999999998</v>
+      </c>
+    </row>
+    <row r="399" spans="1:5">
+      <c r="A399" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B399" s="12">
+        <v>33590</v>
+      </c>
+      <c r="E399">
+        <v>1455.98</v>
+      </c>
+    </row>
+    <row r="400" spans="1:5">
+      <c r="A400" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B400" s="12">
+        <v>33595</v>
+      </c>
+      <c r="E400">
+        <v>2313.6999999999998</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5">
+      <c r="A401" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B401" s="12">
+        <v>33595</v>
+      </c>
+      <c r="E401">
+        <v>2238.63</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5">
+      <c r="A402" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B402" s="12">
+        <v>33595</v>
+      </c>
+      <c r="E402">
+        <v>2337.1999999999998</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5">
+      <c r="A403" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B403" s="12">
+        <v>33595</v>
+      </c>
+      <c r="E403">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5">
+      <c r="A404" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B404" s="12">
+        <v>33595</v>
+      </c>
+      <c r="E404">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5">
+      <c r="A405" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B405" s="12">
+        <v>33595</v>
+      </c>
+      <c r="E405">
+        <v>1362.03</v>
+      </c>
+    </row>
+    <row r="406" spans="1:5">
+      <c r="A406" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B406" s="12">
+        <v>33595</v>
+      </c>
+      <c r="E406">
+        <v>1698.15</v>
+      </c>
+    </row>
+    <row r="407" spans="1:5">
+      <c r="A407" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B407" s="12">
+        <v>33595</v>
+      </c>
+      <c r="E407">
+        <v>2075.23</v>
+      </c>
+    </row>
+    <row r="408" spans="1:5">
+      <c r="A408" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B408" s="12">
+        <v>33595</v>
+      </c>
+      <c r="E408">
+        <v>1831.4</v>
+      </c>
+    </row>
+    <row r="409" spans="1:5">
+      <c r="A409" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B409" s="12">
+        <v>33595</v>
+      </c>
+      <c r="E409">
+        <v>1932.68</v>
+      </c>
+    </row>
+    <row r="410" spans="1:5">
+      <c r="A410" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B410" s="12">
+        <v>33595</v>
+      </c>
+      <c r="E410">
+        <v>2174.83</v>
+      </c>
+    </row>
+    <row r="411" spans="1:5">
+      <c r="A411" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B411" s="12">
+        <v>33595</v>
+      </c>
+      <c r="E411">
+        <v>1439.9</v>
+      </c>
+    </row>
+    <row r="412" spans="1:5">
+      <c r="A412" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B412" s="12">
+        <v>33602</v>
+      </c>
+      <c r="E412">
+        <v>2315.5500000000002</v>
+      </c>
+    </row>
+    <row r="413" spans="1:5">
+      <c r="A413" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B413" s="12">
+        <v>33602</v>
+      </c>
+      <c r="E413">
+        <v>2452.4</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5">
+      <c r="A414" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B414" s="12">
+        <v>33602</v>
+      </c>
+      <c r="E414">
+        <v>2457.38</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5">
+      <c r="A415" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B415" s="12">
+        <v>33602</v>
+      </c>
+      <c r="E415">
+        <v>1634.63</v>
+      </c>
+    </row>
+    <row r="416" spans="1:5">
+      <c r="A416" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B416" s="12">
+        <v>33602</v>
+      </c>
+      <c r="E416">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="417" spans="1:5">
+      <c r="A417" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B417" s="12">
+        <v>33602</v>
+      </c>
+      <c r="E417">
+        <v>1880.6</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5">
+      <c r="A418" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B418" s="12">
+        <v>33602</v>
+      </c>
+    </row>
+    <row r="419" spans="1:5">
+      <c r="A419" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B419" s="12">
+        <v>33602</v>
+      </c>
+      <c r="E419">
+        <v>1831.08</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5">
+      <c r="A420" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B420" s="12">
+        <v>33602</v>
+      </c>
+      <c r="E420">
+        <v>2186.3000000000002</v>
+      </c>
+    </row>
+    <row r="421" spans="1:5">
+      <c r="A421" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B421" s="12">
+        <v>33602</v>
+      </c>
+      <c r="E421">
+        <v>2030.43</v>
+      </c>
+    </row>
+    <row r="422" spans="1:5">
+      <c r="A422" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B422" s="12">
+        <v>33602</v>
+      </c>
+      <c r="E422">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5">
+      <c r="A423" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B423" s="12">
+        <v>33602</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5">
+      <c r="A424" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B424" s="12">
+        <v>33609</v>
+      </c>
+      <c r="E424">
+        <v>2595.6999999999998</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5">
+      <c r="A425" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B425" s="12">
+        <v>33609</v>
+      </c>
+      <c r="E425">
+        <v>2308.2800000000002</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5">
+      <c r="A426" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B426" s="12">
+        <v>33609</v>
+      </c>
+      <c r="E426">
+        <v>2505.4499999999998</v>
+      </c>
+    </row>
+    <row r="427" spans="1:5">
+      <c r="A427" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B427" s="12">
+        <v>33609</v>
+      </c>
+      <c r="E427">
+        <v>1955.8</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5">
+      <c r="A428" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B428" s="12">
+        <v>33609</v>
+      </c>
+      <c r="E428">
+        <v>1854.05</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5">
+      <c r="A429" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B429" s="12">
+        <v>33609</v>
+      </c>
+      <c r="E429">
+        <v>2191.6</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5">
+      <c r="A430" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B430" s="12">
+        <v>33609</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5">
+      <c r="A431" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B431" s="12">
+        <v>33609</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5">
+      <c r="A432" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B432" s="12">
+        <v>33609</v>
+      </c>
+      <c r="E432">
+        <v>2068.9</v>
+      </c>
+    </row>
+    <row r="433" spans="1:5">
+      <c r="A433" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B433" s="12">
+        <v>33609</v>
+      </c>
+      <c r="E433">
+        <v>1944.28</v>
+      </c>
+    </row>
+    <row r="434" spans="1:5">
+      <c r="A434" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B434" s="12">
+        <v>33609</v>
+      </c>
+      <c r="E434">
+        <v>2391.83</v>
+      </c>
+    </row>
+    <row r="435" spans="1:5">
+      <c r="A435" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B435" s="12">
+        <v>33609</v>
+      </c>
+    </row>
+    <row r="436" spans="1:5">
+      <c r="A436" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B436" s="12">
+        <v>33613</v>
+      </c>
+      <c r="E436">
+        <v>2526.5</v>
+      </c>
+    </row>
+    <row r="437" spans="1:5">
+      <c r="A437" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B437" s="12">
+        <v>33613</v>
+      </c>
+      <c r="E437">
+        <v>2427.6799999999998</v>
+      </c>
+    </row>
+    <row r="438" spans="1:5">
+      <c r="A438" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B438" s="12">
+        <v>33613</v>
+      </c>
+      <c r="E438">
+        <v>2200.08</v>
+      </c>
+    </row>
+    <row r="439" spans="1:5">
+      <c r="A439" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B439" s="12">
+        <v>33613</v>
+      </c>
+      <c r="E439">
+        <v>2316.58</v>
+      </c>
+    </row>
+    <row r="440" spans="1:5">
+      <c r="A440" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B440" s="12">
+        <v>33613</v>
+      </c>
+      <c r="E440">
+        <v>1700.28</v>
+      </c>
+    </row>
+    <row r="441" spans="1:5">
+      <c r="A441" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B441" s="12">
+        <v>33613</v>
+      </c>
+    </row>
+    <row r="442" spans="1:5">
+      <c r="A442" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B442" s="12">
+        <v>33613</v>
+      </c>
+    </row>
+    <row r="443" spans="1:5">
+      <c r="A443" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B443" s="12">
+        <v>33613</v>
+      </c>
+    </row>
+    <row r="444" spans="1:5">
+      <c r="A444" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B444" s="12">
+        <v>33613</v>
+      </c>
+    </row>
+    <row r="445" spans="1:5">
+      <c r="A445" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B445" s="12">
+        <v>33613</v>
+      </c>
+      <c r="E445">
+        <v>2344.8000000000002</v>
+      </c>
+    </row>
+    <row r="446" spans="1:5">
+      <c r="A446" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B446" s="12">
+        <v>33613</v>
+      </c>
+      <c r="E446">
+        <v>2747.95</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5">
+      <c r="A447" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B447" s="12">
+        <v>33613</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5">
+      <c r="A448" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B448" s="12">
+        <v>33618</v>
+      </c>
+    </row>
+    <row r="449" spans="1:7">
+      <c r="A449" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B449" s="12">
+        <v>33618</v>
+      </c>
+    </row>
+    <row r="450" spans="1:7">
+      <c r="A450" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B450" s="12">
+        <v>33618</v>
+      </c>
+    </row>
+    <row r="451" spans="1:7">
+      <c r="A451" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B451" s="12">
+        <v>33618</v>
+      </c>
+    </row>
+    <row r="452" spans="1:7">
+      <c r="A452" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B452" s="12">
+        <v>33618</v>
+      </c>
+    </row>
+    <row r="453" spans="1:7">
+      <c r="A453" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B453" s="12">
+        <v>33618</v>
+      </c>
+    </row>
+    <row r="454" spans="1:7">
+      <c r="A454" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B454" s="12">
+        <v>33618</v>
+      </c>
+    </row>
+    <row r="455" spans="1:7">
+      <c r="A455" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B455" s="12">
+        <v>33618</v>
+      </c>
+    </row>
+    <row r="456" spans="1:7">
+      <c r="A456" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B456" s="12">
+        <v>33618</v>
+      </c>
+    </row>
+    <row r="457" spans="1:7">
+      <c r="A457" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B457" s="12">
+        <v>33618</v>
+      </c>
+    </row>
+    <row r="458" spans="1:7">
+      <c r="A458" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B458" s="12">
+        <v>33618</v>
+      </c>
+    </row>
+    <row r="459" spans="1:7">
+      <c r="A459" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B459" s="12">
+        <v>33618</v>
+      </c>
+    </row>
+    <row r="460" spans="1:7">
+      <c r="A460" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B460" s="12">
+        <v>33623</v>
+      </c>
+      <c r="C460">
+        <v>90</v>
+      </c>
+      <c r="D460" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G460">
+        <v>778.47</v>
+      </c>
+    </row>
+    <row r="461" spans="1:7">
+      <c r="A461" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B461" s="12">
+        <v>33623</v>
+      </c>
+      <c r="C461">
+        <v>90</v>
+      </c>
+      <c r="D461" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G461">
+        <v>752.04</v>
+      </c>
+    </row>
+    <row r="462" spans="1:7">
+      <c r="A462" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B462" s="12">
+        <v>33623</v>
+      </c>
+      <c r="C462">
+        <v>90</v>
+      </c>
+      <c r="D462" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G462">
+        <v>875.14</v>
+      </c>
+    </row>
+    <row r="463" spans="1:7">
+      <c r="A463" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B463" s="12">
+        <v>33623</v>
+      </c>
+      <c r="C463">
+        <v>90</v>
+      </c>
+      <c r="D463" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G463">
+        <v>799.72</v>
+      </c>
+    </row>
+    <row r="464" spans="1:7">
+      <c r="A464" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B464" s="12">
+        <v>33623</v>
+      </c>
+      <c r="C464">
+        <v>90</v>
+      </c>
+      <c r="D464" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G464">
+        <v>547.62</v>
+      </c>
+    </row>
+    <row r="465" spans="1:7">
+      <c r="A465" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B465" s="12">
+        <v>33623</v>
+      </c>
+      <c r="C465">
+        <v>90</v>
+      </c>
+      <c r="D465" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G465">
+        <v>502.62</v>
+      </c>
+    </row>
+    <row r="466" spans="1:7">
+      <c r="A466" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B466" s="12">
+        <v>33623</v>
+      </c>
+      <c r="C466">
+        <v>90</v>
+      </c>
+      <c r="D466" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G466">
+        <v>521.15</v>
+      </c>
+    </row>
+    <row r="467" spans="1:7">
+      <c r="A467" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B467" s="12">
+        <v>33623</v>
+      </c>
+      <c r="C467">
+        <v>90</v>
+      </c>
+      <c r="D467" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G467">
+        <v>583.44000000000005</v>
+      </c>
+    </row>
+    <row r="468" spans="1:7">
+      <c r="A468" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B468" s="12">
+        <v>33623</v>
+      </c>
+      <c r="C468">
+        <v>90</v>
+      </c>
+      <c r="D468" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G468">
+        <v>713.96</v>
+      </c>
+    </row>
+    <row r="469" spans="1:7">
+      <c r="A469" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B469" s="12">
+        <v>33623</v>
+      </c>
+      <c r="C469">
+        <v>90</v>
+      </c>
+      <c r="D469" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G469">
+        <v>846.94</v>
+      </c>
+    </row>
+    <row r="470" spans="1:7">
+      <c r="A470" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B470" s="12">
+        <v>33623</v>
+      </c>
+      <c r="C470">
+        <v>90</v>
+      </c>
+      <c r="D470" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G470">
+        <v>791.54</v>
+      </c>
+    </row>
+    <row r="471" spans="1:7">
+      <c r="A471" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B471" s="12">
+        <v>33623</v>
+      </c>
+      <c r="C471">
+        <v>90</v>
+      </c>
+      <c r="D471" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G471">
+        <v>324.31</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A3:AD253">
     <sortCondition ref="A3:A253"/>
@@ -13877,9 +16743,11 @@
   <dimension ref="A1:M159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="576" topLeftCell="A142" activePane="bottomLeft"/>
+      <pane xSplit="4356" ySplit="576" topLeftCell="I1" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A159" sqref="A159"/>
+      <selection pane="topRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="I49" sqref="I2:I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -27220,7 +30088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M359"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="864" activePane="bottomLeft"/>
       <selection activeCell="M2" sqref="M2"/>
       <selection pane="bottomLeft"/>

</xml_diff>

<commit_message>
Work on dead leaf dynamics
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="12" windowWidth="12024" windowHeight="5844"/>
+    <workbookView xWindow="192" yWindow="12" windowWidth="12024" windowHeight="5844" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2231" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2233" uniqueCount="295">
   <si>
     <t>SimulationName</t>
   </si>
@@ -998,7 +998,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1037,6 +1037,7 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1454,23 +1455,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="157716864"/>
-        <c:axId val="157718400"/>
+        <c:axId val="123769600"/>
+        <c:axId val="123771136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="157716864"/>
+        <c:axId val="123769600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="157718400"/>
+        <c:crossAx val="123771136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="157718400"/>
+        <c:axId val="123771136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1478,7 +1479,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="157716864"/>
+        <c:crossAx val="123769600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1490,7 +1491,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1818,11 +1819,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE479"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="11280" ySplit="708" topLeftCell="AC24" activePane="bottomRight"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="11280" ySplit="708" topLeftCell="AC222" activePane="bottomLeft"/>
       <selection activeCell="B443" sqref="B443"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomLeft" activeCell="B236" sqref="B236"/>
       <selection pane="bottomRight" activeCell="AC26" sqref="AC26:AC37"/>
     </sheetView>
   </sheetViews>
@@ -20597,12 +20598,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F395"/>
+  <dimension ref="A1:F397"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="576" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4212" ySplit="576" topLeftCell="D369" activePane="bottomRight"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="B384" sqref="B384"/>
+      <selection pane="bottomRight" activeCell="E380" sqref="E380"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -25349,42 +25352,35 @@
     </row>
     <row r="379" spans="1:6">
       <c r="A379" t="s">
-        <v>264</v>
-      </c>
-      <c r="B379" s="13">
-        <v>33483</v>
-      </c>
-      <c r="C379">
-        <v>5.9285714285714288</v>
-      </c>
-      <c r="D379">
-        <v>4.2142857142857144</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="B379" s="12">
+        <v>33529</v>
+      </c>
+      <c r="C379" s="22"/>
       <c r="E379">
-        <v>2</v>
-      </c>
-      <c r="F379">
-        <v>5.6</v>
+        <f>D378</f>
+        <v>11.666666666666666</v>
       </c>
     </row>
     <row r="380" spans="1:6">
       <c r="A380" t="s">
         <v>264</v>
       </c>
-      <c r="B380" s="14">
-        <v>33507</v>
+      <c r="B380" s="13">
+        <v>33483</v>
       </c>
       <c r="C380">
-        <v>10</v>
+        <v>5.9285714285714288</v>
       </c>
       <c r="D380">
-        <v>9</v>
+        <v>4.2142857142857144</v>
       </c>
       <c r="E380">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F380">
-        <v>11.166666666666666</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="381" spans="1:6">
@@ -25392,61 +25388,71 @@
         <v>264</v>
       </c>
       <c r="B381" s="14">
-        <v>33518</v>
+        <v>33507</v>
       </c>
       <c r="C381">
-        <v>9.5</v>
+        <v>10</v>
       </c>
       <c r="D381">
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="E381">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="F381">
-        <v>11.2</v>
+        <v>11.166666666666666</v>
       </c>
     </row>
     <row r="382" spans="1:6">
       <c r="A382" t="s">
         <v>264</v>
       </c>
-      <c r="B382" s="15">
-        <v>33541</v>
+      <c r="B382" s="14">
+        <v>33518</v>
       </c>
       <c r="C382">
-        <v>9.6999999999999993</v>
+        <v>9.5</v>
       </c>
       <c r="D382">
-        <v>9.6999999999999993</v>
+        <v>9.5</v>
       </c>
       <c r="E382">
-        <v>7.3</v>
+        <v>5.5</v>
       </c>
       <c r="F382">
-        <v>5.8888888888888893</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="383" spans="1:6">
       <c r="A383" t="s">
-        <v>268</v>
-      </c>
-      <c r="B383" s="12">
-        <v>40745</v>
+        <v>264</v>
+      </c>
+      <c r="B383" s="15">
+        <v>33541</v>
       </c>
       <c r="C383">
-        <v>4.1666666670000003</v>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="D383">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E383">
+        <v>7.3</v>
+      </c>
+      <c r="F383">
+        <v>5.8888888888888893</v>
       </c>
     </row>
     <row r="384" spans="1:6">
       <c r="A384" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B384" s="12">
-        <v>40752</v>
-      </c>
-      <c r="C384">
-        <v>5.4249999999999998</v>
+        <v>33554</v>
+      </c>
+      <c r="E384">
+        <f>D383</f>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="385" spans="1:3">
@@ -25454,10 +25460,10 @@
         <v>268</v>
       </c>
       <c r="B385" s="12">
-        <v>40756</v>
+        <v>40745</v>
       </c>
       <c r="C385">
-        <v>5.9083333329999999</v>
+        <v>4.1666666670000003</v>
       </c>
     </row>
     <row r="386" spans="1:3">
@@ -25465,10 +25471,10 @@
         <v>268</v>
       </c>
       <c r="B386" s="12">
-        <v>40764</v>
+        <v>40752</v>
       </c>
       <c r="C386">
-        <v>6.5416666670000003</v>
+        <v>5.4249999999999998</v>
       </c>
     </row>
     <row r="387" spans="1:3">
@@ -25476,10 +25482,10 @@
         <v>268</v>
       </c>
       <c r="B387" s="12">
-        <v>40788</v>
+        <v>40756</v>
       </c>
       <c r="C387">
-        <v>9.75</v>
+        <v>5.9083333329999999</v>
       </c>
     </row>
     <row r="388" spans="1:3">
@@ -25487,29 +25493,29 @@
         <v>268</v>
       </c>
       <c r="B388" s="12">
-        <v>40851</v>
+        <v>40764</v>
+      </c>
+      <c r="C388">
+        <v>6.5416666670000003</v>
       </c>
     </row>
     <row r="389" spans="1:3">
       <c r="A389" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B389" s="12">
-        <v>40745</v>
+        <v>40788</v>
       </c>
       <c r="C389">
-        <v>4.1666666670000003</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="390" spans="1:3">
       <c r="A390" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B390" s="12">
-        <v>40752</v>
-      </c>
-      <c r="C390">
-        <v>5.2833333329999999</v>
+        <v>40851</v>
       </c>
     </row>
     <row r="391" spans="1:3">
@@ -25517,10 +25523,10 @@
         <v>269</v>
       </c>
       <c r="B391" s="12">
-        <v>40756</v>
+        <v>40745</v>
       </c>
       <c r="C391">
-        <v>5.8416666670000001</v>
+        <v>4.1666666670000003</v>
       </c>
     </row>
     <row r="392" spans="1:3">
@@ -25528,10 +25534,10 @@
         <v>269</v>
       </c>
       <c r="B392" s="12">
-        <v>40764</v>
+        <v>40752</v>
       </c>
       <c r="C392">
-        <v>6.7916666670000003</v>
+        <v>5.2833333329999999</v>
       </c>
     </row>
     <row r="393" spans="1:3">
@@ -25539,10 +25545,10 @@
         <v>269</v>
       </c>
       <c r="B393" s="12">
-        <v>40788</v>
+        <v>40756</v>
       </c>
       <c r="C393">
-        <v>10</v>
+        <v>5.8416666670000001</v>
       </c>
     </row>
     <row r="394" spans="1:3">
@@ -25550,11 +25556,33 @@
         <v>269</v>
       </c>
       <c r="B394" s="12">
+        <v>40764</v>
+      </c>
+      <c r="C394">
+        <v>6.7916666670000003</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3">
+      <c r="A395" t="s">
+        <v>269</v>
+      </c>
+      <c r="B395" s="12">
+        <v>40788</v>
+      </c>
+      <c r="C395">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3">
+      <c r="A396" t="s">
+        <v>269</v>
+      </c>
+      <c r="B396" s="12">
         <v>40851</v>
       </c>
     </row>
-    <row r="395" spans="1:3">
-      <c r="B395" s="12"/>
+    <row r="397" spans="1:3">
+      <c r="B397" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Konya dataset from Turkey
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1879" uniqueCount="330">
   <si>
     <t>SimulationName</t>
   </si>
@@ -886,6 +886,138 @@
   <si>
     <t>Wagga2014CvLivingstonWaterDry</t>
   </si>
+  <si>
+    <t>Konya09WaterAAA</t>
+  </si>
+  <si>
+    <t>Konya09WaterBAA</t>
+  </si>
+  <si>
+    <t>Konya09WaterCAA</t>
+  </si>
+  <si>
+    <t>Konya09WaterDAA</t>
+  </si>
+  <si>
+    <t>Konya09WaterABA</t>
+  </si>
+  <si>
+    <t>Konya09WaterACA</t>
+  </si>
+  <si>
+    <t>Konya09WaterADA</t>
+  </si>
+  <si>
+    <t>Konya09WaterAAB</t>
+  </si>
+  <si>
+    <t>Konya09WaterAAC</t>
+  </si>
+  <si>
+    <t>Konya09WaterAAD</t>
+  </si>
+  <si>
+    <t>Konya09WaterABB</t>
+  </si>
+  <si>
+    <t>Konya09WaterACC</t>
+  </si>
+  <si>
+    <t>Konya09WaterADD</t>
+  </si>
+  <si>
+    <t>Konya09WaterBAB</t>
+  </si>
+  <si>
+    <t>Konya09WaterCAC</t>
+  </si>
+  <si>
+    <t>Konya09WaterDAD</t>
+  </si>
+  <si>
+    <t>Konya09WaterBBA</t>
+  </si>
+  <si>
+    <t>Konya09WaterCCA</t>
+  </si>
+  <si>
+    <t>Konya09WaterDDA</t>
+  </si>
+  <si>
+    <t>Konya09WaterBBB</t>
+  </si>
+  <si>
+    <t>Konya09WaterCCC</t>
+  </si>
+  <si>
+    <t>Konya09WaterDDD</t>
+  </si>
+  <si>
+    <t>Konya11WaterBAA</t>
+  </si>
+  <si>
+    <t>Konya11WaterCAA</t>
+  </si>
+  <si>
+    <t>Konya11WaterDAA</t>
+  </si>
+  <si>
+    <t>Konya11WaterABA</t>
+  </si>
+  <si>
+    <t>Konya11WaterACA</t>
+  </si>
+  <si>
+    <t>Konya11WaterADA</t>
+  </si>
+  <si>
+    <t>Konya11WaterAAB</t>
+  </si>
+  <si>
+    <t>Konya11WaterAAC</t>
+  </si>
+  <si>
+    <t>Konya11WaterAAD</t>
+  </si>
+  <si>
+    <t>Konya11WaterABB</t>
+  </si>
+  <si>
+    <t>Konya11WaterACC</t>
+  </si>
+  <si>
+    <t>Konya11WaterADD</t>
+  </si>
+  <si>
+    <t>Konya11WaterBAB</t>
+  </si>
+  <si>
+    <t>Konya11WaterCAC</t>
+  </si>
+  <si>
+    <t>Konya11WaterDAD</t>
+  </si>
+  <si>
+    <t>Konya11WaterBBA</t>
+  </si>
+  <si>
+    <t>Konya11WaterCCA</t>
+  </si>
+  <si>
+    <t>Konya11WaterDDA</t>
+  </si>
+  <si>
+    <t>Konya11WaterBBB</t>
+  </si>
+  <si>
+    <t>Konya11WaterCCC</t>
+  </si>
+  <si>
+    <t>Konya11WaterDDD</t>
+  </si>
+  <si>
+    <t>Konya11WaterAAA</t>
+  </si>
 </sst>
 </file>
 
@@ -1456,11 +1588,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="216251968"/>
-        <c:axId val="206452200"/>
+        <c:axId val="370514216"/>
+        <c:axId val="370514608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="216251968"/>
+        <c:axId val="370514216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1470,12 +1602,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206452200"/>
+        <c:crossAx val="370514608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="206452200"/>
+        <c:axId val="370514608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1486,7 +1618,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216251968"/>
+        <c:crossAx val="370514216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1829,14 +1961,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE239"/>
+  <dimension ref="A1:AE283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="9012" ySplit="576" topLeftCell="A214" activePane="bottomRight"/>
+      <pane xSplit="9012" ySplit="576" topLeftCell="AB157" activePane="bottomRight"/>
       <selection sqref="A1:XFD1"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A236" sqref="A236:A239"/>
-      <selection pane="bottomRight" activeCell="D231" sqref="D231:D239"/>
+      <selection pane="bottomLeft" activeCell="D261" sqref="C261:D283"/>
+      <selection pane="bottomRight" activeCell="AB157" sqref="AB157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14139,6 +14271,1194 @@
       </c>
       <c r="AD239">
         <v>10.3</v>
+      </c>
+    </row>
+    <row r="240" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A240" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C240" s="1">
+        <v>90</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E240">
+        <v>2094</v>
+      </c>
+      <c r="G240">
+        <v>682</v>
+      </c>
+      <c r="AB240">
+        <f>G240/AC240*1000</f>
+        <v>17442.455242966753</v>
+      </c>
+      <c r="AC240">
+        <v>39.1</v>
+      </c>
+      <c r="AD240">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A241" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C241" s="1">
+        <v>90</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E241">
+        <v>2011</v>
+      </c>
+      <c r="G241">
+        <v>630</v>
+      </c>
+      <c r="AB241">
+        <f t="shared" ref="AB241:AB283" si="1">G241/AC241*1000</f>
+        <v>15750</v>
+      </c>
+      <c r="AC241">
+        <v>40</v>
+      </c>
+      <c r="AD241">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="242" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A242" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C242" s="1">
+        <v>90</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E242">
+        <v>1926</v>
+      </c>
+      <c r="G242">
+        <v>572</v>
+      </c>
+      <c r="AB242">
+        <f t="shared" si="1"/>
+        <v>14554.707379134861</v>
+      </c>
+      <c r="AC242">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="AD242">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="243" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A243" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C243" s="1">
+        <v>90</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E243">
+        <v>1702</v>
+      </c>
+      <c r="G243">
+        <v>435</v>
+      </c>
+      <c r="AB243">
+        <f t="shared" si="1"/>
+        <v>11096.938775510203</v>
+      </c>
+      <c r="AC243">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="AD243">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A244" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="C244" s="1">
+        <v>90</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E244">
+        <v>1985</v>
+      </c>
+      <c r="G244">
+        <v>627</v>
+      </c>
+      <c r="AB244">
+        <f t="shared" si="1"/>
+        <v>15873.417721518987</v>
+      </c>
+      <c r="AC244">
+        <v>39.5</v>
+      </c>
+      <c r="AD244">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="245" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A245" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="C245" s="1">
+        <v>90</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E245">
+        <v>1759</v>
+      </c>
+      <c r="G245">
+        <v>551</v>
+      </c>
+      <c r="AB245">
+        <f t="shared" si="1"/>
+        <v>14851.752021563343</v>
+      </c>
+      <c r="AC245">
+        <v>37.1</v>
+      </c>
+      <c r="AD245">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="246" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A246" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="C246" s="1">
+        <v>90</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E246">
+        <v>1644</v>
+      </c>
+      <c r="G246">
+        <v>441</v>
+      </c>
+      <c r="AB246">
+        <f t="shared" si="1"/>
+        <v>12284.122562674096</v>
+      </c>
+      <c r="AC246">
+        <v>35.9</v>
+      </c>
+      <c r="AD246">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A247" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="C247" s="1">
+        <v>90</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E247">
+        <v>2009</v>
+      </c>
+      <c r="G247">
+        <v>667</v>
+      </c>
+      <c r="AB247">
+        <f t="shared" si="1"/>
+        <v>17146.529562982007</v>
+      </c>
+      <c r="AC247">
+        <v>38.9</v>
+      </c>
+      <c r="AD247">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="248" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A248" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="C248" s="1">
+        <v>90</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E248">
+        <v>1934</v>
+      </c>
+      <c r="G248">
+        <v>637</v>
+      </c>
+      <c r="AB248">
+        <f t="shared" si="1"/>
+        <v>15964.912280701756</v>
+      </c>
+      <c r="AC248">
+        <v>39.9</v>
+      </c>
+      <c r="AD248">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="249" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A249" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C249" s="1">
+        <v>90</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E249">
+        <v>1822</v>
+      </c>
+      <c r="G249">
+        <v>533</v>
+      </c>
+      <c r="AB249">
+        <f t="shared" si="1"/>
+        <v>14175.531914893616</v>
+      </c>
+      <c r="AC249">
+        <v>37.6</v>
+      </c>
+      <c r="AD249">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="250" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A250" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C250" s="1">
+        <v>90</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E250">
+        <v>1801</v>
+      </c>
+      <c r="G250">
+        <v>564</v>
+      </c>
+      <c r="AB250">
+        <f t="shared" si="1"/>
+        <v>14351.145038167941</v>
+      </c>
+      <c r="AC250">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="AD250">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="251" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A251" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C251" s="1">
+        <v>90</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E251">
+        <v>1759</v>
+      </c>
+      <c r="G251">
+        <v>497</v>
+      </c>
+      <c r="AB251">
+        <f t="shared" si="1"/>
+        <v>12875.647668393782</v>
+      </c>
+      <c r="AC251">
+        <v>38.6</v>
+      </c>
+      <c r="AD251">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="252" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A252" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C252" s="1">
+        <v>90</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E252">
+        <v>1492</v>
+      </c>
+      <c r="G252">
+        <v>411</v>
+      </c>
+      <c r="AB252">
+        <f t="shared" si="1"/>
+        <v>12492.401215805472</v>
+      </c>
+      <c r="AC252">
+        <v>32.9</v>
+      </c>
+      <c r="AD252">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="253" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A253" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C253" s="1">
+        <v>90</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E253">
+        <v>1847</v>
+      </c>
+      <c r="G253">
+        <v>602</v>
+      </c>
+      <c r="AB253">
+        <f t="shared" si="1"/>
+        <v>15718.015665796345</v>
+      </c>
+      <c r="AC253">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="AD253">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="254" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A254" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C254" s="1">
+        <v>90</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E254">
+        <v>1649</v>
+      </c>
+      <c r="G254">
+        <v>521</v>
+      </c>
+      <c r="AB254">
+        <f t="shared" si="1"/>
+        <v>13674.540682414698</v>
+      </c>
+      <c r="AC254">
+        <v>38.1</v>
+      </c>
+      <c r="AD254">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A255" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C255" s="1">
+        <v>90</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E255">
+        <v>1531</v>
+      </c>
+      <c r="G255">
+        <v>454</v>
+      </c>
+      <c r="AB255">
+        <f t="shared" si="1"/>
+        <v>12270.27027027027</v>
+      </c>
+      <c r="AC255">
+        <v>37</v>
+      </c>
+      <c r="AD255">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A256" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C256" s="1">
+        <v>90</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E256">
+        <v>1814</v>
+      </c>
+      <c r="G256">
+        <v>547</v>
+      </c>
+      <c r="AB256">
+        <f t="shared" si="1"/>
+        <v>13954.08163265306</v>
+      </c>
+      <c r="AC256">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="AD256">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="257" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A257" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C257" s="1">
+        <v>90</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E257">
+        <v>1731</v>
+      </c>
+      <c r="G257">
+        <v>486</v>
+      </c>
+      <c r="AB257">
+        <f t="shared" si="1"/>
+        <v>12925.531914893616</v>
+      </c>
+      <c r="AC257">
+        <v>37.6</v>
+      </c>
+      <c r="AD257">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="258" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A258" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C258" s="1">
+        <v>90</v>
+      </c>
+      <c r="D258" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E258">
+        <v>1432</v>
+      </c>
+      <c r="G258">
+        <v>357</v>
+      </c>
+      <c r="AB258">
+        <f t="shared" si="1"/>
+        <v>10347.826086956522</v>
+      </c>
+      <c r="AC258">
+        <v>34.5</v>
+      </c>
+      <c r="AD258">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="259" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A259" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C259" s="1">
+        <v>90</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E259">
+        <v>1707</v>
+      </c>
+      <c r="G259">
+        <v>530</v>
+      </c>
+      <c r="AB259">
+        <f t="shared" si="1"/>
+        <v>14247.311827956988</v>
+      </c>
+      <c r="AC259">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="AD259">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="260" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A260" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C260" s="1">
+        <v>90</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E260">
+        <v>1589</v>
+      </c>
+      <c r="G260">
+        <v>409</v>
+      </c>
+      <c r="AB260">
+        <f t="shared" si="1"/>
+        <v>10906.666666666666</v>
+      </c>
+      <c r="AC260">
+        <v>37.5</v>
+      </c>
+      <c r="AD260">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="261" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A261" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C261" s="1">
+        <v>90</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E261">
+        <v>1328</v>
+      </c>
+      <c r="G261">
+        <v>288</v>
+      </c>
+      <c r="AB261">
+        <f t="shared" si="1"/>
+        <v>8495.575221238938</v>
+      </c>
+      <c r="AC261">
+        <v>33.9</v>
+      </c>
+      <c r="AD261">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A262" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C262" s="1">
+        <v>90</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E262">
+        <v>1743</v>
+      </c>
+      <c r="G262">
+        <v>647</v>
+      </c>
+      <c r="AB262">
+        <f t="shared" si="1"/>
+        <v>13070.707070707071</v>
+      </c>
+      <c r="AC262">
+        <v>49.5</v>
+      </c>
+      <c r="AD262">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="263" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A263" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="C263" s="1">
+        <v>90</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E263">
+        <v>1761</v>
+      </c>
+      <c r="G263">
+        <v>604</v>
+      </c>
+      <c r="AB263">
+        <f t="shared" si="1"/>
+        <v>11570.88122605364</v>
+      </c>
+      <c r="AC263">
+        <v>52.2</v>
+      </c>
+      <c r="AD263">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A264" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C264" s="1">
+        <v>90</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E264">
+        <v>1607</v>
+      </c>
+      <c r="G264">
+        <v>561</v>
+      </c>
+      <c r="AB264">
+        <f t="shared" si="1"/>
+        <v>11175.298804780876</v>
+      </c>
+      <c r="AC264">
+        <v>50.2</v>
+      </c>
+      <c r="AD264">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="265" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A265" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C265" s="1">
+        <v>90</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E265">
+        <v>1437</v>
+      </c>
+      <c r="G265">
+        <v>467</v>
+      </c>
+      <c r="AB265">
+        <f t="shared" si="1"/>
+        <v>9511.2016293279012</v>
+      </c>
+      <c r="AC265">
+        <v>49.1</v>
+      </c>
+      <c r="AD265">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="266" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A266" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C266" s="1">
+        <v>90</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E266">
+        <v>1635</v>
+      </c>
+      <c r="G266">
+        <v>595</v>
+      </c>
+      <c r="AB266">
+        <f t="shared" si="1"/>
+        <v>11805.555555555555</v>
+      </c>
+      <c r="AC266">
+        <v>50.4</v>
+      </c>
+      <c r="AD266">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A267" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C267" s="1">
+        <v>90</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E267">
+        <v>1538</v>
+      </c>
+      <c r="G267">
+        <v>549</v>
+      </c>
+      <c r="AB267">
+        <f t="shared" si="1"/>
+        <v>11461.377870563676</v>
+      </c>
+      <c r="AC267">
+        <v>47.9</v>
+      </c>
+      <c r="AD267">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="268" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A268" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="C268" s="1">
+        <v>90</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E268">
+        <v>1474</v>
+      </c>
+      <c r="G268">
+        <v>451</v>
+      </c>
+      <c r="AB268">
+        <f t="shared" si="1"/>
+        <v>10512.820512820514</v>
+      </c>
+      <c r="AC268">
+        <v>42.9</v>
+      </c>
+      <c r="AD268">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A269" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C269" s="1">
+        <v>90</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E269">
+        <v>1775</v>
+      </c>
+      <c r="G269">
+        <v>625</v>
+      </c>
+      <c r="AB269">
+        <f t="shared" si="1"/>
+        <v>12351.778656126482</v>
+      </c>
+      <c r="AC269">
+        <v>50.6</v>
+      </c>
+      <c r="AD269">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="270" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A270" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C270" s="1">
+        <v>90</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E270">
+        <v>1664</v>
+      </c>
+      <c r="G270">
+        <v>589</v>
+      </c>
+      <c r="AB270">
+        <f t="shared" si="1"/>
+        <v>12916.666666666666</v>
+      </c>
+      <c r="AC270">
+        <v>45.6</v>
+      </c>
+      <c r="AD270">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="271" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A271" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C271" s="1">
+        <v>90</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E271">
+        <v>1547</v>
+      </c>
+      <c r="G271">
+        <v>523</v>
+      </c>
+      <c r="AB271">
+        <f t="shared" si="1"/>
+        <v>11344.902386117135</v>
+      </c>
+      <c r="AC271">
+        <v>46.1</v>
+      </c>
+      <c r="AD271">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="272" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A272" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C272" s="1">
+        <v>90</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E272">
+        <v>1577</v>
+      </c>
+      <c r="G272">
+        <v>571</v>
+      </c>
+      <c r="AB272">
+        <f t="shared" si="1"/>
+        <v>11558.704453441296</v>
+      </c>
+      <c r="AC272">
+        <v>49.4</v>
+      </c>
+      <c r="AD272">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A273" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C273" s="1">
+        <v>90</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E273">
+        <v>1407</v>
+      </c>
+      <c r="G273">
+        <v>522</v>
+      </c>
+      <c r="AB273">
+        <f t="shared" si="1"/>
+        <v>11177.730192719486</v>
+      </c>
+      <c r="AC273">
+        <v>46.7</v>
+      </c>
+      <c r="AD273">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="274" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A274" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C274" s="1">
+        <v>90</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E274">
+        <v>1241</v>
+      </c>
+      <c r="G274">
+        <v>395</v>
+      </c>
+      <c r="AB274">
+        <f t="shared" si="1"/>
+        <v>10675.675675675675</v>
+      </c>
+      <c r="AC274">
+        <v>37</v>
+      </c>
+      <c r="AD274">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="275" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A275" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C275" s="1">
+        <v>90</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E275">
+        <v>1569</v>
+      </c>
+      <c r="G275">
+        <v>579</v>
+      </c>
+      <c r="AB275">
+        <f t="shared" si="1"/>
+        <v>11744.421906693713</v>
+      </c>
+      <c r="AC275">
+        <v>49.3</v>
+      </c>
+      <c r="AD275">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A276" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C276" s="1">
+        <v>90</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E276">
+        <v>1459</v>
+      </c>
+      <c r="G276">
+        <v>537</v>
+      </c>
+      <c r="AB276">
+        <f t="shared" si="1"/>
+        <v>11164.241164241163</v>
+      </c>
+      <c r="AC276">
+        <v>48.1</v>
+      </c>
+      <c r="AD276">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="277" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A277" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C277" s="1">
+        <v>90</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E277">
+        <v>1256</v>
+      </c>
+      <c r="G277">
+        <v>412</v>
+      </c>
+      <c r="AB277">
+        <f t="shared" si="1"/>
+        <v>9196.4285714285706</v>
+      </c>
+      <c r="AC277">
+        <v>44.8</v>
+      </c>
+      <c r="AD277">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A278" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C278" s="1">
+        <v>90</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E278">
+        <v>1528</v>
+      </c>
+      <c r="G278">
+        <v>538</v>
+      </c>
+      <c r="AB278">
+        <f t="shared" si="1"/>
+        <v>10426.356589147286</v>
+      </c>
+      <c r="AC278">
+        <v>51.6</v>
+      </c>
+      <c r="AD278">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A279" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C279" s="1">
+        <v>90</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E279">
+        <v>1361</v>
+      </c>
+      <c r="G279">
+        <v>456</v>
+      </c>
+      <c r="AB279">
+        <f t="shared" si="1"/>
+        <v>9978.1181619256004</v>
+      </c>
+      <c r="AC279">
+        <v>45.7</v>
+      </c>
+      <c r="AD279">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="280" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A280" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C280" s="1">
+        <v>90</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E280">
+        <v>1158</v>
+      </c>
+      <c r="G280">
+        <v>336</v>
+      </c>
+      <c r="AB280">
+        <f t="shared" si="1"/>
+        <v>8337.4689826302729</v>
+      </c>
+      <c r="AC280">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="AD280">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="281" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A281" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="C281" s="1">
+        <v>90</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E281">
+        <v>1478</v>
+      </c>
+      <c r="G281">
+        <v>513</v>
+      </c>
+      <c r="AB281">
+        <f t="shared" si="1"/>
+        <v>10078.585461689589</v>
+      </c>
+      <c r="AC281">
+        <v>50.9</v>
+      </c>
+      <c r="AD281">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="282" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A282" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C282" s="1">
+        <v>90</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E282">
+        <v>1112</v>
+      </c>
+      <c r="G282">
+        <v>407</v>
+      </c>
+      <c r="AB282">
+        <f t="shared" si="1"/>
+        <v>8867.1023965141612</v>
+      </c>
+      <c r="AC282">
+        <v>45.9</v>
+      </c>
+      <c r="AD282">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="283" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A283" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C283" s="1">
+        <v>90</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E283">
+        <v>1013</v>
+      </c>
+      <c r="G283">
+        <v>243</v>
+      </c>
+      <c r="AB283">
+        <f t="shared" si="1"/>
+        <v>6411.6094986807384</v>
+      </c>
+      <c r="AC283">
+        <v>37.9</v>
+      </c>
+      <c r="AD283">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Graphs for Lincoln1992
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2643" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2649" uniqueCount="355">
   <si>
     <t>SimulationName</t>
   </si>
@@ -1678,11 +1678,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="294006712"/>
-        <c:axId val="294007104"/>
+        <c:axId val="319283872"/>
+        <c:axId val="319284264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="294006712"/>
+        <c:axId val="319283872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1692,12 +1692,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="294007104"/>
+        <c:crossAx val="319284264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="294007104"/>
+        <c:axId val="319284264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1708,7 +1708,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="294006712"/>
+        <c:crossAx val="319283872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2054,10 +2054,10 @@
   <dimension ref="A1:AQ920"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B445" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AF704" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E457" sqref="E457:BE749"/>
+      <selection pane="bottomRight" activeCell="AK716" sqref="AK716"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21492,6 +21492,9 @@
       <c r="B286" s="5">
         <v>41664</v>
       </c>
+      <c r="D286" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="E286" s="21">
         <v>2625.4943707521256</v>
       </c>
@@ -22033,6 +22036,9 @@
       <c r="B294" s="5">
         <v>41664</v>
       </c>
+      <c r="D294" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="E294" s="21">
         <v>2121.6746017489827</v>
       </c>
@@ -22574,6 +22580,9 @@
       <c r="B302" s="5">
         <v>41664</v>
       </c>
+      <c r="D302" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="E302" s="21">
         <v>2408.9480068087651</v>
       </c>
@@ -23115,6 +23124,9 @@
       <c r="B310" s="5">
         <v>41664</v>
       </c>
+      <c r="D310" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="E310" s="21">
         <v>2468.3094723972449</v>
       </c>
@@ -23656,6 +23668,9 @@
       <c r="B318" s="5">
         <v>41664</v>
       </c>
+      <c r="D318" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="E318" s="21">
         <v>2474.0820469697851</v>
       </c>
@@ -24196,6 +24211,9 @@
       </c>
       <c r="B326" s="11">
         <v>41664</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="E326" s="21">
         <v>2619.6985123527334</v>
@@ -30976,9 +30994,6 @@
       <c r="AE461">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN461">
-        <v>151.167</v>
-      </c>
     </row>
     <row r="462" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A462" s="4" t="s">
@@ -31023,9 +31038,6 @@
       <c r="AE462">
         <v>1.4E-2</v>
       </c>
-      <c r="AN462">
-        <v>173.5</v>
-      </c>
     </row>
     <row r="463" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A463" s="4" t="s">
@@ -31070,9 +31082,6 @@
       <c r="AE463">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN463">
-        <v>214.083</v>
-      </c>
     </row>
     <row r="464" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A464" s="4" t="s">
@@ -31117,9 +31126,6 @@
       <c r="AE464">
         <v>1.2E-2</v>
       </c>
-      <c r="AN464">
-        <v>243</v>
-      </c>
     </row>
     <row r="465" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A465" s="4" t="s">
@@ -31164,9 +31170,6 @@
       <c r="AE465">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AN465">
-        <v>271.95</v>
-      </c>
     </row>
     <row r="466" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A466" s="4" t="s">
@@ -31211,9 +31214,6 @@
       <c r="AE466">
         <v>1.2E-2</v>
       </c>
-      <c r="AN466">
-        <v>353.46699999999998</v>
-      </c>
     </row>
     <row r="467" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A467" s="4" t="s">
@@ -31249,9 +31249,6 @@
       <c r="AE467">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AN467">
-        <v>400.9</v>
-      </c>
     </row>
     <row r="468" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A468" s="4" t="s">
@@ -31287,9 +31284,6 @@
       <c r="AE468">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AN468">
-        <v>441.28300000000002</v>
-      </c>
     </row>
     <row r="469" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A469" s="4" t="s">
@@ -31325,9 +31319,6 @@
       <c r="AE469">
         <v>1.6E-2</v>
       </c>
-      <c r="AN469">
-        <v>461.43299999999999</v>
-      </c>
     </row>
     <row r="470" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A470" s="4" t="s">
@@ -31378,7 +31369,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="AN471">
-        <v>443.88</v>
+        <v>136.66800000000001</v>
       </c>
     </row>
     <row r="472" spans="1:40" x14ac:dyDescent="0.25">
@@ -31546,9 +31537,6 @@
       <c r="AE476">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN476">
-        <v>188.833</v>
-      </c>
     </row>
     <row r="477" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A477" s="4" t="s">
@@ -31593,9 +31581,6 @@
       <c r="AE477">
         <v>1.4E-2</v>
       </c>
-      <c r="AN477">
-        <v>203.767</v>
-      </c>
     </row>
     <row r="478" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A478" s="4" t="s">
@@ -31640,9 +31625,6 @@
       <c r="AE478">
         <v>1.4E-2</v>
       </c>
-      <c r="AN478">
-        <v>291.83300000000003</v>
-      </c>
     </row>
     <row r="479" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A479" s="4" t="s">
@@ -31687,9 +31669,6 @@
       <c r="AE479">
         <v>1.2E-2</v>
       </c>
-      <c r="AN479">
-        <v>328.66699999999997</v>
-      </c>
     </row>
     <row r="480" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A480" s="4" t="s">
@@ -31734,9 +31713,6 @@
       <c r="AE480">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AN480">
-        <v>394.43299999999999</v>
-      </c>
     </row>
     <row r="481" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A481" s="4" t="s">
@@ -31781,9 +31757,6 @@
       <c r="AE481">
         <v>1.4E-2</v>
       </c>
-      <c r="AN481">
-        <v>405.16699999999997</v>
-      </c>
     </row>
     <row r="482" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A482" s="4" t="s">
@@ -31828,9 +31801,6 @@
       <c r="AE482">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AN482">
-        <v>449.85</v>
-      </c>
     </row>
     <row r="483" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A483" s="4" t="s">
@@ -31866,9 +31836,6 @@
       <c r="AE483">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AN483">
-        <v>688.63300000000004</v>
-      </c>
     </row>
     <row r="484" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A484" s="4" t="s">
@@ -31904,9 +31871,6 @@
       <c r="AE484">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN484">
-        <v>673.86699999999996</v>
-      </c>
     </row>
     <row r="485" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A485" s="4" t="s">
@@ -31957,7 +31921,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="AN486">
-        <v>905.40599999999995</v>
+        <v>238.62199999999996</v>
       </c>
     </row>
     <row r="487" spans="1:40" x14ac:dyDescent="0.25">
@@ -32125,9 +32089,6 @@
       <c r="AE491">
         <v>1.9E-2</v>
       </c>
-      <c r="AN491">
-        <v>186.833</v>
-      </c>
     </row>
     <row r="492" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A492" s="4" t="s">
@@ -32172,9 +32133,6 @@
       <c r="AE492">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN492">
-        <v>269.60000000000002</v>
-      </c>
     </row>
     <row r="493" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A493" s="4" t="s">
@@ -32219,9 +32177,6 @@
       <c r="AE493">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN493">
-        <v>327.16699999999997</v>
-      </c>
     </row>
     <row r="494" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A494" s="4" t="s">
@@ -32266,9 +32221,6 @@
       <c r="AE494">
         <v>1.6E-2</v>
       </c>
-      <c r="AN494">
-        <v>402.5</v>
-      </c>
     </row>
     <row r="495" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A495" s="4" t="s">
@@ -32313,9 +32265,6 @@
       <c r="AE495">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN495">
-        <v>560.75</v>
-      </c>
     </row>
     <row r="496" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A496" s="4" t="s">
@@ -32360,9 +32309,6 @@
       <c r="AE496">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN496">
-        <v>544.91700000000003</v>
-      </c>
     </row>
     <row r="497" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A497" s="4" t="s">
@@ -32407,9 +32353,6 @@
       <c r="AE497">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN497">
-        <v>800.41700000000003</v>
-      </c>
     </row>
     <row r="498" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A498" s="4" t="s">
@@ -32445,9 +32388,6 @@
       <c r="AE498">
         <v>1.9E-2</v>
       </c>
-      <c r="AN498">
-        <v>786.45</v>
-      </c>
     </row>
     <row r="499" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A499" s="4" t="s">
@@ -32483,9 +32423,6 @@
       <c r="AE499">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN499">
-        <v>848.26700000000005</v>
-      </c>
     </row>
     <row r="500" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A500" s="4" t="s">
@@ -32536,7 +32473,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="AN501">
-        <v>975.15200000000004</v>
+        <v>235.35400000000004</v>
       </c>
     </row>
     <row r="502" spans="1:40" x14ac:dyDescent="0.25">
@@ -32704,9 +32641,6 @@
       <c r="AE506">
         <v>0.02</v>
       </c>
-      <c r="AN506">
-        <v>225.167</v>
-      </c>
     </row>
     <row r="507" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A507" s="4" t="s">
@@ -32751,9 +32685,6 @@
       <c r="AE507">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN507">
-        <v>241.95</v>
-      </c>
     </row>
     <row r="508" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A508" s="4" t="s">
@@ -32798,9 +32729,6 @@
       <c r="AE508">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN508">
-        <v>390.66699999999997</v>
-      </c>
     </row>
     <row r="509" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A509" s="4" t="s">
@@ -32845,9 +32773,6 @@
       <c r="AE509">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN509">
-        <v>522</v>
-      </c>
     </row>
     <row r="510" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A510" s="4" t="s">
@@ -32892,9 +32817,6 @@
       <c r="AE510">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN510">
-        <v>702.21699999999998</v>
-      </c>
     </row>
     <row r="511" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A511" s="4" t="s">
@@ -32939,9 +32861,6 @@
       <c r="AE511">
         <v>0.02</v>
       </c>
-      <c r="AN511">
-        <v>746.65</v>
-      </c>
     </row>
     <row r="512" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A512" s="4" t="s">
@@ -32986,9 +32905,6 @@
       <c r="AE512">
         <v>0.02</v>
       </c>
-      <c r="AN512">
-        <v>995</v>
-      </c>
     </row>
     <row r="513" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A513" s="4" t="s">
@@ -33033,9 +32949,6 @@
       <c r="AE513">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AN513">
-        <v>1009.333</v>
-      </c>
     </row>
     <row r="514" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A514" s="4" t="s">
@@ -33071,9 +32984,6 @@
       <c r="AE514">
         <v>2.4E-2</v>
       </c>
-      <c r="AN514">
-        <v>1078.1669999999999</v>
-      </c>
     </row>
     <row r="515" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A515" s="4" t="s">
@@ -33124,7 +33034,7 @@
         <v>2.3E-2</v>
       </c>
       <c r="AN516">
-        <v>1099.9390000000001</v>
+        <v>227.58100000000013</v>
       </c>
     </row>
     <row r="517" spans="1:40" x14ac:dyDescent="0.25">
@@ -33298,9 +33208,6 @@
       <c r="AE521">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AN521">
-        <v>104.667</v>
-      </c>
     </row>
     <row r="522" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A522" s="4" t="s">
@@ -33345,9 +33252,6 @@
       <c r="AE522">
         <v>1.4E-2</v>
       </c>
-      <c r="AN522">
-        <v>145.517</v>
-      </c>
     </row>
     <row r="523" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A523" s="4" t="s">
@@ -33392,9 +33296,6 @@
       <c r="AE523">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN523">
-        <v>216.11699999999999</v>
-      </c>
     </row>
     <row r="524" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A524" s="4" t="s">
@@ -33439,9 +33340,6 @@
       <c r="AE524">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AN524">
-        <v>224.667</v>
-      </c>
     </row>
     <row r="525" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A525" s="4" t="s">
@@ -33486,9 +33384,6 @@
       <c r="AE525">
         <v>1.4E-2</v>
       </c>
-      <c r="AN525">
-        <v>305.53300000000002</v>
-      </c>
     </row>
     <row r="526" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A526" s="4" t="s">
@@ -33533,9 +33428,6 @@
       <c r="AE526">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AN526">
-        <v>204.333</v>
-      </c>
     </row>
     <row r="527" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A527" s="4" t="s">
@@ -33580,9 +33472,6 @@
       <c r="AE527">
         <v>1.4E-2</v>
       </c>
-      <c r="AN527">
-        <v>302.45</v>
-      </c>
     </row>
     <row r="528" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A528" s="4" t="s">
@@ -33618,9 +33507,6 @@
       <c r="AE528">
         <v>1.4E-2</v>
       </c>
-      <c r="AN528">
-        <v>276.517</v>
-      </c>
     </row>
     <row r="529" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A529" s="4" t="s">
@@ -33656,9 +33542,6 @@
       <c r="AE529">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN529">
-        <v>258.233</v>
-      </c>
     </row>
     <row r="530" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A530" s="4" t="s">
@@ -33709,7 +33592,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="AN531">
-        <v>347.255</v>
+        <v>102.09</v>
       </c>
     </row>
     <row r="532" spans="1:40" x14ac:dyDescent="0.25">
@@ -33880,9 +33763,6 @@
       <c r="AE536">
         <v>1.9E-2</v>
       </c>
-      <c r="AN536">
-        <v>160.833</v>
-      </c>
     </row>
     <row r="537" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A537" s="4" t="s">
@@ -33927,9 +33807,6 @@
       <c r="AE537">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN537">
-        <v>223.9</v>
-      </c>
     </row>
     <row r="538" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A538" s="4" t="s">
@@ -33974,9 +33851,6 @@
       <c r="AE538">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN538">
-        <v>281.767</v>
-      </c>
     </row>
     <row r="539" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A539" s="4" t="s">
@@ -34021,9 +33895,6 @@
       <c r="AE539">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN539">
-        <v>354.66699999999997</v>
-      </c>
     </row>
     <row r="540" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A540" s="4" t="s">
@@ -34068,9 +33939,6 @@
       <c r="AE540">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN540">
-        <v>432.45</v>
-      </c>
     </row>
     <row r="541" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A541" s="4" t="s">
@@ -34115,9 +33983,6 @@
       <c r="AE541">
         <v>1.4E-2</v>
       </c>
-      <c r="AN541">
-        <v>568.06700000000001</v>
-      </c>
     </row>
     <row r="542" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A542" s="4" t="s">
@@ -34162,9 +34027,6 @@
       <c r="AE542">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN542">
-        <v>547.15</v>
-      </c>
     </row>
     <row r="543" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A543" s="4" t="s">
@@ -34200,9 +34062,6 @@
       <c r="AE543">
         <v>1.4E-2</v>
       </c>
-      <c r="AN543">
-        <v>695.4</v>
-      </c>
     </row>
     <row r="544" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A544" s="4" t="s">
@@ -34238,9 +34097,6 @@
       <c r="AE544">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN544">
-        <v>628.78300000000002</v>
-      </c>
     </row>
     <row r="545" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A545" s="4" t="s">
@@ -34291,7 +34147,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="AN546">
-        <v>629.18600000000004</v>
+        <v>161.32800000000003</v>
       </c>
     </row>
     <row r="547" spans="1:40" x14ac:dyDescent="0.25">
@@ -34459,9 +34315,6 @@
       <c r="AE551">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN551">
-        <v>207.333</v>
-      </c>
     </row>
     <row r="552" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A552" s="4" t="s">
@@ -34506,9 +34359,6 @@
       <c r="AE552">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN552">
-        <v>208.81700000000001</v>
-      </c>
     </row>
     <row r="553" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A553" s="4" t="s">
@@ -34553,9 +34403,6 @@
       <c r="AE553">
         <v>1.6E-2</v>
       </c>
-      <c r="AN553">
-        <v>328.5</v>
-      </c>
     </row>
     <row r="554" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A554" s="4" t="s">
@@ -34600,9 +34447,6 @@
       <c r="AE554">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN554">
-        <v>462</v>
-      </c>
     </row>
     <row r="555" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A555" s="4" t="s">
@@ -34647,9 +34491,6 @@
       <c r="AE555">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN555">
-        <v>548.16700000000003</v>
-      </c>
     </row>
     <row r="556" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A556" s="4" t="s">
@@ -34694,9 +34535,6 @@
       <c r="AE556">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AN556">
-        <v>426.61700000000002</v>
-      </c>
     </row>
     <row r="557" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A557" s="4" t="s">
@@ -34741,9 +34579,6 @@
       <c r="AE557">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AN557">
-        <v>689.95</v>
-      </c>
     </row>
     <row r="558" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A558" s="4" t="s">
@@ -34782,9 +34617,6 @@
       <c r="AE558">
         <v>1.4E-2</v>
       </c>
-      <c r="AN558">
-        <v>556.70000000000005</v>
-      </c>
     </row>
     <row r="559" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A559" s="4" t="s">
@@ -34820,9 +34652,6 @@
       <c r="AE559">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN559">
-        <v>776.16700000000003</v>
-      </c>
     </row>
     <row r="560" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A560" s="4" t="s">
@@ -34873,7 +34702,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="AN561">
-        <v>852.73599999999999</v>
+        <v>225.30899999999997</v>
       </c>
     </row>
     <row r="562" spans="1:40" x14ac:dyDescent="0.25">
@@ -35047,9 +34876,6 @@
       <c r="AE566">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN566">
-        <v>220.167</v>
-      </c>
     </row>
     <row r="567" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A567" s="4" t="s">
@@ -35094,9 +34920,6 @@
       <c r="AE567">
         <v>1.6E-2</v>
       </c>
-      <c r="AN567">
-        <v>259.75</v>
-      </c>
     </row>
     <row r="568" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A568" s="4" t="s">
@@ -35141,9 +34964,6 @@
       <c r="AE568">
         <v>1.6E-2</v>
       </c>
-      <c r="AN568">
-        <v>399.16699999999997</v>
-      </c>
     </row>
     <row r="569" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A569" s="4" t="s">
@@ -35188,9 +35008,6 @@
       <c r="AE569">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN569">
-        <v>515.66700000000003</v>
-      </c>
     </row>
     <row r="570" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A570" s="4" t="s">
@@ -35235,9 +35052,6 @@
       <c r="AE570">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN570">
-        <v>636.78300000000002</v>
-      </c>
     </row>
     <row r="571" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A571" s="4" t="s">
@@ -35282,9 +35096,6 @@
       <c r="AE571">
         <v>1.9E-2</v>
       </c>
-      <c r="AN571">
-        <v>801.16700000000003</v>
-      </c>
     </row>
     <row r="572" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A572" s="4" t="s">
@@ -35329,9 +35140,6 @@
       <c r="AE572">
         <v>1.9E-2</v>
       </c>
-      <c r="AN572">
-        <v>899</v>
-      </c>
     </row>
     <row r="573" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A573" s="4" t="s">
@@ -35376,9 +35184,6 @@
       <c r="AE573">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AN573">
-        <v>874.26700000000005</v>
-      </c>
     </row>
     <row r="574" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A574" s="4" t="s">
@@ -35414,9 +35219,6 @@
       <c r="AE574">
         <v>2.3E-2</v>
       </c>
-      <c r="AN574">
-        <v>877.93299999999999</v>
-      </c>
     </row>
     <row r="575" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A575" s="4" t="s">
@@ -35467,7 +35269,7 @@
         <v>2.3E-2</v>
       </c>
       <c r="AN576">
-        <v>854.68100000000004</v>
+        <v>190.71600000000001</v>
       </c>
     </row>
     <row r="577" spans="1:40" x14ac:dyDescent="0.25">
@@ -35681,9 +35483,6 @@
       <c r="AE583">
         <v>1.4E-2</v>
       </c>
-      <c r="AN583">
-        <v>86.167000000000002</v>
-      </c>
     </row>
     <row r="584" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A584" s="4" t="s">
@@ -35728,9 +35527,6 @@
       <c r="AE584">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN584">
-        <v>159.833</v>
-      </c>
     </row>
     <row r="585" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A585" s="4" t="s">
@@ -35775,9 +35571,6 @@
       <c r="AE585">
         <v>1.6E-2</v>
       </c>
-      <c r="AN585">
-        <v>172.63300000000001</v>
-      </c>
     </row>
     <row r="586" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A586" s="4" t="s">
@@ -35822,9 +35615,6 @@
       <c r="AE586">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN586">
-        <v>216.38300000000001</v>
-      </c>
     </row>
     <row r="587" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A587" s="4" t="s">
@@ -35869,9 +35659,6 @@
       <c r="AE587">
         <v>1.6E-2</v>
       </c>
-      <c r="AN587">
-        <v>268.91699999999997</v>
-      </c>
     </row>
     <row r="588" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A588" s="4" t="s">
@@ -35916,9 +35703,6 @@
       <c r="AE588">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN588">
-        <v>354.55</v>
-      </c>
     </row>
     <row r="589" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A589" s="4" t="s">
@@ -35963,9 +35747,6 @@
       <c r="AE589">
         <v>1.9E-2</v>
       </c>
-      <c r="AN589">
-        <v>304.58300000000003</v>
-      </c>
     </row>
     <row r="590" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A590" s="4" t="s">
@@ -36001,9 +35782,6 @@
       <c r="AE590">
         <v>1.9E-2</v>
       </c>
-      <c r="AN590">
-        <v>339.66699999999997</v>
-      </c>
     </row>
     <row r="591" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A591" s="4" t="s">
@@ -36040,7 +35818,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="AN591">
-        <v>430.661</v>
+        <v>93.73599999999999</v>
       </c>
     </row>
     <row r="592" spans="1:40" x14ac:dyDescent="0.25">
@@ -36254,9 +36032,6 @@
       <c r="AE598">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN598">
-        <v>185</v>
-      </c>
     </row>
     <row r="599" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A599" s="4" t="s">
@@ -36301,9 +36076,6 @@
       <c r="AE599">
         <v>1.6E-2</v>
       </c>
-      <c r="AN599">
-        <v>228.333</v>
-      </c>
     </row>
     <row r="600" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A600" s="4" t="s">
@@ -36348,9 +36120,6 @@
       <c r="AE600">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN600">
-        <v>259.64999999999998</v>
-      </c>
     </row>
     <row r="601" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A601" s="4" t="s">
@@ -36395,9 +36164,6 @@
       <c r="AE601">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN601">
-        <v>469.63299999999998</v>
-      </c>
     </row>
     <row r="602" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A602" s="4" t="s">
@@ -36442,9 +36208,6 @@
       <c r="AE602">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN602">
-        <v>484.6</v>
-      </c>
     </row>
     <row r="603" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A603" s="4" t="s">
@@ -36489,9 +36252,6 @@
       <c r="AE603">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN603">
-        <v>640.1</v>
-      </c>
     </row>
     <row r="604" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A604" s="4" t="s">
@@ -36536,9 +36296,6 @@
       <c r="AE604">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN604">
-        <v>667.16700000000003</v>
-      </c>
     </row>
     <row r="605" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A605" s="4" t="s">
@@ -36574,9 +36331,6 @@
       <c r="AE605">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN605">
-        <v>688.38300000000004</v>
-      </c>
     </row>
     <row r="606" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A606" s="4" t="s">
@@ -36613,7 +36367,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="AN606">
-        <v>768.08500000000004</v>
+        <v>177.47500000000002</v>
       </c>
     </row>
     <row r="607" spans="1:40" x14ac:dyDescent="0.25">
@@ -36827,9 +36581,6 @@
       <c r="AE613">
         <v>0.02</v>
       </c>
-      <c r="AN613">
-        <v>190.95</v>
-      </c>
     </row>
     <row r="614" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A614" s="4" t="s">
@@ -36874,9 +36625,6 @@
       <c r="AE614">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN614">
-        <v>258.83300000000003</v>
-      </c>
     </row>
     <row r="615" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A615" s="4" t="s">
@@ -36921,9 +36669,6 @@
       <c r="AE615">
         <v>0.02</v>
       </c>
-      <c r="AN615">
-        <v>322.43299999999999</v>
-      </c>
     </row>
     <row r="616" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A616" s="4" t="s">
@@ -36968,9 +36713,6 @@
       <c r="AE616">
         <v>0.02</v>
       </c>
-      <c r="AN616">
-        <v>450.03300000000002</v>
-      </c>
     </row>
     <row r="617" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A617" s="4" t="s">
@@ -37015,9 +36757,6 @@
       <c r="AE617">
         <v>1.9E-2</v>
       </c>
-      <c r="AN617">
-        <v>538.76700000000005</v>
-      </c>
     </row>
     <row r="618" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A618" s="4" t="s">
@@ -37062,9 +36801,6 @@
       <c r="AE618">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN618">
-        <v>752.28300000000002</v>
-      </c>
     </row>
     <row r="619" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A619" s="4" t="s">
@@ -37109,9 +36845,6 @@
       <c r="AE619">
         <v>1.9E-2</v>
       </c>
-      <c r="AN619">
-        <v>1014</v>
-      </c>
     </row>
     <row r="620" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A620" s="4" t="s">
@@ -37147,9 +36880,6 @@
       <c r="AE620">
         <v>1.9E-2</v>
       </c>
-      <c r="AN620">
-        <v>655.6</v>
-      </c>
     </row>
     <row r="621" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A621" s="4" t="s">
@@ -37186,7 +36916,7 @@
         <v>1.9E-2</v>
       </c>
       <c r="AN621">
-        <v>812.18100000000004</v>
+        <v>190.90600000000006</v>
       </c>
     </row>
     <row r="622" spans="1:40" x14ac:dyDescent="0.25">
@@ -37400,9 +37130,6 @@
       <c r="AE628">
         <v>0.02</v>
       </c>
-      <c r="AN628">
-        <v>191.833</v>
-      </c>
     </row>
     <row r="629" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A629" s="4" t="s">
@@ -37447,9 +37174,6 @@
       <c r="AE629">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN629">
-        <v>280.16699999999997</v>
-      </c>
     </row>
     <row r="630" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A630" s="4" t="s">
@@ -37494,9 +37218,6 @@
       <c r="AE630">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="AN630">
-        <v>333.38299999999998</v>
-      </c>
     </row>
     <row r="631" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A631" s="4" t="s">
@@ -37541,9 +37262,6 @@
       <c r="AE631">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AN631">
-        <v>439.96699999999998</v>
-      </c>
     </row>
     <row r="632" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A632" s="4" t="s">
@@ -37588,9 +37306,6 @@
       <c r="AE632">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AN632">
-        <v>594.86699999999996</v>
-      </c>
     </row>
     <row r="633" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A633" s="4" t="s">
@@ -37635,9 +37350,6 @@
       <c r="AE633">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="AN633">
-        <v>766.68299999999999</v>
-      </c>
     </row>
     <row r="634" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A634" s="4" t="s">
@@ -37682,9 +37394,6 @@
       <c r="AE634">
         <v>2.4E-2</v>
       </c>
-      <c r="AN634">
-        <v>819</v>
-      </c>
     </row>
     <row r="635" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A635" s="4" t="s">
@@ -37720,9 +37429,6 @@
       <c r="AE635">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AN635">
-        <v>804.31700000000001</v>
-      </c>
     </row>
     <row r="636" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A636" s="4" t="s">
@@ -37759,7 +37465,7 @@
         <v>2.4E-2</v>
       </c>
       <c r="AN636">
-        <v>915.83</v>
+        <v>199.73700000000008</v>
       </c>
     </row>
     <row r="637" spans="1:40" x14ac:dyDescent="0.25">
@@ -37938,9 +37644,6 @@
       <c r="AE642">
         <v>1.6E-2</v>
       </c>
-      <c r="AN642">
-        <v>79.349999999999994</v>
-      </c>
     </row>
     <row r="643" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A643" s="4" t="s">
@@ -37985,9 +37688,6 @@
       <c r="AE643">
         <v>1.4E-2</v>
       </c>
-      <c r="AN643">
-        <v>64.832999999999998</v>
-      </c>
     </row>
     <row r="644" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A644" s="4" t="s">
@@ -38032,9 +37732,6 @@
       <c r="AE644">
         <v>1.4E-2</v>
       </c>
-      <c r="AN644">
-        <v>113</v>
-      </c>
     </row>
     <row r="645" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A645" s="4" t="s">
@@ -38079,9 +37776,6 @@
       <c r="AE645">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN645">
-        <v>138.917</v>
-      </c>
     </row>
     <row r="646" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A646" s="4" t="s">
@@ -38126,9 +37820,6 @@
       <c r="AE646">
         <v>1.6E-2</v>
       </c>
-      <c r="AN646">
-        <v>180.56700000000001</v>
-      </c>
     </row>
     <row r="647" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A647" s="4" t="s">
@@ -38173,9 +37864,6 @@
       <c r="AE647">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN647">
-        <v>223.53299999999999</v>
-      </c>
     </row>
     <row r="648" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A648" s="4" t="s">
@@ -38220,9 +37908,6 @@
       <c r="AE648">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN648">
-        <v>254.06700000000001</v>
-      </c>
     </row>
     <row r="649" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A649" s="4" t="s">
@@ -38258,9 +37943,6 @@
       <c r="AE649">
         <v>1.6E-2</v>
       </c>
-      <c r="AN649">
-        <v>431.21699999999998</v>
-      </c>
     </row>
     <row r="650" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A650" s="4" t="s">
@@ -38296,9 +37978,6 @@
       <c r="AE650">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN650">
-        <v>317.267</v>
-      </c>
     </row>
     <row r="651" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A651" s="4" t="s">
@@ -38335,7 +38014,7 @@
         <v>1.9E-2</v>
       </c>
       <c r="AN651">
-        <v>369.983</v>
+        <v>83.942999999999984</v>
       </c>
     </row>
     <row r="652" spans="1:40" x14ac:dyDescent="0.25">
@@ -38549,9 +38228,6 @@
       <c r="AE658">
         <v>1.6E-2</v>
       </c>
-      <c r="AN658">
-        <v>154</v>
-      </c>
     </row>
     <row r="659" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A659" s="4" t="s">
@@ -38596,9 +38272,6 @@
       <c r="AE659">
         <v>1.4E-2</v>
       </c>
-      <c r="AN659">
-        <v>182.667</v>
-      </c>
     </row>
     <row r="660" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A660" s="4" t="s">
@@ -38643,9 +38316,6 @@
       <c r="AE660">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN660">
-        <v>278.78300000000002</v>
-      </c>
     </row>
     <row r="661" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A661" s="4" t="s">
@@ -38690,9 +38360,6 @@
       <c r="AE661">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN661">
-        <v>357.91699999999997</v>
-      </c>
     </row>
     <row r="662" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A662" s="4" t="s">
@@ -38737,9 +38404,6 @@
       <c r="AE662">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN662">
-        <v>393.017</v>
-      </c>
     </row>
     <row r="663" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A663" s="4" t="s">
@@ -38784,9 +38448,6 @@
       <c r="AE663">
         <v>1.6E-2</v>
       </c>
-      <c r="AN663">
-        <v>533.1</v>
-      </c>
     </row>
     <row r="664" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A664" s="4" t="s">
@@ -38822,9 +38483,6 @@
       <c r="AE664">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="AN664">
-        <v>608.13300000000004</v>
-      </c>
     </row>
     <row r="665" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A665" s="4" t="s">
@@ -38860,9 +38518,6 @@
       <c r="AE665">
         <v>1.6E-2</v>
       </c>
-      <c r="AN665">
-        <v>600.20000000000005</v>
-      </c>
     </row>
     <row r="666" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A666" s="4" t="s">
@@ -38899,7 +38554,7 @@
         <v>1.6E-2</v>
       </c>
       <c r="AN666">
-        <v>772.005</v>
+        <v>171.82600000000002</v>
       </c>
     </row>
     <row r="667" spans="1:40" x14ac:dyDescent="0.25">
@@ -39113,9 +38768,6 @@
       <c r="AE673">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN673">
-        <v>192.667</v>
-      </c>
     </row>
     <row r="674" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A674" s="4" t="s">
@@ -39160,9 +38812,6 @@
       <c r="AE674">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN674">
-        <v>246.167</v>
-      </c>
     </row>
     <row r="675" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A675" s="4" t="s">
@@ -39207,9 +38856,6 @@
       <c r="AE675">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN675">
-        <v>333.1</v>
-      </c>
     </row>
     <row r="676" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A676" s="4" t="s">
@@ -39254,9 +38900,6 @@
       <c r="AE676">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN676">
-        <v>418.31700000000001</v>
-      </c>
     </row>
     <row r="677" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A677" s="4" t="s">
@@ -39301,9 +38944,6 @@
       <c r="AE677">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN677">
-        <v>510.53300000000002</v>
-      </c>
     </row>
     <row r="678" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A678" s="4" t="s">
@@ -39348,9 +38988,6 @@
       <c r="AE678">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN678">
-        <v>649.06700000000001</v>
-      </c>
     </row>
     <row r="679" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A679" s="4" t="s">
@@ -39386,9 +39023,6 @@
       <c r="AE679">
         <v>1.6E-2</v>
       </c>
-      <c r="AN679">
-        <v>805.33299999999997</v>
-      </c>
     </row>
     <row r="680" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A680" s="4" t="s">
@@ -39424,9 +39058,6 @@
       <c r="AE680">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AN680">
-        <v>850.01700000000005</v>
-      </c>
     </row>
     <row r="681" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A681" s="4" t="s">
@@ -39463,7 +39094,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="AN681">
-        <v>887.79399999999998</v>
+        <v>182.548</v>
       </c>
     </row>
     <row r="682" spans="1:40" x14ac:dyDescent="0.25">
@@ -39677,9 +39308,6 @@
       <c r="AE688">
         <v>1.9E-2</v>
       </c>
-      <c r="AN688">
-        <v>215.667</v>
-      </c>
     </row>
     <row r="689" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A689" s="4" t="s">
@@ -39724,9 +39352,6 @@
       <c r="AE689">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AN689">
-        <v>228.167</v>
-      </c>
     </row>
     <row r="690" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A690" s="4" t="s">
@@ -39771,9 +39396,6 @@
       <c r="AE690">
         <v>1.2E-2</v>
       </c>
-      <c r="AN690">
-        <v>337.78300000000002</v>
-      </c>
     </row>
     <row r="691" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A691" s="4" t="s">
@@ -39818,9 +39440,6 @@
       <c r="AE691">
         <v>0.02</v>
       </c>
-      <c r="AN691">
-        <v>513.65</v>
-      </c>
     </row>
     <row r="692" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A692" s="4" t="s">
@@ -39865,9 +39484,6 @@
       <c r="AE692">
         <v>0.02</v>
       </c>
-      <c r="AN692">
-        <v>631.83299999999997</v>
-      </c>
     </row>
     <row r="693" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A693" s="4" t="s">
@@ -39912,9 +39528,6 @@
       <c r="AE693">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AN693">
-        <v>682.53300000000002</v>
-      </c>
     </row>
     <row r="694" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A694" s="4" t="s">
@@ -39953,9 +39566,6 @@
       <c r="AE694">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="AN694">
-        <v>811.76700000000005</v>
-      </c>
     </row>
     <row r="695" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A695" s="4" t="s">
@@ -39991,9 +39601,6 @@
       <c r="AE695">
         <v>2.3E-2</v>
       </c>
-      <c r="AN695">
-        <v>909.5</v>
-      </c>
     </row>
     <row r="696" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A696" s="4" t="s">
@@ -40030,7 +39637,7 @@
         <v>2.3E-2</v>
       </c>
       <c r="AN696">
-        <v>964.33600000000001</v>
+        <v>210.447</v>
       </c>
     </row>
     <row r="750" spans="5:43" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Work on Belgian data
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1158" yWindow="18" windowWidth="12120" windowHeight="6468" tabRatio="862"/>
+    <workbookView xWindow="1158" yWindow="18" windowWidth="12120" windowHeight="6468" tabRatio="862" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3444" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3478" uniqueCount="358">
   <si>
     <t>SimulationName</t>
   </si>
@@ -1095,6 +1095,15 @@
   <si>
     <t>ArizonaFACE93CO2HighIrrWet</t>
   </si>
+  <si>
+    <t>Lonzee04</t>
+  </si>
+  <si>
+    <t>Lonzee06</t>
+  </si>
+  <si>
+    <t>Lonzee08</t>
+  </si>
 </sst>
 </file>
 
@@ -2108,11 +2117,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR1054"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1029" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B1049" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1048" sqref="D1048"/>
+      <selection pane="bottomRight" activeCell="A1052" sqref="A1052"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2148,6 +2157,7 @@
     <col min="34" max="34" width="27.26171875" customWidth="1"/>
     <col min="35" max="35" width="23.41796875" customWidth="1"/>
     <col min="37" max="37" width="30.41796875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.3671875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="17.1015625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="15.9453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -47985,7 +47995,7 @@
         <v>6.45</v>
       </c>
     </row>
-    <row r="1041" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1041" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A1041" s="25" t="s">
         <v>354</v>
       </c>
@@ -48007,7 +48017,7 @@
         <v>5.1989999999999998</v>
       </c>
     </row>
-    <row r="1042" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1042" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A1042" s="25" t="s">
         <v>354</v>
       </c>
@@ -48029,7 +48039,7 @@
         <v>5.3159999999999998</v>
       </c>
     </row>
-    <row r="1043" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1043" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A1043" s="25" t="s">
         <v>354</v>
       </c>
@@ -48051,7 +48061,7 @@
         <v>5.1109999999999998</v>
       </c>
     </row>
-    <row r="1044" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1044" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A1044" s="25" t="s">
         <v>354</v>
       </c>
@@ -48073,7 +48083,7 @@
         <v>3.5390000000000001</v>
       </c>
     </row>
-    <row r="1045" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1045" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A1045" s="25" t="s">
         <v>354</v>
       </c>
@@ -48095,7 +48105,7 @@
         <v>1.581</v>
       </c>
     </row>
-    <row r="1046" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1046" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A1046" s="25" t="s">
         <v>354</v>
       </c>
@@ -48117,7 +48127,7 @@
         <v>9.2700000000000005E-2</v>
       </c>
     </row>
-    <row r="1047" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1047" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A1047" s="25" t="s">
         <v>354</v>
       </c>
@@ -48139,7 +48149,7 @@
         <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="1048" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1048" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A1048" s="25" t="s">
         <v>354</v>
       </c>
@@ -48170,22 +48180,55 @@
         <v>43.11</v>
       </c>
     </row>
-    <row r="1049" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="D1049" s="25"/>
-    </row>
-    <row r="1050" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="D1050" s="25"/>
-    </row>
-    <row r="1051" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="D1051" s="25"/>
-    </row>
-    <row r="1052" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1049" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1049" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1049" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1049">
+        <v>890</v>
+      </c>
+      <c r="AK1049">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1050" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D1050" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1050">
+        <v>750</v>
+      </c>
+      <c r="AK1050">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1051" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="D1051" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1051">
+        <v>910</v>
+      </c>
+      <c r="AK1051">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="D1052" s="25"/>
     </row>
-    <row r="1053" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1053" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="D1053" s="25"/>
     </row>
-    <row r="1054" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1054" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="D1054" s="25"/>
     </row>
   </sheetData>
@@ -56197,10 +56240,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E434"/>
+  <dimension ref="A1:E464"/>
   <sheetViews>
-    <sheetView topLeftCell="A410" workbookViewId="0">
-      <selection activeCell="C435" sqref="C435"/>
+    <sheetView tabSelected="1" topLeftCell="A438" workbookViewId="0">
+      <selection activeCell="B463" sqref="B463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -61232,6 +61275,317 @@
       <c r="C434">
         <v>90</v>
       </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A435" t="s">
+        <v>355</v>
+      </c>
+      <c r="B435" s="11">
+        <v>38274</v>
+      </c>
+      <c r="C435">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A436" t="s">
+        <v>355</v>
+      </c>
+      <c r="B436" s="11">
+        <v>38418</v>
+      </c>
+      <c r="C436">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A437" t="s">
+        <v>355</v>
+      </c>
+      <c r="B437" s="11">
+        <v>38454</v>
+      </c>
+      <c r="C437">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A438" t="s">
+        <v>355</v>
+      </c>
+      <c r="B438" s="11">
+        <v>38457</v>
+      </c>
+      <c r="C438">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A439" t="s">
+        <v>355</v>
+      </c>
+      <c r="B439" s="11">
+        <v>38492</v>
+      </c>
+      <c r="C439">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A440" t="s">
+        <v>355</v>
+      </c>
+      <c r="B440" s="11">
+        <v>38504</v>
+      </c>
+      <c r="C440">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A441" t="s">
+        <v>355</v>
+      </c>
+      <c r="B441" s="11">
+        <v>38517</v>
+      </c>
+      <c r="C441">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A442" t="s">
+        <v>355</v>
+      </c>
+      <c r="B442" s="11">
+        <v>38533</v>
+      </c>
+      <c r="C442">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A443" t="s">
+        <v>355</v>
+      </c>
+      <c r="B443" s="11">
+        <v>38548</v>
+      </c>
+      <c r="C443">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A444" t="s">
+        <v>355</v>
+      </c>
+      <c r="B444" s="11">
+        <v>38563</v>
+      </c>
+      <c r="C444">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A445" t="s">
+        <v>356</v>
+      </c>
+      <c r="B445" s="11">
+        <v>39003</v>
+      </c>
+      <c r="C445">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A446" t="s">
+        <v>356</v>
+      </c>
+      <c r="B446" s="11">
+        <v>39089</v>
+      </c>
+      <c r="C446">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A447" t="s">
+        <v>356</v>
+      </c>
+      <c r="B447" s="11">
+        <v>39167</v>
+      </c>
+      <c r="C447">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A448" t="s">
+        <v>356</v>
+      </c>
+      <c r="B448" s="11">
+        <v>39179</v>
+      </c>
+      <c r="C448">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A449" t="s">
+        <v>356</v>
+      </c>
+      <c r="B449" s="11">
+        <v>39212</v>
+      </c>
+      <c r="C449">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A450" t="s">
+        <v>356</v>
+      </c>
+      <c r="B450" s="11">
+        <v>39224</v>
+      </c>
+      <c r="C450">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A451" t="s">
+        <v>356</v>
+      </c>
+      <c r="B451" s="11">
+        <v>39234</v>
+      </c>
+      <c r="C451">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A452" t="s">
+        <v>356</v>
+      </c>
+      <c r="B452" s="11">
+        <v>39252</v>
+      </c>
+      <c r="C452">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A453" t="s">
+        <v>356</v>
+      </c>
+      <c r="B453" s="11">
+        <v>39263</v>
+      </c>
+      <c r="C453">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A454" t="s">
+        <v>357</v>
+      </c>
+      <c r="B454" s="11">
+        <v>39765</v>
+      </c>
+      <c r="C454">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A455" t="s">
+        <v>357</v>
+      </c>
+      <c r="B455" s="11">
+        <v>39798</v>
+      </c>
+      <c r="C455">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A456" t="s">
+        <v>357</v>
+      </c>
+      <c r="B456" s="11">
+        <v>39889</v>
+      </c>
+      <c r="C456">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="457" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A457" t="s">
+        <v>357</v>
+      </c>
+      <c r="B457" s="11">
+        <v>39927</v>
+      </c>
+      <c r="C457">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="458" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A458" t="s">
+        <v>357</v>
+      </c>
+      <c r="B458" s="11">
+        <v>39966</v>
+      </c>
+      <c r="C458">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="459" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A459" t="s">
+        <v>357</v>
+      </c>
+      <c r="B459" s="11">
+        <v>39975</v>
+      </c>
+      <c r="C459">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="460" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A460" t="s">
+        <v>357</v>
+      </c>
+      <c r="B460" s="11">
+        <v>39983</v>
+      </c>
+      <c r="C460">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="461" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A461" t="s">
+        <v>357</v>
+      </c>
+      <c r="B461" s="11">
+        <v>40001</v>
+      </c>
+      <c r="C461">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="462" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A462" t="s">
+        <v>357</v>
+      </c>
+      <c r="B462" s="11">
+        <v>40009</v>
+      </c>
+      <c r="C462">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="464" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B464" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the mighty GORGAN
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3478" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3493" uniqueCount="359">
   <si>
     <t>SimulationName</t>
   </si>
@@ -1104,6 +1104,9 @@
   <si>
     <t>Lonzee08</t>
   </si>
+  <si>
+    <t>Gorgan05</t>
+  </si>
 </sst>
 </file>
 
@@ -2115,13 +2118,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR1054"/>
+  <dimension ref="A1:AR1065"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1049" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R1049" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A1052" sqref="A1052"/>
+      <selection pane="bottomRight" activeCell="R1052" sqref="R1052:R1058"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -48223,13 +48226,230 @@
       </c>
     </row>
     <row r="1052" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1052" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1052" s="11">
+        <v>38762.5167</v>
+      </c>
       <c r="D1052" s="25"/>
+      <c r="E1052">
+        <v>12.993</v>
+      </c>
+      <c r="I1052">
+        <v>0.29147000000000001</v>
+      </c>
+      <c r="R1052">
+        <v>0.40613500000000002</v>
+      </c>
     </row>
     <row r="1053" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1053" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1053" s="11">
+        <v>38772.504300000001</v>
+      </c>
       <c r="D1053" s="25"/>
+      <c r="E1053">
+        <v>29.234300000000001</v>
+      </c>
+      <c r="I1053">
+        <v>0.48391499999999998</v>
+      </c>
     </row>
     <row r="1054" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1054" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1054" s="11">
+        <v>38781.8531</v>
+      </c>
       <c r="D1054" s="25"/>
+      <c r="E1054">
+        <v>68.213499999999996</v>
+      </c>
+      <c r="I1054">
+        <v>0.94015000000000004</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1055" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1055" s="11">
+        <v>38793.4637</v>
+      </c>
+      <c r="E1055">
+        <v>139.67500000000001</v>
+      </c>
+      <c r="I1055">
+        <v>2.03186</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1056" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1056" s="11">
+        <v>38802.517</v>
+      </c>
+      <c r="E1056">
+        <v>292.34300000000002</v>
+      </c>
+      <c r="I1056">
+        <v>2.8837899999999999</v>
+      </c>
+      <c r="R1056">
+        <v>7.1623700000000001</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1057" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1057" s="11">
+        <v>38812.864000000001</v>
+      </c>
+      <c r="E1057">
+        <v>470.99799999999999</v>
+      </c>
+      <c r="I1057">
+        <v>3.96353</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1058" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1058" s="11">
+        <v>38822.945</v>
+      </c>
+      <c r="E1058">
+        <v>893.27099999999996</v>
+      </c>
+      <c r="I1058">
+        <v>4.2159300000000002</v>
+      </c>
+      <c r="R1058">
+        <v>14.680099999999999</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1059" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1059" s="11">
+        <v>38830.023000000001</v>
+      </c>
+      <c r="E1059">
+        <v>864.03700000000003</v>
+      </c>
+      <c r="I1059">
+        <v>4.4561700000000002</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1060" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1060" s="11">
+        <v>38837.478999999999</v>
+      </c>
+      <c r="E1060">
+        <v>1075.17</v>
+      </c>
+      <c r="G1060">
+        <v>16.241299999999999</v>
+      </c>
+      <c r="I1060">
+        <v>2.7059899999999999</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1061" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1061" s="11">
+        <v>38843.648000000001</v>
+      </c>
+      <c r="E1061">
+        <v>1289.56</v>
+      </c>
+      <c r="G1061">
+        <v>87.703000000000003</v>
+      </c>
+      <c r="I1061">
+        <v>1.2315700000000001</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1062" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1062" s="11">
+        <v>38851.353999999999</v>
+      </c>
+      <c r="E1062">
+        <v>1188.8599999999999</v>
+      </c>
+      <c r="G1062">
+        <v>198.14400000000001</v>
+      </c>
+      <c r="I1062">
+        <v>0.98021999999999998</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1063" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1063" s="11">
+        <v>38857.508999999998</v>
+      </c>
+      <c r="E1063">
+        <v>1344.78</v>
+      </c>
+      <c r="G1063">
+        <v>331.32299999999998</v>
+      </c>
+      <c r="I1063">
+        <v>0.29714800000000002</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1064" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1064" s="11">
+        <v>38865.525000000001</v>
+      </c>
+      <c r="E1064">
+        <v>1192.1099999999999</v>
+      </c>
+      <c r="G1064">
+        <v>500.23200000000003</v>
+      </c>
+      <c r="I1064">
+        <v>9.8136300000000003E-3</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1065" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1065" s="11">
+        <v>38871.985000000001</v>
+      </c>
+      <c r="D1065" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1065">
+        <v>1270.07</v>
+      </c>
+      <c r="G1065">
+        <v>539.21100000000001</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:AP853">
@@ -56240,16 +56460,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E464"/>
+  <dimension ref="A1:E476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A438" workbookViewId="0">
-      <selection activeCell="B463" sqref="B463"/>
+    <sheetView tabSelected="1" topLeftCell="A450" workbookViewId="0">
+      <selection activeCell="B465" sqref="B465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.15625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -61584,8 +61805,47 @@
         <v>89</v>
       </c>
     </row>
+    <row r="463" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C463" s="11"/>
+    </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B464" s="11"/>
+      <c r="C464" s="11"/>
+    </row>
+    <row r="465" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C465" s="11"/>
+    </row>
+    <row r="466" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C466" s="11"/>
+    </row>
+    <row r="467" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C467" s="11"/>
+    </row>
+    <row r="468" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C468" s="11"/>
+    </row>
+    <row r="469" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C469" s="11"/>
+    </row>
+    <row r="470" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C470" s="11"/>
+    </row>
+    <row r="471" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C471" s="11"/>
+    </row>
+    <row r="472" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C472" s="11"/>
+    </row>
+    <row r="473" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C473" s="11"/>
+    </row>
+    <row r="474" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C474" s="11"/>
+    </row>
+    <row r="475" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C475" s="11"/>
+    </row>
+    <row r="476" spans="3:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="C476" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working on Belgian data
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1158" yWindow="18" windowWidth="12120" windowHeight="6468" tabRatio="862" activeTab="3"/>
+    <workbookView xWindow="1158" yWindow="18" windowWidth="12120" windowHeight="6468" tabRatio="862"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3493" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3511" uniqueCount="359">
   <si>
     <t>SimulationName</t>
   </si>
@@ -2118,19 +2118,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR1065"/>
+  <dimension ref="A1:AR1083"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="R1049" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B1060" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R1052" sqref="R1052:R1058"/>
+      <selection pane="bottomRight" activeCell="B1084" sqref="B1084"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="49.578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.89453125" customWidth="1"/>
     <col min="3" max="3" width="24.9453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.15625" customWidth="1"/>
     <col min="5" max="5" width="28.578125" customWidth="1"/>
@@ -2161,6 +2161,7 @@
     <col min="35" max="35" width="23.41796875" customWidth="1"/>
     <col min="37" max="37" width="30.41796875" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="18.3671875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.47265625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="17.1015625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="15.9453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -47998,7 +47999,7 @@
         <v>6.45</v>
       </c>
     </row>
-    <row r="1041" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="1041" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1041" s="25" t="s">
         <v>354</v>
       </c>
@@ -48020,7 +48021,7 @@
         <v>5.1989999999999998</v>
       </c>
     </row>
-    <row r="1042" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="1042" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1042" s="25" t="s">
         <v>354</v>
       </c>
@@ -48042,7 +48043,7 @@
         <v>5.3159999999999998</v>
       </c>
     </row>
-    <row r="1043" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="1043" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1043" s="25" t="s">
         <v>354</v>
       </c>
@@ -48064,7 +48065,7 @@
         <v>5.1109999999999998</v>
       </c>
     </row>
-    <row r="1044" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="1044" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1044" s="25" t="s">
         <v>354</v>
       </c>
@@ -48086,7 +48087,7 @@
         <v>3.5390000000000001</v>
       </c>
     </row>
-    <row r="1045" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="1045" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1045" s="25" t="s">
         <v>354</v>
       </c>
@@ -48108,7 +48109,7 @@
         <v>1.581</v>
       </c>
     </row>
-    <row r="1046" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="1046" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1046" s="25" t="s">
         <v>354</v>
       </c>
@@ -48130,7 +48131,7 @@
         <v>9.2700000000000005E-2</v>
       </c>
     </row>
-    <row r="1047" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="1047" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1047" s="25" t="s">
         <v>354</v>
       </c>
@@ -48152,7 +48153,7 @@
         <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="1048" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="1048" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1048" s="25" t="s">
         <v>354</v>
       </c>
@@ -48183,272 +48184,683 @@
         <v>43.11</v>
       </c>
     </row>
-    <row r="1049" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1049" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="D1049" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G1049">
-        <v>890</v>
-      </c>
-      <c r="AK1049">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="1050" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1050" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="D1050" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G1050">
-        <v>750</v>
-      </c>
-      <c r="AK1050">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="1051" spans="1:37" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1051" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="D1051" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G1051">
-        <v>910</v>
-      </c>
-      <c r="AK1051">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="1052" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="1049" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1049" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1049" s="11">
+        <v>38762</v>
+      </c>
+      <c r="D1049" s="25"/>
+      <c r="E1049">
+        <v>12.993</v>
+      </c>
+      <c r="I1049">
+        <v>0.29147000000000001</v>
+      </c>
+      <c r="R1049">
+        <v>0.40613500000000002</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1050" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1050" s="11">
+        <v>38772</v>
+      </c>
+      <c r="D1050" s="25"/>
+      <c r="E1050">
+        <v>29.234300000000001</v>
+      </c>
+      <c r="I1050">
+        <v>0.48391499999999998</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1051" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1051" s="11">
+        <v>38781</v>
+      </c>
+      <c r="D1051" s="25"/>
+      <c r="E1051">
+        <v>68.213499999999996</v>
+      </c>
+      <c r="I1051">
+        <v>0.94015000000000004</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1052" t="s">
         <v>358</v>
       </c>
       <c r="B1052" s="11">
-        <v>38762.5167</v>
-      </c>
-      <c r="D1052" s="25"/>
+        <v>38793</v>
+      </c>
       <c r="E1052">
-        <v>12.993</v>
+        <v>139.67500000000001</v>
       </c>
       <c r="I1052">
-        <v>0.29147000000000001</v>
-      </c>
-      <c r="R1052">
-        <v>0.40613500000000002</v>
-      </c>
-    </row>
-    <row r="1053" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+        <v>2.03186</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1053" t="s">
         <v>358</v>
       </c>
       <c r="B1053" s="11">
-        <v>38772.504300000001</v>
-      </c>
-      <c r="D1053" s="25"/>
+        <v>38802</v>
+      </c>
       <c r="E1053">
-        <v>29.234300000000001</v>
+        <v>292.34300000000002</v>
       </c>
       <c r="I1053">
-        <v>0.48391499999999998</v>
-      </c>
-    </row>
-    <row r="1054" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+        <v>2.8837899999999999</v>
+      </c>
+      <c r="R1053">
+        <v>7.1623700000000001</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1054" t="s">
         <v>358</v>
       </c>
       <c r="B1054" s="11">
-        <v>38781.8531</v>
-      </c>
-      <c r="D1054" s="25"/>
+        <v>38812</v>
+      </c>
       <c r="E1054">
-        <v>68.213499999999996</v>
+        <v>470.99799999999999</v>
       </c>
       <c r="I1054">
-        <v>0.94015000000000004</v>
-      </c>
-    </row>
-    <row r="1055" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+        <v>3.96353</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1055" t="s">
         <v>358</v>
       </c>
       <c r="B1055" s="11">
-        <v>38793.4637</v>
+        <v>38822</v>
       </c>
       <c r="E1055">
-        <v>139.67500000000001</v>
+        <v>893.27099999999996</v>
       </c>
       <c r="I1055">
-        <v>2.03186</v>
-      </c>
-    </row>
-    <row r="1056" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+        <v>4.2159300000000002</v>
+      </c>
+      <c r="R1055">
+        <v>14.680099999999999</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1056" t="s">
         <v>358</v>
       </c>
       <c r="B1056" s="11">
-        <v>38802.517</v>
+        <v>38830</v>
       </c>
       <c r="E1056">
-        <v>292.34300000000002</v>
+        <v>864.03700000000003</v>
       </c>
       <c r="I1056">
-        <v>2.8837899999999999</v>
-      </c>
-      <c r="R1056">
-        <v>7.1623700000000001</v>
-      </c>
-    </row>
-    <row r="1057" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>4.4561700000000002</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A1057" t="s">
         <v>358</v>
       </c>
       <c r="B1057" s="11">
-        <v>38812.864000000001</v>
+        <v>38837</v>
       </c>
       <c r="E1057">
-        <v>470.99799999999999</v>
+        <v>1075.17</v>
+      </c>
+      <c r="G1057">
+        <v>16.241299999999999</v>
       </c>
       <c r="I1057">
-        <v>3.96353</v>
-      </c>
-    </row>
-    <row r="1058" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>2.7059899999999999</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A1058" t="s">
         <v>358</v>
       </c>
       <c r="B1058" s="11">
-        <v>38822.945</v>
+        <v>38843</v>
       </c>
       <c r="E1058">
-        <v>893.27099999999996</v>
+        <v>1289.56</v>
+      </c>
+      <c r="G1058">
+        <v>87.703000000000003</v>
       </c>
       <c r="I1058">
-        <v>4.2159300000000002</v>
-      </c>
-      <c r="R1058">
-        <v>14.680099999999999</v>
-      </c>
-    </row>
-    <row r="1059" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>1.2315700000000001</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A1059" t="s">
         <v>358</v>
       </c>
       <c r="B1059" s="11">
-        <v>38830.023000000001</v>
+        <v>38851</v>
       </c>
       <c r="E1059">
-        <v>864.03700000000003</v>
+        <v>1188.8599999999999</v>
+      </c>
+      <c r="G1059">
+        <v>198.14400000000001</v>
       </c>
       <c r="I1059">
-        <v>4.4561700000000002</v>
-      </c>
-    </row>
-    <row r="1060" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>0.98021999999999998</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A1060" t="s">
         <v>358</v>
       </c>
       <c r="B1060" s="11">
-        <v>38837.478999999999</v>
+        <v>38857</v>
       </c>
       <c r="E1060">
-        <v>1075.17</v>
+        <v>1344.78</v>
       </c>
       <c r="G1060">
-        <v>16.241299999999999</v>
+        <v>331.32299999999998</v>
       </c>
       <c r="I1060">
-        <v>2.7059899999999999</v>
-      </c>
-    </row>
-    <row r="1061" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>0.29714800000000002</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A1061" t="s">
         <v>358</v>
       </c>
       <c r="B1061" s="11">
-        <v>38843.648000000001</v>
+        <v>38865</v>
       </c>
       <c r="E1061">
-        <v>1289.56</v>
+        <v>1192.1099999999999</v>
       </c>
       <c r="G1061">
-        <v>87.703000000000003</v>
+        <v>500.23200000000003</v>
       </c>
       <c r="I1061">
-        <v>1.2315700000000001</v>
-      </c>
-    </row>
-    <row r="1062" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+        <v>9.8136300000000003E-3</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A1062" t="s">
         <v>358</v>
       </c>
       <c r="B1062" s="11">
-        <v>38851.353999999999</v>
+        <v>38871</v>
+      </c>
+      <c r="D1062" t="s">
+        <v>157</v>
       </c>
       <c r="E1062">
-        <v>1188.8599999999999</v>
+        <v>1270.07</v>
       </c>
       <c r="G1062">
-        <v>198.14400000000001</v>
-      </c>
-      <c r="I1062">
-        <v>0.98021999999999998</v>
-      </c>
-    </row>
-    <row r="1063" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1063" t="s">
-        <v>358</v>
+        <v>539.21100000000001</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1063" s="4" t="s">
+        <v>355</v>
       </c>
       <c r="B1063" s="11">
-        <v>38857.508999999998</v>
+        <v>38425</v>
       </c>
       <c r="E1063">
-        <v>1344.78</v>
-      </c>
-      <c r="G1063">
-        <v>331.32299999999998</v>
-      </c>
-      <c r="I1063">
-        <v>0.29714800000000002</v>
-      </c>
-    </row>
-    <row r="1064" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1064" t="s">
-        <v>358</v>
+        <v>41.257399999999997</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1064" s="4" t="s">
+        <v>355</v>
       </c>
       <c r="B1064" s="11">
-        <v>38865.525000000001</v>
+        <v>38438</v>
       </c>
       <c r="E1064">
-        <v>1192.1099999999999</v>
-      </c>
-      <c r="G1064">
-        <v>500.23200000000003</v>
-      </c>
-      <c r="I1064">
-        <v>9.8136300000000003E-3</v>
-      </c>
-    </row>
-    <row r="1065" spans="1:18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1065" t="s">
-        <v>358</v>
+        <v>100.196</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1065" s="4" t="s">
+        <v>355</v>
       </c>
       <c r="B1065" s="11">
-        <v>38871.985000000001</v>
-      </c>
-      <c r="D1065" t="s">
+        <v>38452</v>
+      </c>
+      <c r="E1065">
+        <v>235.756</v>
+      </c>
+      <c r="K1065">
+        <v>70.726900000000001</v>
+      </c>
+      <c r="N1065">
+        <v>76.620800000000003</v>
+      </c>
+      <c r="P1065">
+        <v>17.681699999999999</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1066" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1066" s="11">
+        <v>38459</v>
+      </c>
+      <c r="E1066">
+        <v>259.33199999999999</v>
+      </c>
+      <c r="I1066">
+        <v>1.4011499999999999</v>
+      </c>
+      <c r="K1066">
+        <v>123.77200000000001</v>
+      </c>
+      <c r="N1066">
+        <v>141.45400000000001</v>
+      </c>
+      <c r="P1066">
+        <v>11.787800000000001</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1067" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1067" s="11">
+        <v>38465</v>
+      </c>
+      <c r="E1067">
+        <v>394.892</v>
+      </c>
+      <c r="I1067">
+        <v>3.02841</v>
+      </c>
+      <c r="K1067">
+        <v>159.136</v>
+      </c>
+      <c r="N1067">
+        <v>200.393</v>
+      </c>
+      <c r="P1067">
+        <v>17.681699999999999</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1068" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1068" s="11">
+        <v>38472</v>
+      </c>
+      <c r="E1068">
+        <v>506.87599999999998</v>
+      </c>
+      <c r="I1068">
+        <v>3.7477399999999998</v>
+      </c>
+      <c r="K1068">
+        <v>153.24199999999999</v>
+      </c>
+      <c r="N1068">
+        <v>300.589</v>
+      </c>
+      <c r="P1068">
+        <v>11.787800000000001</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1069" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1069" s="11">
+        <v>38480</v>
+      </c>
+      <c r="E1069">
+        <v>666.01199999999994</v>
+      </c>
+      <c r="I1069">
+        <v>3.5118399999999999</v>
+      </c>
+      <c r="K1069">
+        <v>218.07499999999999</v>
+      </c>
+      <c r="N1069">
+        <v>412.57400000000001</v>
+      </c>
+      <c r="P1069">
+        <v>41.257399999999997</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1070" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1070" s="11">
+        <v>38486</v>
+      </c>
+      <c r="E1070">
+        <v>854.61699999999996</v>
+      </c>
+      <c r="I1070">
+        <v>3.28382</v>
+      </c>
+      <c r="K1070">
+        <v>194.499</v>
+      </c>
+      <c r="N1070">
+        <v>618.86099999999999</v>
+      </c>
+      <c r="P1070">
+        <v>47.151299999999999</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1071" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1071" s="11">
+        <v>38492</v>
+      </c>
+      <c r="E1071">
+        <v>1113.95</v>
+      </c>
+      <c r="I1071">
+        <v>3.0244300000000002</v>
+      </c>
+      <c r="K1071">
+        <v>153.24199999999999</v>
+      </c>
+      <c r="N1071">
+        <v>548.13400000000001</v>
+      </c>
+      <c r="P1071">
+        <v>53.045200000000001</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1072" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1072" s="11">
+        <v>38500</v>
+      </c>
+      <c r="E1072">
+        <v>1119.8399999999999</v>
+      </c>
+      <c r="I1072">
+        <v>2.9529399999999999</v>
+      </c>
+      <c r="K1072">
+        <v>159.136</v>
+      </c>
+      <c r="N1072">
+        <v>719.05700000000002</v>
+      </c>
+      <c r="P1072">
+        <v>82.514700000000005</v>
+      </c>
+      <c r="AM1072">
+        <v>91.690700000000007</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1073" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1073" s="11">
+        <v>38506</v>
+      </c>
+      <c r="E1073">
+        <v>1408.64</v>
+      </c>
+      <c r="I1073">
+        <v>3.0223399999999998</v>
+      </c>
+      <c r="K1073">
+        <v>165.029</v>
+      </c>
+      <c r="N1073">
+        <v>795.678</v>
+      </c>
+      <c r="P1073">
+        <v>100.196</v>
+      </c>
+      <c r="AM1073">
+        <v>162.55500000000001</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1074" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1074" s="11">
+        <v>38513</v>
+      </c>
+      <c r="E1074">
+        <v>1532.42</v>
+      </c>
+      <c r="I1074">
+        <v>2.67685</v>
+      </c>
+      <c r="K1074">
+        <v>135.56</v>
+      </c>
+      <c r="N1074">
+        <v>760.31399999999996</v>
+      </c>
+      <c r="P1074">
+        <v>123.77200000000001</v>
+      </c>
+      <c r="AM1074">
+        <v>215.74199999999999</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1075" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1075" s="11">
+        <v>38520</v>
+      </c>
+      <c r="E1075">
+        <v>1732.81</v>
+      </c>
+      <c r="I1075">
+        <v>2.2374499999999999</v>
+      </c>
+      <c r="K1075">
+        <v>88.408600000000007</v>
+      </c>
+      <c r="N1075">
+        <v>736.73900000000003</v>
+      </c>
+      <c r="P1075">
+        <v>153.24199999999999</v>
+      </c>
+      <c r="AM1075">
+        <v>380.73200000000003</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1076" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1076" s="11">
+        <v>38526</v>
+      </c>
+      <c r="E1076">
+        <v>2056.9699999999998</v>
+      </c>
+      <c r="I1076">
+        <v>1.6023000000000001</v>
+      </c>
+      <c r="K1076">
+        <v>88.408600000000007</v>
+      </c>
+      <c r="N1076">
+        <v>583.49699999999996</v>
+      </c>
+      <c r="P1076">
+        <v>153.24199999999999</v>
+      </c>
+      <c r="AM1076">
+        <v>728.04300000000001</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1077" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1077" s="11">
+        <v>38533</v>
+      </c>
+      <c r="E1077">
+        <v>2068.7600000000002</v>
+      </c>
+      <c r="I1077">
+        <v>0.99854399999999999</v>
+      </c>
+      <c r="K1077">
+        <v>41.257399999999997</v>
+      </c>
+      <c r="N1077">
+        <v>559.92100000000005</v>
+      </c>
+      <c r="P1077">
+        <v>170.923</v>
+      </c>
+      <c r="AM1077">
+        <v>940.07600000000002</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1078" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1078" s="11">
+        <v>38540</v>
+      </c>
+      <c r="E1078">
+        <v>2068.7600000000002</v>
+      </c>
+      <c r="I1078">
+        <v>0.52780300000000002</v>
+      </c>
+      <c r="K1078">
+        <v>0</v>
+      </c>
+      <c r="N1078">
+        <v>506.87599999999998</v>
+      </c>
+      <c r="P1078">
+        <v>229.86199999999999</v>
+      </c>
+      <c r="AM1078">
+        <v>1052.0999999999999</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1079" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1079" s="11">
+        <v>38547</v>
+      </c>
+      <c r="E1079">
+        <v>2186.64</v>
+      </c>
+      <c r="I1079">
+        <v>0.36234699999999997</v>
+      </c>
+      <c r="AM1079">
+        <v>1152.3699999999999</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1080" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1080" s="11">
+        <v>38553</v>
+      </c>
+      <c r="E1080">
+        <v>1998.04</v>
+      </c>
+      <c r="I1080">
+        <v>0</v>
+      </c>
+      <c r="AM1080">
+        <v>1082.04</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1081" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B1081" s="11">
+        <v>38567</v>
+      </c>
+      <c r="D1081" t="s">
         <v>157</v>
       </c>
-      <c r="E1065">
-        <v>1270.07</v>
-      </c>
-      <c r="G1065">
-        <v>539.21100000000001</v>
+      <c r="E1081">
+        <v>1962.67</v>
+      </c>
+      <c r="G1081">
+        <v>890</v>
+      </c>
+      <c r="AK1081">
+        <v>464</v>
+      </c>
+      <c r="AM1081">
+        <v>1064.6199999999999</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1082" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B1082" s="11">
+        <v>39299</v>
+      </c>
+      <c r="D1082" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1082">
+        <v>750</v>
+      </c>
+      <c r="AK1082">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1083" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B1083" s="11">
+        <v>40032</v>
+      </c>
+      <c r="D1083" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1083">
+        <v>910</v>
+      </c>
+      <c r="AK1083">
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -48466,10 +48878,10 @@
   <dimension ref="A1:M119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="7938" ySplit="570" topLeftCell="A22" activePane="bottomRight"/>
+      <pane xSplit="7938" ySplit="570" topLeftCell="A96" activePane="bottomLeft"/>
       <selection activeCell="A40" sqref="A40"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="B115" sqref="B115:B119"/>
+      <selection pane="bottomLeft" activeCell="B120" sqref="B120"/>
       <selection pane="bottomRight" activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
@@ -56462,7 +56874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A450" workbookViewId="0">
+    <sheetView topLeftCell="A450" workbookViewId="0">
       <selection activeCell="B465" sqref="B465"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Extra leaf appearance data for Janz
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3864" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3898" uniqueCount="857">
   <si>
     <t>SimulationName</t>
   </si>
@@ -2600,9 +2600,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy\-m\-dd"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -2656,7 +2657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2678,6 +2679,8 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2983,13 +2986,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AV3277"/>
+  <dimension ref="A1:AV3122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AJ2910" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AN2945" sqref="AN2945"/>
+      <pane xSplit="6840" ySplit="1440" topLeftCell="AD2948" activePane="bottomRight"/>
+      <selection pane="topRight" activeCell="D2882" sqref="D2882"/>
+      <selection pane="bottomLeft" activeCell="A2956" sqref="A2956"/>
+      <selection pane="bottomRight" activeCell="AE2949" sqref="AE2949"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -68943,135 +68946,407 @@
       </c>
     </row>
     <row r="2949" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="B2949" s="6"/>
+      <c r="A2949" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="B2949" s="9">
+        <v>41103</v>
+      </c>
+      <c r="AE2949" s="10">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="2950" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="B2950" s="6"/>
+      <c r="A2950" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="B2950" s="9">
+        <v>41103</v>
+      </c>
+      <c r="AE2950" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="2951" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="B2951" s="6"/>
+      <c r="A2951" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="B2951" s="9">
+        <v>41110</v>
+      </c>
+      <c r="AE2951" s="10">
+        <v>4</v>
+      </c>
     </row>
     <row r="2952" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="B2952" s="6"/>
+      <c r="A2952" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="B2952" s="9">
+        <v>41116</v>
+      </c>
+      <c r="AE2952" s="10">
+        <v>5.2</v>
+      </c>
     </row>
     <row r="2953" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="B2953" s="6"/>
+      <c r="A2953" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="B2953" s="9">
+        <v>41128</v>
+      </c>
+      <c r="AE2953" s="10">
+        <v>9</v>
+      </c>
     </row>
     <row r="2954" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="B2954" s="6"/>
+      <c r="A2954" s="5" t="s">
+        <v>831</v>
+      </c>
+      <c r="B2954" s="9">
+        <v>41116</v>
+      </c>
+      <c r="AE2954" s="10">
+        <v>2.4</v>
+      </c>
     </row>
     <row r="2955" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="B2955" s="6"/>
+      <c r="A2955" s="5" t="s">
+        <v>831</v>
+      </c>
+      <c r="B2955" s="9">
+        <v>41128</v>
+      </c>
+      <c r="AE2955" s="10">
+        <v>3.55</v>
+      </c>
     </row>
     <row r="2956" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="B2956" s="6"/>
+      <c r="A2956" s="5" t="s">
+        <v>831</v>
+      </c>
+      <c r="B2956" s="9">
+        <v>41136</v>
+      </c>
+      <c r="AE2956" s="10">
+        <v>4.8499999999999996</v>
+      </c>
     </row>
     <row r="2957" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="B2957" s="6"/>
+      <c r="A2957" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="B2957" s="9">
+        <v>41099</v>
+      </c>
+      <c r="AE2957" s="10">
+        <v>5.65</v>
+      </c>
     </row>
     <row r="2958" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="B2958" s="6"/>
+      <c r="A2958" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="B2958" s="9">
+        <v>41109</v>
+      </c>
+      <c r="AE2958" s="10">
+        <v>6.55</v>
+      </c>
     </row>
     <row r="2959" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="B2959" s="6"/>
+      <c r="A2959" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B2959" s="9">
+        <v>41099</v>
+      </c>
+      <c r="AE2959" s="10">
+        <v>4.7</v>
+      </c>
     </row>
     <row r="2960" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="B2960" s="6"/>
-    </row>
-    <row r="2961" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2961" s="6"/>
-    </row>
-    <row r="2962" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2962" s="6"/>
-    </row>
-    <row r="2963" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2963" s="6"/>
-    </row>
-    <row r="2964" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2964" s="6"/>
-    </row>
-    <row r="2965" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2965" s="6"/>
-    </row>
-    <row r="2966" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2966" s="6"/>
-    </row>
-    <row r="2967" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2967" s="6"/>
-    </row>
-    <row r="2968" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2968" s="6"/>
-    </row>
-    <row r="2969" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2969" s="6"/>
-    </row>
-    <row r="2970" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2970" s="6"/>
-    </row>
-    <row r="2971" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2971" s="6"/>
-    </row>
-    <row r="2972" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2972" s="6"/>
-    </row>
-    <row r="2973" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2973" s="6"/>
-    </row>
-    <row r="2974" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2974" s="6"/>
-    </row>
-    <row r="2975" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2975" s="6"/>
-    </row>
-    <row r="2976" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2976" s="6"/>
-    </row>
-    <row r="2977" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2977" s="6"/>
-    </row>
-    <row r="2978" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2978" s="6"/>
-    </row>
-    <row r="2979" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2979" s="6"/>
-    </row>
-    <row r="2980" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2980" s="6"/>
-    </row>
-    <row r="2981" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2981" s="6"/>
-    </row>
-    <row r="2982" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2982" s="6"/>
-    </row>
-    <row r="2983" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="A2960" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B2960" s="9">
+        <v>41109</v>
+      </c>
+      <c r="AE2960" s="10">
+        <v>5.6999999999999993</v>
+      </c>
+    </row>
+    <row r="2961" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2961" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B2961" s="9">
+        <v>41119</v>
+      </c>
+      <c r="AE2961" s="10">
+        <v>6.95</v>
+      </c>
+    </row>
+    <row r="2962" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2962" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="B2962" s="9">
+        <v>41119</v>
+      </c>
+      <c r="AE2962" s="10">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="2963" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2963" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="B2963" s="9">
+        <v>41129</v>
+      </c>
+      <c r="AE2963" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="2964" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2964" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="B2964" s="9">
+        <v>41136</v>
+      </c>
+      <c r="AE2964" s="10">
+        <v>5.8000000000000007</v>
+      </c>
+    </row>
+    <row r="2965" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2965" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="B2965" s="9">
+        <v>41142</v>
+      </c>
+      <c r="AE2965" s="10">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="2966" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2966" s="5" t="s">
+        <v>836</v>
+      </c>
+      <c r="B2966" s="9">
+        <v>41081</v>
+      </c>
+      <c r="AE2966" s="10">
+        <v>4.45</v>
+      </c>
+    </row>
+    <row r="2967" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2967" s="5" t="s">
+        <v>836</v>
+      </c>
+      <c r="B2967" s="9">
+        <v>41108</v>
+      </c>
+      <c r="AE2967" s="10">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="2968" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2968" s="5" t="s">
+        <v>836</v>
+      </c>
+      <c r="B2968" s="9">
+        <v>41117</v>
+      </c>
+      <c r="AE2968" s="10">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="2969" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2969" s="5" t="s">
+        <v>836</v>
+      </c>
+      <c r="B2969" s="9">
+        <v>41124</v>
+      </c>
+      <c r="AE2969" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2970" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2970" s="5" t="s">
+        <v>839</v>
+      </c>
+      <c r="B2970" s="9">
+        <v>41081</v>
+      </c>
+      <c r="AE2970" s="10">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="2971" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2971" s="5" t="s">
+        <v>839</v>
+      </c>
+      <c r="B2971" s="9">
+        <v>41108</v>
+      </c>
+      <c r="AE2971" s="10">
+        <v>4.5500000000000007</v>
+      </c>
+    </row>
+    <row r="2972" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2972" s="5" t="s">
+        <v>839</v>
+      </c>
+      <c r="B2972" s="9">
+        <v>41117</v>
+      </c>
+      <c r="AE2972" s="10">
+        <v>5.4499999999999993</v>
+      </c>
+    </row>
+    <row r="2973" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2973" s="5" t="s">
+        <v>839</v>
+      </c>
+      <c r="B2973" s="9">
+        <v>41124</v>
+      </c>
+      <c r="AE2973" s="10">
+        <v>5.85</v>
+      </c>
+    </row>
+    <row r="2974" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2974" s="5" t="s">
+        <v>839</v>
+      </c>
+      <c r="B2974" s="9">
+        <v>41134</v>
+      </c>
+      <c r="AE2974" s="10">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="2975" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2975" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="B2975" s="9">
+        <v>41108</v>
+      </c>
+      <c r="AE2975" s="10">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="2976" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2976" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="B2976" s="9">
+        <v>41117</v>
+      </c>
+      <c r="AE2976" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2977" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2977" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="B2977" s="9">
+        <v>41124</v>
+      </c>
+      <c r="AE2977" s="10">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="2978" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2978" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="B2978" s="9">
+        <v>41134</v>
+      </c>
+      <c r="AE2978" s="10">
+        <v>3.5999999999999996</v>
+      </c>
+    </row>
+    <row r="2979" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2979" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="B2979" s="9">
+        <v>41142</v>
+      </c>
+      <c r="AE2979" s="10">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="2980" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2980" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="B2980" s="9">
+        <v>41148</v>
+      </c>
+      <c r="AE2980" s="10">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="2981" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2981" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="B2981" s="9">
+        <v>41158</v>
+      </c>
+      <c r="AE2981" s="10">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="2982" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2982" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="B2982" s="9">
+        <v>41164</v>
+      </c>
+      <c r="AE2982" s="10">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="2983" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B2983" s="6"/>
     </row>
-    <row r="2984" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2984" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B2984" s="6"/>
     </row>
-    <row r="2985" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2985" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B2985" s="6"/>
     </row>
-    <row r="2986" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2986" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B2986" s="6"/>
     </row>
-    <row r="2987" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2987" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B2987" s="6"/>
     </row>
-    <row r="2988" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2988" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B2988" s="6"/>
     </row>
-    <row r="2989" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2989" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B2989" s="6"/>
     </row>
-    <row r="2990" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2990" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B2990" s="6"/>
     </row>
-    <row r="2991" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2991" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B2991" s="6"/>
     </row>
-    <row r="2992" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2992" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B2992" s="6"/>
     </row>
     <row r="2993" spans="2:2" x14ac:dyDescent="0.3">
@@ -69463,471 +69738,6 @@
     </row>
     <row r="3122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3122" s="6"/>
-    </row>
-    <row r="3123" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3123" s="6"/>
-    </row>
-    <row r="3124" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3124" s="6"/>
-    </row>
-    <row r="3125" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3125" s="6"/>
-    </row>
-    <row r="3126" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3126" s="6"/>
-    </row>
-    <row r="3127" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3127" s="6"/>
-    </row>
-    <row r="3128" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3128" s="6"/>
-    </row>
-    <row r="3129" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3129" s="6"/>
-    </row>
-    <row r="3130" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3130" s="6"/>
-    </row>
-    <row r="3131" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3131" s="6"/>
-    </row>
-    <row r="3132" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3132" s="6"/>
-    </row>
-    <row r="3133" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3133" s="6"/>
-    </row>
-    <row r="3134" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3134" s="6"/>
-    </row>
-    <row r="3135" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3135" s="6"/>
-    </row>
-    <row r="3136" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3136" s="6"/>
-    </row>
-    <row r="3137" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3137" s="6"/>
-    </row>
-    <row r="3138" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3138" s="6"/>
-    </row>
-    <row r="3139" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3139" s="6"/>
-    </row>
-    <row r="3140" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3140" s="6"/>
-    </row>
-    <row r="3141" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3141" s="6"/>
-    </row>
-    <row r="3142" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3142" s="6"/>
-    </row>
-    <row r="3143" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3143" s="6"/>
-    </row>
-    <row r="3144" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3144" s="6"/>
-    </row>
-    <row r="3145" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3145" s="6"/>
-    </row>
-    <row r="3146" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3146" s="6"/>
-    </row>
-    <row r="3147" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3147" s="6"/>
-    </row>
-    <row r="3148" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3148" s="6"/>
-    </row>
-    <row r="3149" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3149" s="6"/>
-    </row>
-    <row r="3150" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3150" s="6"/>
-    </row>
-    <row r="3151" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3151" s="6"/>
-    </row>
-    <row r="3152" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3152" s="6"/>
-    </row>
-    <row r="3153" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3153" s="6"/>
-    </row>
-    <row r="3154" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3154" s="6"/>
-    </row>
-    <row r="3155" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3155" s="6"/>
-    </row>
-    <row r="3156" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3156" s="6"/>
-    </row>
-    <row r="3157" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3157" s="6"/>
-    </row>
-    <row r="3158" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3158" s="6"/>
-    </row>
-    <row r="3159" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3159" s="6"/>
-    </row>
-    <row r="3160" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3160" s="6"/>
-    </row>
-    <row r="3161" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3161" s="6"/>
-    </row>
-    <row r="3162" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3162" s="6"/>
-    </row>
-    <row r="3163" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3163" s="6"/>
-    </row>
-    <row r="3164" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3164" s="6"/>
-    </row>
-    <row r="3165" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3165" s="6"/>
-    </row>
-    <row r="3166" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3166" s="6"/>
-    </row>
-    <row r="3167" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3167" s="6"/>
-    </row>
-    <row r="3168" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3168" s="6"/>
-    </row>
-    <row r="3169" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3169" s="6"/>
-    </row>
-    <row r="3170" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3170" s="6"/>
-    </row>
-    <row r="3171" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3171" s="6"/>
-    </row>
-    <row r="3172" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3172" s="6"/>
-    </row>
-    <row r="3173" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3173" s="6"/>
-    </row>
-    <row r="3174" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3174" s="6"/>
-    </row>
-    <row r="3175" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3175" s="6"/>
-    </row>
-    <row r="3176" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3176" s="6"/>
-    </row>
-    <row r="3177" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3177" s="6"/>
-    </row>
-    <row r="3178" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3178" s="6"/>
-    </row>
-    <row r="3179" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3179" s="6"/>
-    </row>
-    <row r="3180" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3180" s="6"/>
-    </row>
-    <row r="3181" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3181" s="6"/>
-    </row>
-    <row r="3182" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3182" s="6"/>
-    </row>
-    <row r="3183" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3183" s="6"/>
-    </row>
-    <row r="3184" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3184" s="6"/>
-    </row>
-    <row r="3185" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3185" s="6"/>
-    </row>
-    <row r="3186" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3186" s="6"/>
-    </row>
-    <row r="3187" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3187" s="6"/>
-    </row>
-    <row r="3188" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3188" s="6"/>
-    </row>
-    <row r="3189" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3189" s="6"/>
-    </row>
-    <row r="3190" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3190" s="6"/>
-    </row>
-    <row r="3191" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3191" s="6"/>
-    </row>
-    <row r="3192" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3192" s="6"/>
-    </row>
-    <row r="3193" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3193" s="6"/>
-    </row>
-    <row r="3194" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3194" s="6"/>
-    </row>
-    <row r="3195" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3195" s="6"/>
-    </row>
-    <row r="3196" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3196" s="6"/>
-    </row>
-    <row r="3197" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3197" s="6"/>
-    </row>
-    <row r="3198" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3198" s="6"/>
-    </row>
-    <row r="3199" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3199" s="6"/>
-    </row>
-    <row r="3200" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3200" s="6"/>
-    </row>
-    <row r="3201" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3201" s="6"/>
-    </row>
-    <row r="3202" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3202" s="6"/>
-    </row>
-    <row r="3203" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3203" s="6"/>
-    </row>
-    <row r="3204" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3204" s="6"/>
-    </row>
-    <row r="3205" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3205" s="6"/>
-    </row>
-    <row r="3206" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3206" s="6"/>
-    </row>
-    <row r="3207" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3207" s="6"/>
-    </row>
-    <row r="3208" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3208" s="6"/>
-    </row>
-    <row r="3209" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3209" s="6"/>
-    </row>
-    <row r="3210" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3210" s="6"/>
-    </row>
-    <row r="3211" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3211" s="6"/>
-    </row>
-    <row r="3212" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3212" s="6"/>
-    </row>
-    <row r="3213" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3213" s="6"/>
-    </row>
-    <row r="3214" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3214" s="6"/>
-    </row>
-    <row r="3215" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3215" s="6"/>
-    </row>
-    <row r="3216" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3216" s="6"/>
-    </row>
-    <row r="3217" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3217" s="6"/>
-    </row>
-    <row r="3218" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3218" s="6"/>
-    </row>
-    <row r="3219" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3219" s="6"/>
-    </row>
-    <row r="3220" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3220" s="6"/>
-    </row>
-    <row r="3221" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3221" s="6"/>
-    </row>
-    <row r="3222" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3222" s="6"/>
-    </row>
-    <row r="3223" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3223" s="6"/>
-    </row>
-    <row r="3224" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3224" s="6"/>
-    </row>
-    <row r="3225" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3225" s="6"/>
-    </row>
-    <row r="3226" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3226" s="6"/>
-    </row>
-    <row r="3227" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3227" s="6"/>
-    </row>
-    <row r="3228" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3228" s="6"/>
-    </row>
-    <row r="3229" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3229" s="6"/>
-    </row>
-    <row r="3230" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3230" s="6"/>
-    </row>
-    <row r="3231" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3231" s="6"/>
-    </row>
-    <row r="3232" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3232" s="6"/>
-    </row>
-    <row r="3233" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3233" s="6"/>
-    </row>
-    <row r="3234" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3234" s="6"/>
-    </row>
-    <row r="3235" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3235" s="6"/>
-    </row>
-    <row r="3236" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3236" s="6"/>
-    </row>
-    <row r="3237" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3237" s="6"/>
-    </row>
-    <row r="3238" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3238" s="6"/>
-    </row>
-    <row r="3239" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3239" s="6"/>
-    </row>
-    <row r="3240" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3240" s="6"/>
-    </row>
-    <row r="3241" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3241" s="6"/>
-    </row>
-    <row r="3242" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3242" s="6"/>
-    </row>
-    <row r="3243" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3243" s="6"/>
-    </row>
-    <row r="3244" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3244" s="6"/>
-    </row>
-    <row r="3245" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3245" s="6"/>
-    </row>
-    <row r="3246" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3246" s="6"/>
-    </row>
-    <row r="3247" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3247" s="6"/>
-    </row>
-    <row r="3248" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3248" s="6"/>
-    </row>
-    <row r="3249" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3249" s="6"/>
-    </row>
-    <row r="3250" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3250" s="6"/>
-    </row>
-    <row r="3251" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3251" s="6"/>
-    </row>
-    <row r="3252" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3252" s="6"/>
-    </row>
-    <row r="3253" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3253" s="6"/>
-    </row>
-    <row r="3254" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3254" s="6"/>
-    </row>
-    <row r="3255" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3255" s="6"/>
-    </row>
-    <row r="3256" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3256" s="6"/>
-    </row>
-    <row r="3257" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3257" s="6"/>
-    </row>
-    <row r="3258" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3258" s="6"/>
-    </row>
-    <row r="3259" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3259" s="6"/>
-    </row>
-    <row r="3260" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3260" s="6"/>
-    </row>
-    <row r="3261" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3261" s="6"/>
-    </row>
-    <row r="3262" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3262" s="6"/>
-    </row>
-    <row r="3263" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3263" s="6"/>
-    </row>
-    <row r="3264" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3264" s="6"/>
-    </row>
-    <row r="3265" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3265" s="6"/>
-    </row>
-    <row r="3266" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3266" s="6"/>
-    </row>
-    <row r="3267" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3267" s="6"/>
-    </row>
-    <row r="3268" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3268" s="6"/>
-    </row>
-    <row r="3269" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3269" s="6"/>
-    </row>
-    <row r="3270" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3270" s="6"/>
-    </row>
-    <row r="3271" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3271" s="6"/>
-    </row>
-    <row r="3272" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3272" s="6"/>
-    </row>
-    <row r="3273" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3273" s="6"/>
-    </row>
-    <row r="3274" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3274" s="6"/>
-    </row>
-    <row r="3275" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3275" s="6"/>
-    </row>
-    <row r="3276" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3276" s="6"/>
-    </row>
-    <row r="3277" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3277" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:AP853">

</xml_diff>

<commit_message>
Progress with canopy model
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -2794,7 +2794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2826,6 +2826,9 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3135,10 +3138,10 @@
   <dimension ref="A1:AX3130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2961" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AK2001" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2963" sqref="D2963"/>
+      <selection pane="bottomRight" activeCell="AL2019" sqref="AL2019"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40606,6 +40609,7 @@
       <c r="M1670">
         <v>0.15075</v>
       </c>
+      <c r="V1670" s="14"/>
     </row>
     <row r="1671" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1671" s="4" t="s">
@@ -40617,6 +40621,7 @@
       <c r="C1671" s="13" t="s">
         <v>862</v>
       </c>
+      <c r="V1671" s="14"/>
       <c r="AA1671">
         <v>0.49971334567674602</v>
       </c>
@@ -40661,6 +40666,7 @@
       <c r="M1672">
         <v>0.14824999999999999</v>
       </c>
+      <c r="V1672" s="14"/>
     </row>
     <row r="1673" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1673" s="4" t="s">
@@ -40672,6 +40678,7 @@
       <c r="C1673" s="13" t="s">
         <v>862</v>
       </c>
+      <c r="V1673" s="14"/>
       <c r="AP1673">
         <v>90.5</v>
       </c>
@@ -40713,6 +40720,7 @@
       <c r="M1674">
         <v>0.14774999999999999</v>
       </c>
+      <c r="V1674" s="14"/>
       <c r="AA1674">
         <v>0</v>
       </c>
@@ -40754,6 +40762,7 @@
       <c r="M1675">
         <v>0.14274999999999999</v>
       </c>
+      <c r="V1675" s="14"/>
     </row>
     <row r="1676" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1676" s="4" t="s">
@@ -40788,6 +40797,9 @@
       <c r="S1677">
         <v>1256.0124139288801</v>
       </c>
+      <c r="W1677">
+        <v>25266.818441084899</v>
+      </c>
       <c r="Y1677">
         <v>954.44929749999994</v>
       </c>
@@ -40800,17 +40812,11 @@
       <c r="AL1677" t="s">
         <v>787</v>
       </c>
-      <c r="AQ1677">
-        <v>0</v>
-      </c>
       <c r="AS1677">
         <v>301.56311642887903</v>
       </c>
       <c r="AV1677">
         <v>798.82365915335595</v>
-      </c>
-      <c r="AW1677">
-        <v>845.8125</v>
       </c>
     </row>
     <row r="1678" spans="1:49" x14ac:dyDescent="0.25">
@@ -42773,6 +42779,9 @@
       <c r="S1744">
         <v>1233.09316214398</v>
       </c>
+      <c r="W1744">
+        <v>27609.7279011473</v>
+      </c>
       <c r="Y1744">
         <v>885.45308499999999</v>
       </c>
@@ -42785,17 +42794,11 @@
       <c r="AL1744" t="s">
         <v>787</v>
       </c>
-      <c r="AQ1744">
-        <v>0</v>
-      </c>
       <c r="AS1744">
         <v>347.64007714398502</v>
       </c>
       <c r="AV1744">
         <v>883.743501876148</v>
-      </c>
-      <c r="AW1744">
-        <v>876.1875</v>
       </c>
     </row>
     <row r="1745" spans="1:49" x14ac:dyDescent="0.25">
@@ -44669,7 +44672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1809" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1809" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1809" s="4" t="s">
         <v>148</v>
       </c>
@@ -44707,7 +44710,7 @@
         <v>0.19725000000000001</v>
       </c>
     </row>
-    <row r="1810" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1810" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1810" s="4" t="s">
         <v>148</v>
       </c>
@@ -44724,7 +44727,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1811" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1811" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1811" s="4" t="s">
         <v>148</v>
       </c>
@@ -44740,6 +44743,9 @@
       <c r="S1811">
         <v>1231.5468913737</v>
       </c>
+      <c r="W1811">
+        <v>28433.773147215801</v>
+      </c>
       <c r="Y1811">
         <v>904.03921749999995</v>
       </c>
@@ -44752,20 +44758,14 @@
       <c r="AL1811" t="s">
         <v>787</v>
       </c>
-      <c r="AQ1811">
-        <v>0</v>
-      </c>
       <c r="AS1811">
         <v>327.50767387369598</v>
       </c>
       <c r="AV1811">
         <v>901.35902355859503</v>
       </c>
-      <c r="AW1811">
-        <v>897.5625</v>
-      </c>
-    </row>
-    <row r="1812" spans="1:49" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1812" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1812" s="4" t="s">
         <v>148</v>
       </c>
@@ -44803,7 +44803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1813" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1813" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1813" s="4" t="s">
         <v>147</v>
       </c>
@@ -44823,7 +44823,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="1814" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1814" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1814" s="4" t="s">
         <v>147</v>
       </c>
@@ -44861,7 +44861,7 @@
         <v>0.23849999999999999</v>
       </c>
     </row>
-    <row r="1815" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1815" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1815" s="4" t="s">
         <v>147</v>
       </c>
@@ -44899,7 +44899,7 @@
         <v>0.23849999999999999</v>
       </c>
     </row>
-    <row r="1816" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1816" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1816" s="4" t="s">
         <v>147</v>
       </c>
@@ -44919,7 +44919,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="1817" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1817" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1817" s="4" t="s">
         <v>147</v>
       </c>
@@ -44933,7 +44933,7 @@
         <v>0.21659329775748001</v>
       </c>
     </row>
-    <row r="1818" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1818" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1818" s="4" t="s">
         <v>147</v>
       </c>
@@ -44974,7 +44974,7 @@
         <v>0.43667134245053102</v>
       </c>
     </row>
-    <row r="1819" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1819" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1819" s="4" t="s">
         <v>147</v>
       </c>
@@ -44994,7 +44994,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="1820" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1820" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1820" s="4" t="s">
         <v>147</v>
       </c>
@@ -45038,7 +45038,7 @@
         <v>5.95</v>
       </c>
     </row>
-    <row r="1821" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1821" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1821" s="4" t="s">
         <v>147</v>
       </c>
@@ -45055,7 +45055,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1822" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1822" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1822" s="4" t="s">
         <v>147</v>
       </c>
@@ -45093,7 +45093,7 @@
         <v>0.23674999999999999</v>
       </c>
     </row>
-    <row r="1823" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1823" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1823" s="4" t="s">
         <v>147</v>
       </c>
@@ -45116,7 +45116,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="1824" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1824" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1824" s="4" t="s">
         <v>147</v>
       </c>
@@ -46543,7 +46543,7 @@
         <v>90.75</v>
       </c>
     </row>
-    <row r="1873" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1873" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1873" s="4" t="s">
         <v>147</v>
       </c>
@@ -46581,7 +46581,7 @@
         <v>0.1885</v>
       </c>
     </row>
-    <row r="1874" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1874" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1874" s="4" t="s">
         <v>147</v>
       </c>
@@ -46595,7 +46595,7 @@
         <v>90.75</v>
       </c>
     </row>
-    <row r="1875" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1875" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1875" s="4" t="s">
         <v>147</v>
       </c>
@@ -46636,7 +46636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1876" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1876" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1876" s="4" t="s">
         <v>147</v>
       </c>
@@ -46674,7 +46674,7 @@
         <v>0.1895</v>
       </c>
     </row>
-    <row r="1877" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1877" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1877" s="4" t="s">
         <v>147</v>
       </c>
@@ -46691,7 +46691,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1878" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1878" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1878" s="4" t="s">
         <v>147</v>
       </c>
@@ -46707,6 +46707,9 @@
       <c r="S1878">
         <v>1159.6031345220499</v>
       </c>
+      <c r="W1878">
+        <v>23906.626917524201</v>
+      </c>
       <c r="Y1878">
         <v>861.81991500000004</v>
       </c>
@@ -46719,20 +46722,14 @@
       <c r="AL1878" t="s">
         <v>787</v>
       </c>
-      <c r="AQ1878">
-        <v>0</v>
-      </c>
       <c r="AS1878">
         <v>297.78321952204601</v>
       </c>
       <c r="AV1878">
         <v>820.25531414114505</v>
       </c>
-      <c r="AW1878">
-        <v>815.4375</v>
-      </c>
-    </row>
-    <row r="1879" spans="1:49" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1879" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1879" s="4" t="s">
         <v>147</v>
       </c>
@@ -46770,7 +46767,7 @@
         <v>0.18725</v>
       </c>
     </row>
-    <row r="1880" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1880" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1880" s="4" t="s">
         <v>144</v>
       </c>
@@ -46790,7 +46787,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="1881" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1881" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1881" s="4" t="s">
         <v>144</v>
       </c>
@@ -46828,7 +46825,7 @@
         <v>0.18225</v>
       </c>
     </row>
-    <row r="1882" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1882" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1882" s="4" t="s">
         <v>144</v>
       </c>
@@ -46866,7 +46863,7 @@
         <v>0.18074999999999999</v>
       </c>
     </row>
-    <row r="1883" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1883" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1883" s="4" t="s">
         <v>144</v>
       </c>
@@ -46886,7 +46883,7 @@
         <v>22.25</v>
       </c>
     </row>
-    <row r="1884" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1884" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1884" s="4" t="s">
         <v>144</v>
       </c>
@@ -46900,7 +46897,7 @@
         <v>0.20034810498982</v>
       </c>
     </row>
-    <row r="1885" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1885" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1885" s="4" t="s">
         <v>144</v>
       </c>
@@ -46941,7 +46938,7 @@
         <v>0.43562341935058402</v>
       </c>
     </row>
-    <row r="1886" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1886" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1886" s="4" t="s">
         <v>144</v>
       </c>
@@ -46961,7 +46958,7 @@
         <v>24.25</v>
       </c>
     </row>
-    <row r="1887" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1887" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1887" s="4" t="s">
         <v>144</v>
       </c>
@@ -47005,7 +47002,7 @@
         <v>6.15</v>
       </c>
     </row>
-    <row r="1888" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1888" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1888" s="4" t="s">
         <v>144</v>
       </c>
@@ -48441,7 +48438,7 @@
         <v>0.1255</v>
       </c>
     </row>
-    <row r="1937" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1937" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1937" s="4" t="s">
         <v>144</v>
       </c>
@@ -48455,7 +48452,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="1938" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1938" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1938" s="4" t="s">
         <v>144</v>
       </c>
@@ -48493,7 +48490,7 @@
         <v>0.12625</v>
       </c>
     </row>
-    <row r="1939" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1939" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1939" s="4" t="s">
         <v>144</v>
       </c>
@@ -48510,7 +48507,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="1940" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1940" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1940" s="4" t="s">
         <v>144</v>
       </c>
@@ -48548,7 +48545,7 @@
         <v>0.12325</v>
       </c>
     </row>
-    <row r="1941" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1941" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1941" s="4" t="s">
         <v>144</v>
       </c>
@@ -48562,7 +48559,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="1942" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1942" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1942" s="4" t="s">
         <v>144</v>
       </c>
@@ -48603,7 +48600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1943" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1943" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1943" s="4" t="s">
         <v>144</v>
       </c>
@@ -48641,7 +48638,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="1944" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1944" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1944" s="4" t="s">
         <v>144</v>
       </c>
@@ -48655,7 +48652,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1945" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1945" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1945" s="4" t="s">
         <v>144</v>
       </c>
@@ -48671,6 +48668,9 @@
       <c r="S1945">
         <v>947.294439637339</v>
       </c>
+      <c r="W1945">
+        <v>17324.2225803978</v>
+      </c>
       <c r="Y1945">
         <v>682.31069500000001</v>
       </c>
@@ -48683,20 +48683,14 @@
       <c r="AL1945" t="s">
         <v>787</v>
       </c>
-      <c r="AQ1945">
-        <v>0</v>
-      </c>
       <c r="AS1945">
         <v>264.98374463733899</v>
       </c>
       <c r="AV1945">
         <v>734.85205635114403</v>
       </c>
-      <c r="AW1945">
-        <v>791.25</v>
-      </c>
-    </row>
-    <row r="1946" spans="1:49" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1946" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1946" s="4" t="s">
         <v>144</v>
       </c>
@@ -48734,7 +48728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1947" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1947" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1947" s="4" t="s">
         <v>145</v>
       </c>
@@ -48754,7 +48748,7 @@
         <v>15.75</v>
       </c>
     </row>
-    <row r="1948" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1948" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1948" s="4" t="s">
         <v>145</v>
       </c>
@@ -48792,7 +48786,7 @@
         <v>0.18174999999999999</v>
       </c>
     </row>
-    <row r="1949" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1949" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1949" s="4" t="s">
         <v>145</v>
       </c>
@@ -48830,7 +48824,7 @@
         <v>0.18124999999999999</v>
       </c>
     </row>
-    <row r="1950" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1950" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1950" s="4" t="s">
         <v>145</v>
       </c>
@@ -48850,7 +48844,7 @@
         <v>21.75</v>
       </c>
     </row>
-    <row r="1951" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1951" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1951" s="4" t="s">
         <v>145</v>
       </c>
@@ -48864,7 +48858,7 @@
         <v>0.22411051883682101</v>
       </c>
     </row>
-    <row r="1952" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1952" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1952" s="4" t="s">
         <v>145</v>
       </c>
@@ -50339,7 +50333,7 @@
         <v>813.92857142857099</v>
       </c>
     </row>
-    <row r="2001" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2001" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2001" s="4" t="s">
         <v>145</v>
       </c>
@@ -50353,7 +50347,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2002" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2002" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2002" s="4" t="s">
         <v>145</v>
       </c>
@@ -50367,7 +50361,7 @@
         <v>0.98882777807271205</v>
       </c>
     </row>
-    <row r="2003" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2003" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2003" s="4" t="s">
         <v>145</v>
       </c>
@@ -50405,7 +50399,7 @@
         <v>0.16550000000000001</v>
       </c>
     </row>
-    <row r="2004" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2004" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2004" s="4" t="s">
         <v>145</v>
       </c>
@@ -50419,7 +50413,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2005" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2005" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2005" s="4" t="s">
         <v>145</v>
       </c>
@@ -50457,7 +50451,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="2006" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2006" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2006" s="4" t="s">
         <v>145</v>
       </c>
@@ -50474,7 +50468,7 @@
         <v>87.5</v>
       </c>
     </row>
-    <row r="2007" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2007" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2007" s="4" t="s">
         <v>145</v>
       </c>
@@ -50512,7 +50506,7 @@
         <v>0.157</v>
       </c>
     </row>
-    <row r="2008" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2008" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2008" s="4" t="s">
         <v>145</v>
       </c>
@@ -50526,7 +50520,7 @@
         <v>89.75</v>
       </c>
     </row>
-    <row r="2009" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2009" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2009" s="4" t="s">
         <v>145</v>
       </c>
@@ -50567,7 +50561,7 @@
         <v>0.30249058887758001</v>
       </c>
     </row>
-    <row r="2010" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2010" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2010" s="4" t="s">
         <v>145</v>
       </c>
@@ -50605,7 +50599,7 @@
         <v>0.15075</v>
       </c>
     </row>
-    <row r="2011" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2011" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2011" s="4" t="s">
         <v>145</v>
       </c>
@@ -50622,7 +50616,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2012" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2012" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2012" s="4" t="s">
         <v>145</v>
       </c>
@@ -50638,6 +50632,9 @@
       <c r="S2012">
         <v>1221.2595441127801</v>
       </c>
+      <c r="W2012">
+        <v>21687.383565656499</v>
+      </c>
       <c r="Y2012">
         <v>939.17182000000003</v>
       </c>
@@ -50650,20 +50647,14 @@
       <c r="AL2012" t="s">
         <v>787</v>
       </c>
-      <c r="AQ2012">
-        <v>0</v>
-      </c>
       <c r="AS2012">
         <v>282.08772411277698</v>
       </c>
       <c r="AV2012">
         <v>780.86968134003996</v>
       </c>
-      <c r="AW2012">
-        <v>838.6875</v>
-      </c>
-    </row>
-    <row r="2013" spans="1:49" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2013" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2013" s="4" t="s">
         <v>145</v>
       </c>
@@ -50701,7 +50692,7 @@
         <v>0.14774999999999999</v>
       </c>
     </row>
-    <row r="2014" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2014" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2014" s="4" t="s">
         <v>82</v>
       </c>
@@ -50737,7 +50728,7 @@
         <v>0.20795</v>
       </c>
     </row>
-    <row r="2015" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2015" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2015" s="4" t="s">
         <v>82</v>
       </c>
@@ -50773,7 +50764,7 @@
         <v>0.20895</v>
       </c>
     </row>
-    <row r="2016" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2016" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2016" s="4" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
Fixing HaunStage Variable again.  Fixing FractionComplete in leaf appearance phase
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -2826,7 +2826,7 @@
     <t>Kennedy</t>
   </si>
   <si>
-    <t>Wheat.Structure.HaunStage</t>
+    <t>Wheat.Structure.HaunStage.Value</t>
   </si>
 </sst>
 </file>
@@ -3255,7 +3255,7 @@
   <dimension ref="A1:BP3251"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AV10" sqref="AV10"/>
+      <selection activeCell="AX4" sqref="AX4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Got some leaf size comparison graphs working
</commit_message>
<xml_diff>
--- a/Prototypes/Wheat/Observed.xlsx
+++ b/Prototypes/Wheat/Observed.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14295" tabRatio="862"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14295" tabRatio="862" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
+    <sheet name="MaxLeafSize" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$B$2871</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5791" uniqueCount="935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5986" uniqueCount="937">
   <si>
     <t>SimulationName</t>
   </si>
@@ -2827,6 +2828,12 @@
   </si>
   <si>
     <t>Wheat.Structure.HaunStage.Value</t>
+  </si>
+  <si>
+    <t>MaxLeafSize.Script.LeafPosition</t>
+  </si>
+  <si>
+    <t>MaxLeafSize.Script.MaxLeafSize</t>
   </si>
 </sst>
 </file>
@@ -3252,10 +3259,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BP3251"/>
+  <dimension ref="A1:BP3255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AX4" sqref="AX4"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="AV3026" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3252" sqref="A3252:XFD3255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -81905,7 +81915,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3249" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3249" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A3249" s="3" t="s">
         <v>761</v>
       </c>
@@ -81928,7 +81938,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3250" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3250" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A3250" s="3" t="s">
         <v>761</v>
       </c>
@@ -81951,7 +81961,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3251" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3251" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A3251" s="3" t="s">
         <v>761</v>
       </c>
@@ -81987,6 +81997,245 @@
       </c>
       <c r="AW3251">
         <v>597.76562030000002</v>
+      </c>
+    </row>
+    <row r="3252" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A3252" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="C3252" t="s">
+        <v>855</v>
+      </c>
+      <c r="AL3252" t="s">
+        <v>784</v>
+      </c>
+      <c r="AY3252">
+        <v>192.14999999999998</v>
+      </c>
+      <c r="AZ3252">
+        <v>356.91100000000006</v>
+      </c>
+      <c r="BA3252">
+        <v>486.9020000000001</v>
+      </c>
+      <c r="BB3252">
+        <v>696.82333333333327</v>
+      </c>
+      <c r="BC3252">
+        <v>909.50999999999988</v>
+      </c>
+      <c r="BD3252">
+        <v>1225.124</v>
+      </c>
+      <c r="BE3252">
+        <v>1486.923157894737</v>
+      </c>
+      <c r="BF3252">
+        <v>1915.3036842105262</v>
+      </c>
+      <c r="BG3252">
+        <v>2068.6063157894737</v>
+      </c>
+      <c r="BH3252">
+        <v>2224.6378947368421</v>
+      </c>
+      <c r="BI3252">
+        <v>2283.4868421052638</v>
+      </c>
+      <c r="BJ3252">
+        <v>2214.1715789473687</v>
+      </c>
+      <c r="BK3252">
+        <v>1896.7468421052629</v>
+      </c>
+      <c r="BL3252">
+        <v>1715.7694736842104</v>
+      </c>
+      <c r="BM3252">
+        <v>1819.6621052631574</v>
+      </c>
+      <c r="BN3252">
+        <v>1890.0368421052628</v>
+      </c>
+      <c r="BO3252">
+        <v>1766.6242105263154</v>
+      </c>
+      <c r="BP3252">
+        <v>1549.2373333333335</v>
+      </c>
+    </row>
+    <row r="3253" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A3253" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="C3253" t="s">
+        <v>855</v>
+      </c>
+      <c r="AL3253" t="s">
+        <v>784</v>
+      </c>
+      <c r="AY3253">
+        <v>245.76899999999995</v>
+      </c>
+      <c r="AZ3253">
+        <v>458.20150000000001</v>
+      </c>
+      <c r="BA3253">
+        <v>687.43949999999984</v>
+      </c>
+      <c r="BB3253">
+        <v>872.94049999999982</v>
+      </c>
+      <c r="BC3253">
+        <v>1152.5949999999998</v>
+      </c>
+      <c r="BD3253">
+        <v>1489.4505555555554</v>
+      </c>
+      <c r="BE3253">
+        <v>1495.7538888888889</v>
+      </c>
+      <c r="BF3253">
+        <v>1520.7977777777778</v>
+      </c>
+      <c r="BG3253">
+        <v>1603.1138888888891</v>
+      </c>
+      <c r="BH3253">
+        <v>1600.4366666666665</v>
+      </c>
+      <c r="BI3253">
+        <v>1484.096111111111</v>
+      </c>
+      <c r="BJ3253">
+        <v>1662.3177777777773</v>
+      </c>
+      <c r="BK3253">
+        <v>1904.6233333333325</v>
+      </c>
+      <c r="BL3253">
+        <v>1930.5144444444441</v>
+      </c>
+      <c r="BM3253">
+        <v>1774.7949999999996</v>
+      </c>
+      <c r="BN3253">
+        <v>1517.141764705882</v>
+      </c>
+      <c r="BO3253">
+        <v>1260.4633333333331</v>
+      </c>
+    </row>
+    <row r="3254" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A3254" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="C3254" t="s">
+        <v>855</v>
+      </c>
+      <c r="AL3254" t="s">
+        <v>784</v>
+      </c>
+      <c r="AY3254">
+        <v>238.571</v>
+      </c>
+      <c r="AZ3254">
+        <v>471.94736842105254</v>
+      </c>
+      <c r="BA3254">
+        <v>624.15842105263164</v>
+      </c>
+      <c r="BB3254">
+        <v>675.88</v>
+      </c>
+      <c r="BC3254">
+        <v>774.5474999999999</v>
+      </c>
+      <c r="BD3254">
+        <v>850.75736842105255</v>
+      </c>
+      <c r="BE3254">
+        <v>947.36388888888871</v>
+      </c>
+      <c r="BF3254">
+        <v>1032.2216666666666</v>
+      </c>
+      <c r="BG3254">
+        <v>1253.7194444444444</v>
+      </c>
+      <c r="BH3254">
+        <v>1760.5955555555554</v>
+      </c>
+      <c r="BI3254">
+        <v>2228.1944444444443</v>
+      </c>
+      <c r="BJ3254">
+        <v>2382.3888888888887</v>
+      </c>
+      <c r="BK3254">
+        <v>2202.0661111111112</v>
+      </c>
+      <c r="BL3254">
+        <v>1973.7905555555558</v>
+      </c>
+      <c r="BM3254">
+        <v>1693.1566666666668</v>
+      </c>
+      <c r="BN3254">
+        <v>1665.3</v>
+      </c>
+    </row>
+    <row r="3255" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A3255" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="C3255" t="s">
+        <v>855</v>
+      </c>
+      <c r="AL3255" t="s">
+        <v>784</v>
+      </c>
+      <c r="AY3255">
+        <v>133.53454545454545</v>
+      </c>
+      <c r="AZ3255">
+        <v>231.02947368421044</v>
+      </c>
+      <c r="BA3255">
+        <v>312.68599999999998</v>
+      </c>
+      <c r="BB3255">
+        <v>351.3599999999999</v>
+      </c>
+      <c r="BC3255">
+        <v>425.16999999999996</v>
+      </c>
+      <c r="BD3255">
+        <v>586.24049999999988</v>
+      </c>
+      <c r="BE3255">
+        <v>902.76187500000003</v>
+      </c>
+      <c r="BF3255">
+        <v>1327.001176470588</v>
+      </c>
+      <c r="BG3255">
+        <v>1922.076111111111</v>
+      </c>
+      <c r="BH3255">
+        <v>2315.9259999999995</v>
+      </c>
+      <c r="BI3255">
+        <v>2395.0735</v>
+      </c>
+      <c r="BJ3255">
+        <v>2426.4579999999996</v>
+      </c>
+      <c r="BK3255">
+        <v>2130.7299999999996</v>
+      </c>
+      <c r="BL3255">
+        <v>1549.4</v>
       </c>
     </row>
   </sheetData>
@@ -81997,4 +82246,1940 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C181"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>935</v>
+      </c>
+      <c r="C1" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>755</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>192.14999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>758</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>245.76899999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>760</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>238.571</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>762</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>133.53454545454545</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>281.10833333333335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>237.96099999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>233.142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>239.24199999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>224.51049999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>226.61499999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>755</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>356.91100000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>758</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>458.20150000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>760</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>471.94736842105254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>762</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>231.02947368421044</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>489.15222222222224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>401.83750000000009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>411.94263157894738</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>426.63400000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>435.66199999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>413.06149999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>755</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>486.9020000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>758</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>687.43949999999984</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>760</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>624.15842105263164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>762</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>312.68599999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>596.73250000000007</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>479.97850000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>522.46499999999992</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>515.0535000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>535.73250000000007</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>490.745</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>755</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>696.82333333333327</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>758</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>872.94049999999982</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>760</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>675.88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>762</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>351.3599999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>658.678</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>594.25437499999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>631.77699999999993</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>632.05149999999992</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>622.32199999999989</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>144</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>621.46800000000007</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>755</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>909.50999999999988</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>758</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>1152.5949999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>760</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>774.5474999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>762</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>425.16999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>816.3325000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <v>755.02749999999992</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>763.84199999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>821.09050000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>143</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50">
+        <v>785.46649999999977</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>144</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <v>762.01199999999994</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>755</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <v>1225.124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>758</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>1489.4505555555554</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>760</v>
+      </c>
+      <c r="B54">
+        <v>6</v>
+      </c>
+      <c r="C54">
+        <v>850.75736842105255</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>762</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+      <c r="C55">
+        <v>586.24049999999988</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>906.82599999999979</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>142</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+      <c r="C57">
+        <v>821.76149999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58">
+        <v>6</v>
+      </c>
+      <c r="C58">
+        <v>829.81349999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>146</v>
+      </c>
+      <c r="B59">
+        <v>6</v>
+      </c>
+      <c r="C59">
+        <v>863.88199999999995</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60">
+        <v>6</v>
+      </c>
+      <c r="C60">
+        <v>906.33799999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>144</v>
+      </c>
+      <c r="B61">
+        <v>6</v>
+      </c>
+      <c r="C61">
+        <v>807.51799999999992</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>755</v>
+      </c>
+      <c r="B62">
+        <v>7</v>
+      </c>
+      <c r="C62">
+        <v>1486.923157894737</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>758</v>
+      </c>
+      <c r="B63">
+        <v>7</v>
+      </c>
+      <c r="C63">
+        <v>1495.7538888888889</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>760</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+      <c r="C64">
+        <v>947.36388888888871</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>762</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
+      </c>
+      <c r="C65">
+        <v>902.76187500000003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>145</v>
+      </c>
+      <c r="B66">
+        <v>7</v>
+      </c>
+      <c r="C66">
+        <v>1050.9690000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>142</v>
+      </c>
+      <c r="B67">
+        <v>7</v>
+      </c>
+      <c r="C67">
+        <v>958.1880000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68">
+        <v>7</v>
+      </c>
+      <c r="C68">
+        <v>1002.7179999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>146</v>
+      </c>
+      <c r="B69">
+        <v>7</v>
+      </c>
+      <c r="C69">
+        <v>1037.3965000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>143</v>
+      </c>
+      <c r="B70">
+        <v>7</v>
+      </c>
+      <c r="C70">
+        <v>1017.7850000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>144</v>
+      </c>
+      <c r="B71">
+        <v>7</v>
+      </c>
+      <c r="C71">
+        <v>906.1244999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>755</v>
+      </c>
+      <c r="B72">
+        <v>8</v>
+      </c>
+      <c r="C72">
+        <v>1915.3036842105262</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>758</v>
+      </c>
+      <c r="B73">
+        <v>8</v>
+      </c>
+      <c r="C73">
+        <v>1520.7977777777778</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>760</v>
+      </c>
+      <c r="B74">
+        <v>8</v>
+      </c>
+      <c r="C74">
+        <v>1032.2216666666666</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>762</v>
+      </c>
+      <c r="B75">
+        <v>8</v>
+      </c>
+      <c r="C75">
+        <v>1327.001176470588</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>145</v>
+      </c>
+      <c r="B76">
+        <v>8</v>
+      </c>
+      <c r="C76">
+        <v>1139.663</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>142</v>
+      </c>
+      <c r="B77">
+        <v>8</v>
+      </c>
+      <c r="C77">
+        <v>1133.8375000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>147</v>
+      </c>
+      <c r="B78">
+        <v>8</v>
+      </c>
+      <c r="C78">
+        <v>1141.5539999999996</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>146</v>
+      </c>
+      <c r="B79">
+        <v>8</v>
+      </c>
+      <c r="C79">
+        <v>1154.3944999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>143</v>
+      </c>
+      <c r="B80">
+        <v>8</v>
+      </c>
+      <c r="C80">
+        <v>1152.1680000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>144</v>
+      </c>
+      <c r="B81">
+        <v>8</v>
+      </c>
+      <c r="C81">
+        <v>1029.1309999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>755</v>
+      </c>
+      <c r="B82">
+        <v>9</v>
+      </c>
+      <c r="C82">
+        <v>2068.6063157894737</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>758</v>
+      </c>
+      <c r="B83">
+        <v>9</v>
+      </c>
+      <c r="C83">
+        <v>1603.1138888888891</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>760</v>
+      </c>
+      <c r="B84">
+        <v>9</v>
+      </c>
+      <c r="C84">
+        <v>1253.7194444444444</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>762</v>
+      </c>
+      <c r="B85">
+        <v>9</v>
+      </c>
+      <c r="C85">
+        <v>1922.076111111111</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>145</v>
+      </c>
+      <c r="B86">
+        <v>9</v>
+      </c>
+      <c r="C86">
+        <v>1435.0554999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>142</v>
+      </c>
+      <c r="B87">
+        <v>9</v>
+      </c>
+      <c r="C87">
+        <v>1420.3544999999997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>147</v>
+      </c>
+      <c r="B88">
+        <v>9</v>
+      </c>
+      <c r="C88">
+        <v>1439.0509999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>146</v>
+      </c>
+      <c r="B89">
+        <v>9</v>
+      </c>
+      <c r="C89">
+        <v>1483.0930000000003</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>143</v>
+      </c>
+      <c r="B90">
+        <v>9</v>
+      </c>
+      <c r="C90">
+        <v>1334.009</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>144</v>
+      </c>
+      <c r="B91">
+        <v>9</v>
+      </c>
+      <c r="C91">
+        <v>1306.5894999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>755</v>
+      </c>
+      <c r="B92">
+        <v>10</v>
+      </c>
+      <c r="C92">
+        <v>2224.6378947368421</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>758</v>
+      </c>
+      <c r="B93">
+        <v>10</v>
+      </c>
+      <c r="C93">
+        <v>1600.4366666666665</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>760</v>
+      </c>
+      <c r="B94">
+        <v>10</v>
+      </c>
+      <c r="C94">
+        <v>1760.5955555555554</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>762</v>
+      </c>
+      <c r="B95">
+        <v>10</v>
+      </c>
+      <c r="C95">
+        <v>2315.9259999999995</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>145</v>
+      </c>
+      <c r="B96">
+        <v>10</v>
+      </c>
+      <c r="C96">
+        <v>2067.6254999999996</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>142</v>
+      </c>
+      <c r="B97">
+        <v>10</v>
+      </c>
+      <c r="C97">
+        <v>2067.0154999999995</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>147</v>
+      </c>
+      <c r="B98">
+        <v>10</v>
+      </c>
+      <c r="C98">
+        <v>2059.7869999999994</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>146</v>
+      </c>
+      <c r="B99">
+        <v>10</v>
+      </c>
+      <c r="C99">
+        <v>2107.5804999999991</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>143</v>
+      </c>
+      <c r="B100">
+        <v>10</v>
+      </c>
+      <c r="C100">
+        <v>1986.7394999999997</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>144</v>
+      </c>
+      <c r="B101">
+        <v>10</v>
+      </c>
+      <c r="C101">
+        <v>2021.5399999999997</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>755</v>
+      </c>
+      <c r="B102">
+        <v>11</v>
+      </c>
+      <c r="C102">
+        <v>2283.4868421052638</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>758</v>
+      </c>
+      <c r="B103">
+        <v>11</v>
+      </c>
+      <c r="C103">
+        <v>1484.096111111111</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>760</v>
+      </c>
+      <c r="B104">
+        <v>11</v>
+      </c>
+      <c r="C104">
+        <v>2228.1944444444443</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>762</v>
+      </c>
+      <c r="B105">
+        <v>11</v>
+      </c>
+      <c r="C105">
+        <v>2395.0735</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>145</v>
+      </c>
+      <c r="B106">
+        <v>11</v>
+      </c>
+      <c r="C106">
+        <v>2258.3419999999996</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>142</v>
+      </c>
+      <c r="B107">
+        <v>11</v>
+      </c>
+      <c r="C107">
+        <v>2317.5119999999997</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>147</v>
+      </c>
+      <c r="B108">
+        <v>11</v>
+      </c>
+      <c r="C108">
+        <v>2336.8490000000006</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>146</v>
+      </c>
+      <c r="B109">
+        <v>11</v>
+      </c>
+      <c r="C109">
+        <v>2302.75</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>143</v>
+      </c>
+      <c r="B110">
+        <v>11</v>
+      </c>
+      <c r="C110">
+        <v>2317.4205000000002</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>144</v>
+      </c>
+      <c r="B111">
+        <v>11</v>
+      </c>
+      <c r="C111">
+        <v>2356.4605000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>755</v>
+      </c>
+      <c r="B112">
+        <v>12</v>
+      </c>
+      <c r="C112">
+        <v>2214.1715789473687</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>758</v>
+      </c>
+      <c r="B113">
+        <v>12</v>
+      </c>
+      <c r="C113">
+        <v>1662.3177777777773</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>760</v>
+      </c>
+      <c r="B114">
+        <v>12</v>
+      </c>
+      <c r="C114">
+        <v>2382.3888888888887</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>762</v>
+      </c>
+      <c r="B115">
+        <v>12</v>
+      </c>
+      <c r="C115">
+        <v>2426.4579999999996</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>145</v>
+      </c>
+      <c r="B116">
+        <v>12</v>
+      </c>
+      <c r="C116">
+        <v>2191.7910000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>142</v>
+      </c>
+      <c r="B117">
+        <v>12</v>
+      </c>
+      <c r="C117">
+        <v>2259.8364999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>147</v>
+      </c>
+      <c r="B118">
+        <v>12</v>
+      </c>
+      <c r="C118">
+        <v>2197.0065000000004</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>146</v>
+      </c>
+      <c r="B119">
+        <v>12</v>
+      </c>
+      <c r="C119">
+        <v>2117.7979999999998</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>143</v>
+      </c>
+      <c r="B120">
+        <v>12</v>
+      </c>
+      <c r="C120">
+        <v>2219.1189999999997</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>144</v>
+      </c>
+      <c r="B121">
+        <v>12</v>
+      </c>
+      <c r="C121">
+        <v>2301.1945000000005</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>755</v>
+      </c>
+      <c r="B122">
+        <v>13</v>
+      </c>
+      <c r="C122">
+        <v>1896.7468421052629</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>758</v>
+      </c>
+      <c r="B123">
+        <v>13</v>
+      </c>
+      <c r="C123">
+        <v>1904.6233333333325</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>760</v>
+      </c>
+      <c r="B124">
+        <v>13</v>
+      </c>
+      <c r="C124">
+        <v>2202.0661111111112</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>762</v>
+      </c>
+      <c r="B125">
+        <v>13</v>
+      </c>
+      <c r="C125">
+        <v>2130.7299999999996</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>145</v>
+      </c>
+      <c r="B126">
+        <v>13</v>
+      </c>
+      <c r="C126">
+        <v>2572.0039999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>142</v>
+      </c>
+      <c r="B127">
+        <v>13</v>
+      </c>
+      <c r="C127">
+        <v>2548.0919999999996</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>147</v>
+      </c>
+      <c r="B128">
+        <v>13</v>
+      </c>
+      <c r="C128">
+        <v>2446.893</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>146</v>
+      </c>
+      <c r="B129">
+        <v>13</v>
+      </c>
+      <c r="C129">
+        <v>2377.9629999999993</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>143</v>
+      </c>
+      <c r="B130">
+        <v>13</v>
+      </c>
+      <c r="C130">
+        <v>2375.8584999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>144</v>
+      </c>
+      <c r="B131">
+        <v>13</v>
+      </c>
+      <c r="C131">
+        <v>2478.4910000000004</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>755</v>
+      </c>
+      <c r="B132">
+        <v>14</v>
+      </c>
+      <c r="C132">
+        <v>1715.7694736842104</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>758</v>
+      </c>
+      <c r="B133">
+        <v>14</v>
+      </c>
+      <c r="C133">
+        <v>1930.5144444444441</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>760</v>
+      </c>
+      <c r="B134">
+        <v>14</v>
+      </c>
+      <c r="C134">
+        <v>1973.7905555555558</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>762</v>
+      </c>
+      <c r="B135">
+        <v>14</v>
+      </c>
+      <c r="C135">
+        <v>1549.4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>145</v>
+      </c>
+      <c r="B136">
+        <v>14</v>
+      </c>
+      <c r="C136">
+        <v>2710.0165000000002</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>142</v>
+      </c>
+      <c r="B137">
+        <v>14</v>
+      </c>
+      <c r="C137">
+        <v>3005.3784999999998</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>147</v>
+      </c>
+      <c r="B138">
+        <v>14</v>
+      </c>
+      <c r="C138">
+        <v>2840.2819999999997</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>146</v>
+      </c>
+      <c r="B139">
+        <v>14</v>
+      </c>
+      <c r="C139">
+        <v>2700.148947368421</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>143</v>
+      </c>
+      <c r="B140">
+        <v>14</v>
+      </c>
+      <c r="C140">
+        <v>2432.9544999999994</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>144</v>
+      </c>
+      <c r="B141">
+        <v>14</v>
+      </c>
+      <c r="C141">
+        <v>2406.0839999999998</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>755</v>
+      </c>
+      <c r="B142">
+        <v>15</v>
+      </c>
+      <c r="C142">
+        <v>1819.6621052631574</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>758</v>
+      </c>
+      <c r="B143">
+        <v>15</v>
+      </c>
+      <c r="C143">
+        <v>1774.7949999999996</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>760</v>
+      </c>
+      <c r="B144">
+        <v>15</v>
+      </c>
+      <c r="C144">
+        <v>1693.1566666666668</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>762</v>
+      </c>
+      <c r="B145">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <v>15</v>
+      </c>
+      <c r="C146">
+        <v>2198.2366666666662</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>142</v>
+      </c>
+      <c r="B147">
+        <v>15</v>
+      </c>
+      <c r="C147">
+        <v>2983.4228571428575</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>15</v>
+      </c>
+      <c r="C148">
+        <v>2841.1766666666667</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>146</v>
+      </c>
+      <c r="B149">
+        <v>15</v>
+      </c>
+      <c r="C149">
+        <v>2503.5162500000001</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>143</v>
+      </c>
+      <c r="B150">
+        <v>15</v>
+      </c>
+      <c r="C150">
+        <v>2149.25875</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>144</v>
+      </c>
+      <c r="B151">
+        <v>15</v>
+      </c>
+      <c r="C151">
+        <v>2193.1025</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>755</v>
+      </c>
+      <c r="B152">
+        <v>16</v>
+      </c>
+      <c r="C152">
+        <v>1890.0368421052628</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>758</v>
+      </c>
+      <c r="B153">
+        <v>16</v>
+      </c>
+      <c r="C153">
+        <v>1517.141764705882</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>760</v>
+      </c>
+      <c r="B154">
+        <v>16</v>
+      </c>
+      <c r="C154">
+        <v>1665.3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>762</v>
+      </c>
+      <c r="B155">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>145</v>
+      </c>
+      <c r="B156">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>142</v>
+      </c>
+      <c r="B157">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>147</v>
+      </c>
+      <c r="B158">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>146</v>
+      </c>
+      <c r="B159">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>143</v>
+      </c>
+      <c r="B160">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>144</v>
+      </c>
+      <c r="B161">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>755</v>
+      </c>
+      <c r="B162">
+        <v>17</v>
+      </c>
+      <c r="C162">
+        <v>1766.6242105263154</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>758</v>
+      </c>
+      <c r="B163">
+        <v>17</v>
+      </c>
+      <c r="C163">
+        <v>1260.4633333333331</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>760</v>
+      </c>
+      <c r="B164">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>762</v>
+      </c>
+      <c r="B165">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>145</v>
+      </c>
+      <c r="B166">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>142</v>
+      </c>
+      <c r="B167">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>147</v>
+      </c>
+      <c r="B168">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>146</v>
+      </c>
+      <c r="B169">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>143</v>
+      </c>
+      <c r="B170">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>144</v>
+      </c>
+      <c r="B171">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>755</v>
+      </c>
+      <c r="B172">
+        <v>18</v>
+      </c>
+      <c r="C172">
+        <v>1549.2373333333335</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>758</v>
+      </c>
+      <c r="B173">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>760</v>
+      </c>
+      <c r="B174">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>762</v>
+      </c>
+      <c r="B175">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>145</v>
+      </c>
+      <c r="B176">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>142</v>
+      </c>
+      <c r="B177">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>147</v>
+      </c>
+      <c r="B178">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>146</v>
+      </c>
+      <c r="B179">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>143</v>
+      </c>
+      <c r="B180">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>144</v>
+      </c>
+      <c r="B181">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>